<commit_message>
PROS6112 - Setup completed
</commit_message>
<xml_diff>
--- a/Projects/BIMY/Data/Template.xlsx
+++ b/Projects/BIMY/Data/Template.xlsx
@@ -16,22 +16,23 @@
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
@@ -297,7 +298,7 @@
     <t xml:space="preserve">PHARMATON 2X100'S</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rhinathiol</t>
+    <t xml:space="preserve">RHINATHIOL</t>
   </si>
   <si>
     <t xml:space="preserve">RHINATHIOL ADULT SYRUP 125ml,
@@ -1452,17 +1453,17 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="1" sqref="E13:E14 F15"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.497975708502"/>
   </cols>
   <sheetData>
@@ -1724,14 +1725,14 @@
   <dimension ref="1:19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="E13:E14 E26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="16.3886639676113"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="23" width="0"/>
@@ -6200,7 +6201,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G9"/>
+  <autoFilter ref="A2:H9"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6221,14 +6222,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="E13:E14 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -6287,19 +6288,15 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13:E14"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="61" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="61" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1023" min="7" style="61" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.0242914979757"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.0242914979757"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6312,7 +6309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
@@ -6331,8 +6328,1026 @@
       <c r="F2" s="68" t="s">
         <v>36</v>
       </c>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
+      <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
+      <c r="IX2" s="0"/>
+      <c r="IY2" s="0"/>
+      <c r="IZ2" s="0"/>
+      <c r="JA2" s="0"/>
+      <c r="JB2" s="0"/>
+      <c r="JC2" s="0"/>
+      <c r="JD2" s="0"/>
+      <c r="JE2" s="0"/>
+      <c r="JF2" s="0"/>
+      <c r="JG2" s="0"/>
+      <c r="JH2" s="0"/>
+      <c r="JI2" s="0"/>
+      <c r="JJ2" s="0"/>
+      <c r="JK2" s="0"/>
+      <c r="JL2" s="0"/>
+      <c r="JM2" s="0"/>
+      <c r="JN2" s="0"/>
+      <c r="JO2" s="0"/>
+      <c r="JP2" s="0"/>
+      <c r="JQ2" s="0"/>
+      <c r="JR2" s="0"/>
+      <c r="JS2" s="0"/>
+      <c r="JT2" s="0"/>
+      <c r="JU2" s="0"/>
+      <c r="JV2" s="0"/>
+      <c r="JW2" s="0"/>
+      <c r="JX2" s="0"/>
+      <c r="JY2" s="0"/>
+      <c r="JZ2" s="0"/>
+      <c r="KA2" s="0"/>
+      <c r="KB2" s="0"/>
+      <c r="KC2" s="0"/>
+      <c r="KD2" s="0"/>
+      <c r="KE2" s="0"/>
+      <c r="KF2" s="0"/>
+      <c r="KG2" s="0"/>
+      <c r="KH2" s="0"/>
+      <c r="KI2" s="0"/>
+      <c r="KJ2" s="0"/>
+      <c r="KK2" s="0"/>
+      <c r="KL2" s="0"/>
+      <c r="KM2" s="0"/>
+      <c r="KN2" s="0"/>
+      <c r="KO2" s="0"/>
+      <c r="KP2" s="0"/>
+      <c r="KQ2" s="0"/>
+      <c r="KR2" s="0"/>
+      <c r="KS2" s="0"/>
+      <c r="KT2" s="0"/>
+      <c r="KU2" s="0"/>
+      <c r="KV2" s="0"/>
+      <c r="KW2" s="0"/>
+      <c r="KX2" s="0"/>
+      <c r="KY2" s="0"/>
+      <c r="KZ2" s="0"/>
+      <c r="LA2" s="0"/>
+      <c r="LB2" s="0"/>
+      <c r="LC2" s="0"/>
+      <c r="LD2" s="0"/>
+      <c r="LE2" s="0"/>
+      <c r="LF2" s="0"/>
+      <c r="LG2" s="0"/>
+      <c r="LH2" s="0"/>
+      <c r="LI2" s="0"/>
+      <c r="LJ2" s="0"/>
+      <c r="LK2" s="0"/>
+      <c r="LL2" s="0"/>
+      <c r="LM2" s="0"/>
+      <c r="LN2" s="0"/>
+      <c r="LO2" s="0"/>
+      <c r="LP2" s="0"/>
+      <c r="LQ2" s="0"/>
+      <c r="LR2" s="0"/>
+      <c r="LS2" s="0"/>
+      <c r="LT2" s="0"/>
+      <c r="LU2" s="0"/>
+      <c r="LV2" s="0"/>
+      <c r="LW2" s="0"/>
+      <c r="LX2" s="0"/>
+      <c r="LY2" s="0"/>
+      <c r="LZ2" s="0"/>
+      <c r="MA2" s="0"/>
+      <c r="MB2" s="0"/>
+      <c r="MC2" s="0"/>
+      <c r="MD2" s="0"/>
+      <c r="ME2" s="0"/>
+      <c r="MF2" s="0"/>
+      <c r="MG2" s="0"/>
+      <c r="MH2" s="0"/>
+      <c r="MI2" s="0"/>
+      <c r="MJ2" s="0"/>
+      <c r="MK2" s="0"/>
+      <c r="ML2" s="0"/>
+      <c r="MM2" s="0"/>
+      <c r="MN2" s="0"/>
+      <c r="MO2" s="0"/>
+      <c r="MP2" s="0"/>
+      <c r="MQ2" s="0"/>
+      <c r="MR2" s="0"/>
+      <c r="MS2" s="0"/>
+      <c r="MT2" s="0"/>
+      <c r="MU2" s="0"/>
+      <c r="MV2" s="0"/>
+      <c r="MW2" s="0"/>
+      <c r="MX2" s="0"/>
+      <c r="MY2" s="0"/>
+      <c r="MZ2" s="0"/>
+      <c r="NA2" s="0"/>
+      <c r="NB2" s="0"/>
+      <c r="NC2" s="0"/>
+      <c r="ND2" s="0"/>
+      <c r="NE2" s="0"/>
+      <c r="NF2" s="0"/>
+      <c r="NG2" s="0"/>
+      <c r="NH2" s="0"/>
+      <c r="NI2" s="0"/>
+      <c r="NJ2" s="0"/>
+      <c r="NK2" s="0"/>
+      <c r="NL2" s="0"/>
+      <c r="NM2" s="0"/>
+      <c r="NN2" s="0"/>
+      <c r="NO2" s="0"/>
+      <c r="NP2" s="0"/>
+      <c r="NQ2" s="0"/>
+      <c r="NR2" s="0"/>
+      <c r="NS2" s="0"/>
+      <c r="NT2" s="0"/>
+      <c r="NU2" s="0"/>
+      <c r="NV2" s="0"/>
+      <c r="NW2" s="0"/>
+      <c r="NX2" s="0"/>
+      <c r="NY2" s="0"/>
+      <c r="NZ2" s="0"/>
+      <c r="OA2" s="0"/>
+      <c r="OB2" s="0"/>
+      <c r="OC2" s="0"/>
+      <c r="OD2" s="0"/>
+      <c r="OE2" s="0"/>
+      <c r="OF2" s="0"/>
+      <c r="OG2" s="0"/>
+      <c r="OH2" s="0"/>
+      <c r="OI2" s="0"/>
+      <c r="OJ2" s="0"/>
+      <c r="OK2" s="0"/>
+      <c r="OL2" s="0"/>
+      <c r="OM2" s="0"/>
+      <c r="ON2" s="0"/>
+      <c r="OO2" s="0"/>
+      <c r="OP2" s="0"/>
+      <c r="OQ2" s="0"/>
+      <c r="OR2" s="0"/>
+      <c r="OS2" s="0"/>
+      <c r="OT2" s="0"/>
+      <c r="OU2" s="0"/>
+      <c r="OV2" s="0"/>
+      <c r="OW2" s="0"/>
+      <c r="OX2" s="0"/>
+      <c r="OY2" s="0"/>
+      <c r="OZ2" s="0"/>
+      <c r="PA2" s="0"/>
+      <c r="PB2" s="0"/>
+      <c r="PC2" s="0"/>
+      <c r="PD2" s="0"/>
+      <c r="PE2" s="0"/>
+      <c r="PF2" s="0"/>
+      <c r="PG2" s="0"/>
+      <c r="PH2" s="0"/>
+      <c r="PI2" s="0"/>
+      <c r="PJ2" s="0"/>
+      <c r="PK2" s="0"/>
+      <c r="PL2" s="0"/>
+      <c r="PM2" s="0"/>
+      <c r="PN2" s="0"/>
+      <c r="PO2" s="0"/>
+      <c r="PP2" s="0"/>
+      <c r="PQ2" s="0"/>
+      <c r="PR2" s="0"/>
+      <c r="PS2" s="0"/>
+      <c r="PT2" s="0"/>
+      <c r="PU2" s="0"/>
+      <c r="PV2" s="0"/>
+      <c r="PW2" s="0"/>
+      <c r="PX2" s="0"/>
+      <c r="PY2" s="0"/>
+      <c r="PZ2" s="0"/>
+      <c r="QA2" s="0"/>
+      <c r="QB2" s="0"/>
+      <c r="QC2" s="0"/>
+      <c r="QD2" s="0"/>
+      <c r="QE2" s="0"/>
+      <c r="QF2" s="0"/>
+      <c r="QG2" s="0"/>
+      <c r="QH2" s="0"/>
+      <c r="QI2" s="0"/>
+      <c r="QJ2" s="0"/>
+      <c r="QK2" s="0"/>
+      <c r="QL2" s="0"/>
+      <c r="QM2" s="0"/>
+      <c r="QN2" s="0"/>
+      <c r="QO2" s="0"/>
+      <c r="QP2" s="0"/>
+      <c r="QQ2" s="0"/>
+      <c r="QR2" s="0"/>
+      <c r="QS2" s="0"/>
+      <c r="QT2" s="0"/>
+      <c r="QU2" s="0"/>
+      <c r="QV2" s="0"/>
+      <c r="QW2" s="0"/>
+      <c r="QX2" s="0"/>
+      <c r="QY2" s="0"/>
+      <c r="QZ2" s="0"/>
+      <c r="RA2" s="0"/>
+      <c r="RB2" s="0"/>
+      <c r="RC2" s="0"/>
+      <c r="RD2" s="0"/>
+      <c r="RE2" s="0"/>
+      <c r="RF2" s="0"/>
+      <c r="RG2" s="0"/>
+      <c r="RH2" s="0"/>
+      <c r="RI2" s="0"/>
+      <c r="RJ2" s="0"/>
+      <c r="RK2" s="0"/>
+      <c r="RL2" s="0"/>
+      <c r="RM2" s="0"/>
+      <c r="RN2" s="0"/>
+      <c r="RO2" s="0"/>
+      <c r="RP2" s="0"/>
+      <c r="RQ2" s="0"/>
+      <c r="RR2" s="0"/>
+      <c r="RS2" s="0"/>
+      <c r="RT2" s="0"/>
+      <c r="RU2" s="0"/>
+      <c r="RV2" s="0"/>
+      <c r="RW2" s="0"/>
+      <c r="RX2" s="0"/>
+      <c r="RY2" s="0"/>
+      <c r="RZ2" s="0"/>
+      <c r="SA2" s="0"/>
+      <c r="SB2" s="0"/>
+      <c r="SC2" s="0"/>
+      <c r="SD2" s="0"/>
+      <c r="SE2" s="0"/>
+      <c r="SF2" s="0"/>
+      <c r="SG2" s="0"/>
+      <c r="SH2" s="0"/>
+      <c r="SI2" s="0"/>
+      <c r="SJ2" s="0"/>
+      <c r="SK2" s="0"/>
+      <c r="SL2" s="0"/>
+      <c r="SM2" s="0"/>
+      <c r="SN2" s="0"/>
+      <c r="SO2" s="0"/>
+      <c r="SP2" s="0"/>
+      <c r="SQ2" s="0"/>
+      <c r="SR2" s="0"/>
+      <c r="SS2" s="0"/>
+      <c r="ST2" s="0"/>
+      <c r="SU2" s="0"/>
+      <c r="SV2" s="0"/>
+      <c r="SW2" s="0"/>
+      <c r="SX2" s="0"/>
+      <c r="SY2" s="0"/>
+      <c r="SZ2" s="0"/>
+      <c r="TA2" s="0"/>
+      <c r="TB2" s="0"/>
+      <c r="TC2" s="0"/>
+      <c r="TD2" s="0"/>
+      <c r="TE2" s="0"/>
+      <c r="TF2" s="0"/>
+      <c r="TG2" s="0"/>
+      <c r="TH2" s="0"/>
+      <c r="TI2" s="0"/>
+      <c r="TJ2" s="0"/>
+      <c r="TK2" s="0"/>
+      <c r="TL2" s="0"/>
+      <c r="TM2" s="0"/>
+      <c r="TN2" s="0"/>
+      <c r="TO2" s="0"/>
+      <c r="TP2" s="0"/>
+      <c r="TQ2" s="0"/>
+      <c r="TR2" s="0"/>
+      <c r="TS2" s="0"/>
+      <c r="TT2" s="0"/>
+      <c r="TU2" s="0"/>
+      <c r="TV2" s="0"/>
+      <c r="TW2" s="0"/>
+      <c r="TX2" s="0"/>
+      <c r="TY2" s="0"/>
+      <c r="TZ2" s="0"/>
+      <c r="UA2" s="0"/>
+      <c r="UB2" s="0"/>
+      <c r="UC2" s="0"/>
+      <c r="UD2" s="0"/>
+      <c r="UE2" s="0"/>
+      <c r="UF2" s="0"/>
+      <c r="UG2" s="0"/>
+      <c r="UH2" s="0"/>
+      <c r="UI2" s="0"/>
+      <c r="UJ2" s="0"/>
+      <c r="UK2" s="0"/>
+      <c r="UL2" s="0"/>
+      <c r="UM2" s="0"/>
+      <c r="UN2" s="0"/>
+      <c r="UO2" s="0"/>
+      <c r="UP2" s="0"/>
+      <c r="UQ2" s="0"/>
+      <c r="UR2" s="0"/>
+      <c r="US2" s="0"/>
+      <c r="UT2" s="0"/>
+      <c r="UU2" s="0"/>
+      <c r="UV2" s="0"/>
+      <c r="UW2" s="0"/>
+      <c r="UX2" s="0"/>
+      <c r="UY2" s="0"/>
+      <c r="UZ2" s="0"/>
+      <c r="VA2" s="0"/>
+      <c r="VB2" s="0"/>
+      <c r="VC2" s="0"/>
+      <c r="VD2" s="0"/>
+      <c r="VE2" s="0"/>
+      <c r="VF2" s="0"/>
+      <c r="VG2" s="0"/>
+      <c r="VH2" s="0"/>
+      <c r="VI2" s="0"/>
+      <c r="VJ2" s="0"/>
+      <c r="VK2" s="0"/>
+      <c r="VL2" s="0"/>
+      <c r="VM2" s="0"/>
+      <c r="VN2" s="0"/>
+      <c r="VO2" s="0"/>
+      <c r="VP2" s="0"/>
+      <c r="VQ2" s="0"/>
+      <c r="VR2" s="0"/>
+      <c r="VS2" s="0"/>
+      <c r="VT2" s="0"/>
+      <c r="VU2" s="0"/>
+      <c r="VV2" s="0"/>
+      <c r="VW2" s="0"/>
+      <c r="VX2" s="0"/>
+      <c r="VY2" s="0"/>
+      <c r="VZ2" s="0"/>
+      <c r="WA2" s="0"/>
+      <c r="WB2" s="0"/>
+      <c r="WC2" s="0"/>
+      <c r="WD2" s="0"/>
+      <c r="WE2" s="0"/>
+      <c r="WF2" s="0"/>
+      <c r="WG2" s="0"/>
+      <c r="WH2" s="0"/>
+      <c r="WI2" s="0"/>
+      <c r="WJ2" s="0"/>
+      <c r="WK2" s="0"/>
+      <c r="WL2" s="0"/>
+      <c r="WM2" s="0"/>
+      <c r="WN2" s="0"/>
+      <c r="WO2" s="0"/>
+      <c r="WP2" s="0"/>
+      <c r="WQ2" s="0"/>
+      <c r="WR2" s="0"/>
+      <c r="WS2" s="0"/>
+      <c r="WT2" s="0"/>
+      <c r="WU2" s="0"/>
+      <c r="WV2" s="0"/>
+      <c r="WW2" s="0"/>
+      <c r="WX2" s="0"/>
+      <c r="WY2" s="0"/>
+      <c r="WZ2" s="0"/>
+      <c r="XA2" s="0"/>
+      <c r="XB2" s="0"/>
+      <c r="XC2" s="0"/>
+      <c r="XD2" s="0"/>
+      <c r="XE2" s="0"/>
+      <c r="XF2" s="0"/>
+      <c r="XG2" s="0"/>
+      <c r="XH2" s="0"/>
+      <c r="XI2" s="0"/>
+      <c r="XJ2" s="0"/>
+      <c r="XK2" s="0"/>
+      <c r="XL2" s="0"/>
+      <c r="XM2" s="0"/>
+      <c r="XN2" s="0"/>
+      <c r="XO2" s="0"/>
+      <c r="XP2" s="0"/>
+      <c r="XQ2" s="0"/>
+      <c r="XR2" s="0"/>
+      <c r="XS2" s="0"/>
+      <c r="XT2" s="0"/>
+      <c r="XU2" s="0"/>
+      <c r="XV2" s="0"/>
+      <c r="XW2" s="0"/>
+      <c r="XX2" s="0"/>
+      <c r="XY2" s="0"/>
+      <c r="XZ2" s="0"/>
+      <c r="YA2" s="0"/>
+      <c r="YB2" s="0"/>
+      <c r="YC2" s="0"/>
+      <c r="YD2" s="0"/>
+      <c r="YE2" s="0"/>
+      <c r="YF2" s="0"/>
+      <c r="YG2" s="0"/>
+      <c r="YH2" s="0"/>
+      <c r="YI2" s="0"/>
+      <c r="YJ2" s="0"/>
+      <c r="YK2" s="0"/>
+      <c r="YL2" s="0"/>
+      <c r="YM2" s="0"/>
+      <c r="YN2" s="0"/>
+      <c r="YO2" s="0"/>
+      <c r="YP2" s="0"/>
+      <c r="YQ2" s="0"/>
+      <c r="YR2" s="0"/>
+      <c r="YS2" s="0"/>
+      <c r="YT2" s="0"/>
+      <c r="YU2" s="0"/>
+      <c r="YV2" s="0"/>
+      <c r="YW2" s="0"/>
+      <c r="YX2" s="0"/>
+      <c r="YY2" s="0"/>
+      <c r="YZ2" s="0"/>
+      <c r="ZA2" s="0"/>
+      <c r="ZB2" s="0"/>
+      <c r="ZC2" s="0"/>
+      <c r="ZD2" s="0"/>
+      <c r="ZE2" s="0"/>
+      <c r="ZF2" s="0"/>
+      <c r="ZG2" s="0"/>
+      <c r="ZH2" s="0"/>
+      <c r="ZI2" s="0"/>
+      <c r="ZJ2" s="0"/>
+      <c r="ZK2" s="0"/>
+      <c r="ZL2" s="0"/>
+      <c r="ZM2" s="0"/>
+      <c r="ZN2" s="0"/>
+      <c r="ZO2" s="0"/>
+      <c r="ZP2" s="0"/>
+      <c r="ZQ2" s="0"/>
+      <c r="ZR2" s="0"/>
+      <c r="ZS2" s="0"/>
+      <c r="ZT2" s="0"/>
+      <c r="ZU2" s="0"/>
+      <c r="ZV2" s="0"/>
+      <c r="ZW2" s="0"/>
+      <c r="ZX2" s="0"/>
+      <c r="ZY2" s="0"/>
+      <c r="ZZ2" s="0"/>
+      <c r="AAA2" s="0"/>
+      <c r="AAB2" s="0"/>
+      <c r="AAC2" s="0"/>
+      <c r="AAD2" s="0"/>
+      <c r="AAE2" s="0"/>
+      <c r="AAF2" s="0"/>
+      <c r="AAG2" s="0"/>
+      <c r="AAH2" s="0"/>
+      <c r="AAI2" s="0"/>
+      <c r="AAJ2" s="0"/>
+      <c r="AAK2" s="0"/>
+      <c r="AAL2" s="0"/>
+      <c r="AAM2" s="0"/>
+      <c r="AAN2" s="0"/>
+      <c r="AAO2" s="0"/>
+      <c r="AAP2" s="0"/>
+      <c r="AAQ2" s="0"/>
+      <c r="AAR2" s="0"/>
+      <c r="AAS2" s="0"/>
+      <c r="AAT2" s="0"/>
+      <c r="AAU2" s="0"/>
+      <c r="AAV2" s="0"/>
+      <c r="AAW2" s="0"/>
+      <c r="AAX2" s="0"/>
+      <c r="AAY2" s="0"/>
+      <c r="AAZ2" s="0"/>
+      <c r="ABA2" s="0"/>
+      <c r="ABB2" s="0"/>
+      <c r="ABC2" s="0"/>
+      <c r="ABD2" s="0"/>
+      <c r="ABE2" s="0"/>
+      <c r="ABF2" s="0"/>
+      <c r="ABG2" s="0"/>
+      <c r="ABH2" s="0"/>
+      <c r="ABI2" s="0"/>
+      <c r="ABJ2" s="0"/>
+      <c r="ABK2" s="0"/>
+      <c r="ABL2" s="0"/>
+      <c r="ABM2" s="0"/>
+      <c r="ABN2" s="0"/>
+      <c r="ABO2" s="0"/>
+      <c r="ABP2" s="0"/>
+      <c r="ABQ2" s="0"/>
+      <c r="ABR2" s="0"/>
+      <c r="ABS2" s="0"/>
+      <c r="ABT2" s="0"/>
+      <c r="ABU2" s="0"/>
+      <c r="ABV2" s="0"/>
+      <c r="ABW2" s="0"/>
+      <c r="ABX2" s="0"/>
+      <c r="ABY2" s="0"/>
+      <c r="ABZ2" s="0"/>
+      <c r="ACA2" s="0"/>
+      <c r="ACB2" s="0"/>
+      <c r="ACC2" s="0"/>
+      <c r="ACD2" s="0"/>
+      <c r="ACE2" s="0"/>
+      <c r="ACF2" s="0"/>
+      <c r="ACG2" s="0"/>
+      <c r="ACH2" s="0"/>
+      <c r="ACI2" s="0"/>
+      <c r="ACJ2" s="0"/>
+      <c r="ACK2" s="0"/>
+      <c r="ACL2" s="0"/>
+      <c r="ACM2" s="0"/>
+      <c r="ACN2" s="0"/>
+      <c r="ACO2" s="0"/>
+      <c r="ACP2" s="0"/>
+      <c r="ACQ2" s="0"/>
+      <c r="ACR2" s="0"/>
+      <c r="ACS2" s="0"/>
+      <c r="ACT2" s="0"/>
+      <c r="ACU2" s="0"/>
+      <c r="ACV2" s="0"/>
+      <c r="ACW2" s="0"/>
+      <c r="ACX2" s="0"/>
+      <c r="ACY2" s="0"/>
+      <c r="ACZ2" s="0"/>
+      <c r="ADA2" s="0"/>
+      <c r="ADB2" s="0"/>
+      <c r="ADC2" s="0"/>
+      <c r="ADD2" s="0"/>
+      <c r="ADE2" s="0"/>
+      <c r="ADF2" s="0"/>
+      <c r="ADG2" s="0"/>
+      <c r="ADH2" s="0"/>
+      <c r="ADI2" s="0"/>
+      <c r="ADJ2" s="0"/>
+      <c r="ADK2" s="0"/>
+      <c r="ADL2" s="0"/>
+      <c r="ADM2" s="0"/>
+      <c r="ADN2" s="0"/>
+      <c r="ADO2" s="0"/>
+      <c r="ADP2" s="0"/>
+      <c r="ADQ2" s="0"/>
+      <c r="ADR2" s="0"/>
+      <c r="ADS2" s="0"/>
+      <c r="ADT2" s="0"/>
+      <c r="ADU2" s="0"/>
+      <c r="ADV2" s="0"/>
+      <c r="ADW2" s="0"/>
+      <c r="ADX2" s="0"/>
+      <c r="ADY2" s="0"/>
+      <c r="ADZ2" s="0"/>
+      <c r="AEA2" s="0"/>
+      <c r="AEB2" s="0"/>
+      <c r="AEC2" s="0"/>
+      <c r="AED2" s="0"/>
+      <c r="AEE2" s="0"/>
+      <c r="AEF2" s="0"/>
+      <c r="AEG2" s="0"/>
+      <c r="AEH2" s="0"/>
+      <c r="AEI2" s="0"/>
+      <c r="AEJ2" s="0"/>
+      <c r="AEK2" s="0"/>
+      <c r="AEL2" s="0"/>
+      <c r="AEM2" s="0"/>
+      <c r="AEN2" s="0"/>
+      <c r="AEO2" s="0"/>
+      <c r="AEP2" s="0"/>
+      <c r="AEQ2" s="0"/>
+      <c r="AER2" s="0"/>
+      <c r="AES2" s="0"/>
+      <c r="AET2" s="0"/>
+      <c r="AEU2" s="0"/>
+      <c r="AEV2" s="0"/>
+      <c r="AEW2" s="0"/>
+      <c r="AEX2" s="0"/>
+      <c r="AEY2" s="0"/>
+      <c r="AEZ2" s="0"/>
+      <c r="AFA2" s="0"/>
+      <c r="AFB2" s="0"/>
+      <c r="AFC2" s="0"/>
+      <c r="AFD2" s="0"/>
+      <c r="AFE2" s="0"/>
+      <c r="AFF2" s="0"/>
+      <c r="AFG2" s="0"/>
+      <c r="AFH2" s="0"/>
+      <c r="AFI2" s="0"/>
+      <c r="AFJ2" s="0"/>
+      <c r="AFK2" s="0"/>
+      <c r="AFL2" s="0"/>
+      <c r="AFM2" s="0"/>
+      <c r="AFN2" s="0"/>
+      <c r="AFO2" s="0"/>
+      <c r="AFP2" s="0"/>
+      <c r="AFQ2" s="0"/>
+      <c r="AFR2" s="0"/>
+      <c r="AFS2" s="0"/>
+      <c r="AFT2" s="0"/>
+      <c r="AFU2" s="0"/>
+      <c r="AFV2" s="0"/>
+      <c r="AFW2" s="0"/>
+      <c r="AFX2" s="0"/>
+      <c r="AFY2" s="0"/>
+      <c r="AFZ2" s="0"/>
+      <c r="AGA2" s="0"/>
+      <c r="AGB2" s="0"/>
+      <c r="AGC2" s="0"/>
+      <c r="AGD2" s="0"/>
+      <c r="AGE2" s="0"/>
+      <c r="AGF2" s="0"/>
+      <c r="AGG2" s="0"/>
+      <c r="AGH2" s="0"/>
+      <c r="AGI2" s="0"/>
+      <c r="AGJ2" s="0"/>
+      <c r="AGK2" s="0"/>
+      <c r="AGL2" s="0"/>
+      <c r="AGM2" s="0"/>
+      <c r="AGN2" s="0"/>
+      <c r="AGO2" s="0"/>
+      <c r="AGP2" s="0"/>
+      <c r="AGQ2" s="0"/>
+      <c r="AGR2" s="0"/>
+      <c r="AGS2" s="0"/>
+      <c r="AGT2" s="0"/>
+      <c r="AGU2" s="0"/>
+      <c r="AGV2" s="0"/>
+      <c r="AGW2" s="0"/>
+      <c r="AGX2" s="0"/>
+      <c r="AGY2" s="0"/>
+      <c r="AGZ2" s="0"/>
+      <c r="AHA2" s="0"/>
+      <c r="AHB2" s="0"/>
+      <c r="AHC2" s="0"/>
+      <c r="AHD2" s="0"/>
+      <c r="AHE2" s="0"/>
+      <c r="AHF2" s="0"/>
+      <c r="AHG2" s="0"/>
+      <c r="AHH2" s="0"/>
+      <c r="AHI2" s="0"/>
+      <c r="AHJ2" s="0"/>
+      <c r="AHK2" s="0"/>
+      <c r="AHL2" s="0"/>
+      <c r="AHM2" s="0"/>
+      <c r="AHN2" s="0"/>
+      <c r="AHO2" s="0"/>
+      <c r="AHP2" s="0"/>
+      <c r="AHQ2" s="0"/>
+      <c r="AHR2" s="0"/>
+      <c r="AHS2" s="0"/>
+      <c r="AHT2" s="0"/>
+      <c r="AHU2" s="0"/>
+      <c r="AHV2" s="0"/>
+      <c r="AHW2" s="0"/>
+      <c r="AHX2" s="0"/>
+      <c r="AHY2" s="0"/>
+      <c r="AHZ2" s="0"/>
+      <c r="AIA2" s="0"/>
+      <c r="AIB2" s="0"/>
+      <c r="AIC2" s="0"/>
+      <c r="AID2" s="0"/>
+      <c r="AIE2" s="0"/>
+      <c r="AIF2" s="0"/>
+      <c r="AIG2" s="0"/>
+      <c r="AIH2" s="0"/>
+      <c r="AII2" s="0"/>
+      <c r="AIJ2" s="0"/>
+      <c r="AIK2" s="0"/>
+      <c r="AIL2" s="0"/>
+      <c r="AIM2" s="0"/>
+      <c r="AIN2" s="0"/>
+      <c r="AIO2" s="0"/>
+      <c r="AIP2" s="0"/>
+      <c r="AIQ2" s="0"/>
+      <c r="AIR2" s="0"/>
+      <c r="AIS2" s="0"/>
+      <c r="AIT2" s="0"/>
+      <c r="AIU2" s="0"/>
+      <c r="AIV2" s="0"/>
+      <c r="AIW2" s="0"/>
+      <c r="AIX2" s="0"/>
+      <c r="AIY2" s="0"/>
+      <c r="AIZ2" s="0"/>
+      <c r="AJA2" s="0"/>
+      <c r="AJB2" s="0"/>
+      <c r="AJC2" s="0"/>
+      <c r="AJD2" s="0"/>
+      <c r="AJE2" s="0"/>
+      <c r="AJF2" s="0"/>
+      <c r="AJG2" s="0"/>
+      <c r="AJH2" s="0"/>
+      <c r="AJI2" s="0"/>
+      <c r="AJJ2" s="0"/>
+      <c r="AJK2" s="0"/>
+      <c r="AJL2" s="0"/>
+      <c r="AJM2" s="0"/>
+      <c r="AJN2" s="0"/>
+      <c r="AJO2" s="0"/>
+      <c r="AJP2" s="0"/>
+      <c r="AJQ2" s="0"/>
+      <c r="AJR2" s="0"/>
+      <c r="AJS2" s="0"/>
+      <c r="AJT2" s="0"/>
+      <c r="AJU2" s="0"/>
+      <c r="AJV2" s="0"/>
+      <c r="AJW2" s="0"/>
+      <c r="AJX2" s="0"/>
+      <c r="AJY2" s="0"/>
+      <c r="AJZ2" s="0"/>
+      <c r="AKA2" s="0"/>
+      <c r="AKB2" s="0"/>
+      <c r="AKC2" s="0"/>
+      <c r="AKD2" s="0"/>
+      <c r="AKE2" s="0"/>
+      <c r="AKF2" s="0"/>
+      <c r="AKG2" s="0"/>
+      <c r="AKH2" s="0"/>
+      <c r="AKI2" s="0"/>
+      <c r="AKJ2" s="0"/>
+      <c r="AKK2" s="0"/>
+      <c r="AKL2" s="0"/>
+      <c r="AKM2" s="0"/>
+      <c r="AKN2" s="0"/>
+      <c r="AKO2" s="0"/>
+      <c r="AKP2" s="0"/>
+      <c r="AKQ2" s="0"/>
+      <c r="AKR2" s="0"/>
+      <c r="AKS2" s="0"/>
+      <c r="AKT2" s="0"/>
+      <c r="AKU2" s="0"/>
+      <c r="AKV2" s="0"/>
+      <c r="AKW2" s="0"/>
+      <c r="AKX2" s="0"/>
+      <c r="AKY2" s="0"/>
+      <c r="AKZ2" s="0"/>
+      <c r="ALA2" s="0"/>
+      <c r="ALB2" s="0"/>
+      <c r="ALC2" s="0"/>
+      <c r="ALD2" s="0"/>
+      <c r="ALE2" s="0"/>
+      <c r="ALF2" s="0"/>
+      <c r="ALG2" s="0"/>
+      <c r="ALH2" s="0"/>
+      <c r="ALI2" s="0"/>
+      <c r="ALJ2" s="0"/>
+      <c r="ALK2" s="0"/>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="23" customFormat="true" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="69" t="s">
         <v>14</v>
       </c>
@@ -6351,8 +7366,1026 @@
       <c r="F3" s="74" t="n">
         <v>1</v>
       </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
+      <c r="AJ3" s="0"/>
+      <c r="AK3" s="0"/>
+      <c r="AL3" s="0"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
+      <c r="AO3" s="0"/>
+      <c r="AP3" s="0"/>
+      <c r="AQ3" s="0"/>
+      <c r="AR3" s="0"/>
+      <c r="AS3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
+      <c r="AV3" s="0"/>
+      <c r="AW3" s="0"/>
+      <c r="AX3" s="0"/>
+      <c r="AY3" s="0"/>
+      <c r="AZ3" s="0"/>
+      <c r="BA3" s="0"/>
+      <c r="BB3" s="0"/>
+      <c r="BC3" s="0"/>
+      <c r="BD3" s="0"/>
+      <c r="BE3" s="0"/>
+      <c r="BF3" s="0"/>
+      <c r="BG3" s="0"/>
+      <c r="BH3" s="0"/>
+      <c r="BI3" s="0"/>
+      <c r="BJ3" s="0"/>
+      <c r="BK3" s="0"/>
+      <c r="BL3" s="0"/>
+      <c r="BM3" s="0"/>
+      <c r="BN3" s="0"/>
+      <c r="BO3" s="0"/>
+      <c r="BP3" s="0"/>
+      <c r="BQ3" s="0"/>
+      <c r="BR3" s="0"/>
+      <c r="BS3" s="0"/>
+      <c r="BT3" s="0"/>
+      <c r="BU3" s="0"/>
+      <c r="BV3" s="0"/>
+      <c r="BW3" s="0"/>
+      <c r="BX3" s="0"/>
+      <c r="BY3" s="0"/>
+      <c r="BZ3" s="0"/>
+      <c r="CA3" s="0"/>
+      <c r="CB3" s="0"/>
+      <c r="CC3" s="0"/>
+      <c r="CD3" s="0"/>
+      <c r="CE3" s="0"/>
+      <c r="CF3" s="0"/>
+      <c r="CG3" s="0"/>
+      <c r="CH3" s="0"/>
+      <c r="CI3" s="0"/>
+      <c r="CJ3" s="0"/>
+      <c r="CK3" s="0"/>
+      <c r="CL3" s="0"/>
+      <c r="CM3" s="0"/>
+      <c r="CN3" s="0"/>
+      <c r="CO3" s="0"/>
+      <c r="CP3" s="0"/>
+      <c r="CQ3" s="0"/>
+      <c r="CR3" s="0"/>
+      <c r="CS3" s="0"/>
+      <c r="CT3" s="0"/>
+      <c r="CU3" s="0"/>
+      <c r="CV3" s="0"/>
+      <c r="CW3" s="0"/>
+      <c r="CX3" s="0"/>
+      <c r="CY3" s="0"/>
+      <c r="CZ3" s="0"/>
+      <c r="DA3" s="0"/>
+      <c r="DB3" s="0"/>
+      <c r="DC3" s="0"/>
+      <c r="DD3" s="0"/>
+      <c r="DE3" s="0"/>
+      <c r="DF3" s="0"/>
+      <c r="DG3" s="0"/>
+      <c r="DH3" s="0"/>
+      <c r="DI3" s="0"/>
+      <c r="DJ3" s="0"/>
+      <c r="DK3" s="0"/>
+      <c r="DL3" s="0"/>
+      <c r="DM3" s="0"/>
+      <c r="DN3" s="0"/>
+      <c r="DO3" s="0"/>
+      <c r="DP3" s="0"/>
+      <c r="DQ3" s="0"/>
+      <c r="DR3" s="0"/>
+      <c r="DS3" s="0"/>
+      <c r="DT3" s="0"/>
+      <c r="DU3" s="0"/>
+      <c r="DV3" s="0"/>
+      <c r="DW3" s="0"/>
+      <c r="DX3" s="0"/>
+      <c r="DY3" s="0"/>
+      <c r="DZ3" s="0"/>
+      <c r="EA3" s="0"/>
+      <c r="EB3" s="0"/>
+      <c r="EC3" s="0"/>
+      <c r="ED3" s="0"/>
+      <c r="EE3" s="0"/>
+      <c r="EF3" s="0"/>
+      <c r="EG3" s="0"/>
+      <c r="EH3" s="0"/>
+      <c r="EI3" s="0"/>
+      <c r="EJ3" s="0"/>
+      <c r="EK3" s="0"/>
+      <c r="EL3" s="0"/>
+      <c r="EM3" s="0"/>
+      <c r="EN3" s="0"/>
+      <c r="EO3" s="0"/>
+      <c r="EP3" s="0"/>
+      <c r="EQ3" s="0"/>
+      <c r="ER3" s="0"/>
+      <c r="ES3" s="0"/>
+      <c r="ET3" s="0"/>
+      <c r="EU3" s="0"/>
+      <c r="EV3" s="0"/>
+      <c r="EW3" s="0"/>
+      <c r="EX3" s="0"/>
+      <c r="EY3" s="0"/>
+      <c r="EZ3" s="0"/>
+      <c r="FA3" s="0"/>
+      <c r="FB3" s="0"/>
+      <c r="FC3" s="0"/>
+      <c r="FD3" s="0"/>
+      <c r="FE3" s="0"/>
+      <c r="FF3" s="0"/>
+      <c r="FG3" s="0"/>
+      <c r="FH3" s="0"/>
+      <c r="FI3" s="0"/>
+      <c r="FJ3" s="0"/>
+      <c r="FK3" s="0"/>
+      <c r="FL3" s="0"/>
+      <c r="FM3" s="0"/>
+      <c r="FN3" s="0"/>
+      <c r="FO3" s="0"/>
+      <c r="FP3" s="0"/>
+      <c r="FQ3" s="0"/>
+      <c r="FR3" s="0"/>
+      <c r="FS3" s="0"/>
+      <c r="FT3" s="0"/>
+      <c r="FU3" s="0"/>
+      <c r="FV3" s="0"/>
+      <c r="FW3" s="0"/>
+      <c r="FX3" s="0"/>
+      <c r="FY3" s="0"/>
+      <c r="FZ3" s="0"/>
+      <c r="GA3" s="0"/>
+      <c r="GB3" s="0"/>
+      <c r="GC3" s="0"/>
+      <c r="GD3" s="0"/>
+      <c r="GE3" s="0"/>
+      <c r="GF3" s="0"/>
+      <c r="GG3" s="0"/>
+      <c r="GH3" s="0"/>
+      <c r="GI3" s="0"/>
+      <c r="GJ3" s="0"/>
+      <c r="GK3" s="0"/>
+      <c r="GL3" s="0"/>
+      <c r="GM3" s="0"/>
+      <c r="GN3" s="0"/>
+      <c r="GO3" s="0"/>
+      <c r="GP3" s="0"/>
+      <c r="GQ3" s="0"/>
+      <c r="GR3" s="0"/>
+      <c r="GS3" s="0"/>
+      <c r="GT3" s="0"/>
+      <c r="GU3" s="0"/>
+      <c r="GV3" s="0"/>
+      <c r="GW3" s="0"/>
+      <c r="GX3" s="0"/>
+      <c r="GY3" s="0"/>
+      <c r="GZ3" s="0"/>
+      <c r="HA3" s="0"/>
+      <c r="HB3" s="0"/>
+      <c r="HC3" s="0"/>
+      <c r="HD3" s="0"/>
+      <c r="HE3" s="0"/>
+      <c r="HF3" s="0"/>
+      <c r="HG3" s="0"/>
+      <c r="HH3" s="0"/>
+      <c r="HI3" s="0"/>
+      <c r="HJ3" s="0"/>
+      <c r="HK3" s="0"/>
+      <c r="HL3" s="0"/>
+      <c r="HM3" s="0"/>
+      <c r="HN3" s="0"/>
+      <c r="HO3" s="0"/>
+      <c r="HP3" s="0"/>
+      <c r="HQ3" s="0"/>
+      <c r="HR3" s="0"/>
+      <c r="HS3" s="0"/>
+      <c r="HT3" s="0"/>
+      <c r="HU3" s="0"/>
+      <c r="HV3" s="0"/>
+      <c r="HW3" s="0"/>
+      <c r="HX3" s="0"/>
+      <c r="HY3" s="0"/>
+      <c r="HZ3" s="0"/>
+      <c r="IA3" s="0"/>
+      <c r="IB3" s="0"/>
+      <c r="IC3" s="0"/>
+      <c r="ID3" s="0"/>
+      <c r="IE3" s="0"/>
+      <c r="IF3" s="0"/>
+      <c r="IG3" s="0"/>
+      <c r="IH3" s="0"/>
+      <c r="II3" s="0"/>
+      <c r="IJ3" s="0"/>
+      <c r="IK3" s="0"/>
+      <c r="IL3" s="0"/>
+      <c r="IM3" s="0"/>
+      <c r="IN3" s="0"/>
+      <c r="IO3" s="0"/>
+      <c r="IP3" s="0"/>
+      <c r="IQ3" s="0"/>
+      <c r="IR3" s="0"/>
+      <c r="IS3" s="0"/>
+      <c r="IT3" s="0"/>
+      <c r="IU3" s="0"/>
+      <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
+      <c r="IX3" s="0"/>
+      <c r="IY3" s="0"/>
+      <c r="IZ3" s="0"/>
+      <c r="JA3" s="0"/>
+      <c r="JB3" s="0"/>
+      <c r="JC3" s="0"/>
+      <c r="JD3" s="0"/>
+      <c r="JE3" s="0"/>
+      <c r="JF3" s="0"/>
+      <c r="JG3" s="0"/>
+      <c r="JH3" s="0"/>
+      <c r="JI3" s="0"/>
+      <c r="JJ3" s="0"/>
+      <c r="JK3" s="0"/>
+      <c r="JL3" s="0"/>
+      <c r="JM3" s="0"/>
+      <c r="JN3" s="0"/>
+      <c r="JO3" s="0"/>
+      <c r="JP3" s="0"/>
+      <c r="JQ3" s="0"/>
+      <c r="JR3" s="0"/>
+      <c r="JS3" s="0"/>
+      <c r="JT3" s="0"/>
+      <c r="JU3" s="0"/>
+      <c r="JV3" s="0"/>
+      <c r="JW3" s="0"/>
+      <c r="JX3" s="0"/>
+      <c r="JY3" s="0"/>
+      <c r="JZ3" s="0"/>
+      <c r="KA3" s="0"/>
+      <c r="KB3" s="0"/>
+      <c r="KC3" s="0"/>
+      <c r="KD3" s="0"/>
+      <c r="KE3" s="0"/>
+      <c r="KF3" s="0"/>
+      <c r="KG3" s="0"/>
+      <c r="KH3" s="0"/>
+      <c r="KI3" s="0"/>
+      <c r="KJ3" s="0"/>
+      <c r="KK3" s="0"/>
+      <c r="KL3" s="0"/>
+      <c r="KM3" s="0"/>
+      <c r="KN3" s="0"/>
+      <c r="KO3" s="0"/>
+      <c r="KP3" s="0"/>
+      <c r="KQ3" s="0"/>
+      <c r="KR3" s="0"/>
+      <c r="KS3" s="0"/>
+      <c r="KT3" s="0"/>
+      <c r="KU3" s="0"/>
+      <c r="KV3" s="0"/>
+      <c r="KW3" s="0"/>
+      <c r="KX3" s="0"/>
+      <c r="KY3" s="0"/>
+      <c r="KZ3" s="0"/>
+      <c r="LA3" s="0"/>
+      <c r="LB3" s="0"/>
+      <c r="LC3" s="0"/>
+      <c r="LD3" s="0"/>
+      <c r="LE3" s="0"/>
+      <c r="LF3" s="0"/>
+      <c r="LG3" s="0"/>
+      <c r="LH3" s="0"/>
+      <c r="LI3" s="0"/>
+      <c r="LJ3" s="0"/>
+      <c r="LK3" s="0"/>
+      <c r="LL3" s="0"/>
+      <c r="LM3" s="0"/>
+      <c r="LN3" s="0"/>
+      <c r="LO3" s="0"/>
+      <c r="LP3" s="0"/>
+      <c r="LQ3" s="0"/>
+      <c r="LR3" s="0"/>
+      <c r="LS3" s="0"/>
+      <c r="LT3" s="0"/>
+      <c r="LU3" s="0"/>
+      <c r="LV3" s="0"/>
+      <c r="LW3" s="0"/>
+      <c r="LX3" s="0"/>
+      <c r="LY3" s="0"/>
+      <c r="LZ3" s="0"/>
+      <c r="MA3" s="0"/>
+      <c r="MB3" s="0"/>
+      <c r="MC3" s="0"/>
+      <c r="MD3" s="0"/>
+      <c r="ME3" s="0"/>
+      <c r="MF3" s="0"/>
+      <c r="MG3" s="0"/>
+      <c r="MH3" s="0"/>
+      <c r="MI3" s="0"/>
+      <c r="MJ3" s="0"/>
+      <c r="MK3" s="0"/>
+      <c r="ML3" s="0"/>
+      <c r="MM3" s="0"/>
+      <c r="MN3" s="0"/>
+      <c r="MO3" s="0"/>
+      <c r="MP3" s="0"/>
+      <c r="MQ3" s="0"/>
+      <c r="MR3" s="0"/>
+      <c r="MS3" s="0"/>
+      <c r="MT3" s="0"/>
+      <c r="MU3" s="0"/>
+      <c r="MV3" s="0"/>
+      <c r="MW3" s="0"/>
+      <c r="MX3" s="0"/>
+      <c r="MY3" s="0"/>
+      <c r="MZ3" s="0"/>
+      <c r="NA3" s="0"/>
+      <c r="NB3" s="0"/>
+      <c r="NC3" s="0"/>
+      <c r="ND3" s="0"/>
+      <c r="NE3" s="0"/>
+      <c r="NF3" s="0"/>
+      <c r="NG3" s="0"/>
+      <c r="NH3" s="0"/>
+      <c r="NI3" s="0"/>
+      <c r="NJ3" s="0"/>
+      <c r="NK3" s="0"/>
+      <c r="NL3" s="0"/>
+      <c r="NM3" s="0"/>
+      <c r="NN3" s="0"/>
+      <c r="NO3" s="0"/>
+      <c r="NP3" s="0"/>
+      <c r="NQ3" s="0"/>
+      <c r="NR3" s="0"/>
+      <c r="NS3" s="0"/>
+      <c r="NT3" s="0"/>
+      <c r="NU3" s="0"/>
+      <c r="NV3" s="0"/>
+      <c r="NW3" s="0"/>
+      <c r="NX3" s="0"/>
+      <c r="NY3" s="0"/>
+      <c r="NZ3" s="0"/>
+      <c r="OA3" s="0"/>
+      <c r="OB3" s="0"/>
+      <c r="OC3" s="0"/>
+      <c r="OD3" s="0"/>
+      <c r="OE3" s="0"/>
+      <c r="OF3" s="0"/>
+      <c r="OG3" s="0"/>
+      <c r="OH3" s="0"/>
+      <c r="OI3" s="0"/>
+      <c r="OJ3" s="0"/>
+      <c r="OK3" s="0"/>
+      <c r="OL3" s="0"/>
+      <c r="OM3" s="0"/>
+      <c r="ON3" s="0"/>
+      <c r="OO3" s="0"/>
+      <c r="OP3" s="0"/>
+      <c r="OQ3" s="0"/>
+      <c r="OR3" s="0"/>
+      <c r="OS3" s="0"/>
+      <c r="OT3" s="0"/>
+      <c r="OU3" s="0"/>
+      <c r="OV3" s="0"/>
+      <c r="OW3" s="0"/>
+      <c r="OX3" s="0"/>
+      <c r="OY3" s="0"/>
+      <c r="OZ3" s="0"/>
+      <c r="PA3" s="0"/>
+      <c r="PB3" s="0"/>
+      <c r="PC3" s="0"/>
+      <c r="PD3" s="0"/>
+      <c r="PE3" s="0"/>
+      <c r="PF3" s="0"/>
+      <c r="PG3" s="0"/>
+      <c r="PH3" s="0"/>
+      <c r="PI3" s="0"/>
+      <c r="PJ3" s="0"/>
+      <c r="PK3" s="0"/>
+      <c r="PL3" s="0"/>
+      <c r="PM3" s="0"/>
+      <c r="PN3" s="0"/>
+      <c r="PO3" s="0"/>
+      <c r="PP3" s="0"/>
+      <c r="PQ3" s="0"/>
+      <c r="PR3" s="0"/>
+      <c r="PS3" s="0"/>
+      <c r="PT3" s="0"/>
+      <c r="PU3" s="0"/>
+      <c r="PV3" s="0"/>
+      <c r="PW3" s="0"/>
+      <c r="PX3" s="0"/>
+      <c r="PY3" s="0"/>
+      <c r="PZ3" s="0"/>
+      <c r="QA3" s="0"/>
+      <c r="QB3" s="0"/>
+      <c r="QC3" s="0"/>
+      <c r="QD3" s="0"/>
+      <c r="QE3" s="0"/>
+      <c r="QF3" s="0"/>
+      <c r="QG3" s="0"/>
+      <c r="QH3" s="0"/>
+      <c r="QI3" s="0"/>
+      <c r="QJ3" s="0"/>
+      <c r="QK3" s="0"/>
+      <c r="QL3" s="0"/>
+      <c r="QM3" s="0"/>
+      <c r="QN3" s="0"/>
+      <c r="QO3" s="0"/>
+      <c r="QP3" s="0"/>
+      <c r="QQ3" s="0"/>
+      <c r="QR3" s="0"/>
+      <c r="QS3" s="0"/>
+      <c r="QT3" s="0"/>
+      <c r="QU3" s="0"/>
+      <c r="QV3" s="0"/>
+      <c r="QW3" s="0"/>
+      <c r="QX3" s="0"/>
+      <c r="QY3" s="0"/>
+      <c r="QZ3" s="0"/>
+      <c r="RA3" s="0"/>
+      <c r="RB3" s="0"/>
+      <c r="RC3" s="0"/>
+      <c r="RD3" s="0"/>
+      <c r="RE3" s="0"/>
+      <c r="RF3" s="0"/>
+      <c r="RG3" s="0"/>
+      <c r="RH3" s="0"/>
+      <c r="RI3" s="0"/>
+      <c r="RJ3" s="0"/>
+      <c r="RK3" s="0"/>
+      <c r="RL3" s="0"/>
+      <c r="RM3" s="0"/>
+      <c r="RN3" s="0"/>
+      <c r="RO3" s="0"/>
+      <c r="RP3" s="0"/>
+      <c r="RQ3" s="0"/>
+      <c r="RR3" s="0"/>
+      <c r="RS3" s="0"/>
+      <c r="RT3" s="0"/>
+      <c r="RU3" s="0"/>
+      <c r="RV3" s="0"/>
+      <c r="RW3" s="0"/>
+      <c r="RX3" s="0"/>
+      <c r="RY3" s="0"/>
+      <c r="RZ3" s="0"/>
+      <c r="SA3" s="0"/>
+      <c r="SB3" s="0"/>
+      <c r="SC3" s="0"/>
+      <c r="SD3" s="0"/>
+      <c r="SE3" s="0"/>
+      <c r="SF3" s="0"/>
+      <c r="SG3" s="0"/>
+      <c r="SH3" s="0"/>
+      <c r="SI3" s="0"/>
+      <c r="SJ3" s="0"/>
+      <c r="SK3" s="0"/>
+      <c r="SL3" s="0"/>
+      <c r="SM3" s="0"/>
+      <c r="SN3" s="0"/>
+      <c r="SO3" s="0"/>
+      <c r="SP3" s="0"/>
+      <c r="SQ3" s="0"/>
+      <c r="SR3" s="0"/>
+      <c r="SS3" s="0"/>
+      <c r="ST3" s="0"/>
+      <c r="SU3" s="0"/>
+      <c r="SV3" s="0"/>
+      <c r="SW3" s="0"/>
+      <c r="SX3" s="0"/>
+      <c r="SY3" s="0"/>
+      <c r="SZ3" s="0"/>
+      <c r="TA3" s="0"/>
+      <c r="TB3" s="0"/>
+      <c r="TC3" s="0"/>
+      <c r="TD3" s="0"/>
+      <c r="TE3" s="0"/>
+      <c r="TF3" s="0"/>
+      <c r="TG3" s="0"/>
+      <c r="TH3" s="0"/>
+      <c r="TI3" s="0"/>
+      <c r="TJ3" s="0"/>
+      <c r="TK3" s="0"/>
+      <c r="TL3" s="0"/>
+      <c r="TM3" s="0"/>
+      <c r="TN3" s="0"/>
+      <c r="TO3" s="0"/>
+      <c r="TP3" s="0"/>
+      <c r="TQ3" s="0"/>
+      <c r="TR3" s="0"/>
+      <c r="TS3" s="0"/>
+      <c r="TT3" s="0"/>
+      <c r="TU3" s="0"/>
+      <c r="TV3" s="0"/>
+      <c r="TW3" s="0"/>
+      <c r="TX3" s="0"/>
+      <c r="TY3" s="0"/>
+      <c r="TZ3" s="0"/>
+      <c r="UA3" s="0"/>
+      <c r="UB3" s="0"/>
+      <c r="UC3" s="0"/>
+      <c r="UD3" s="0"/>
+      <c r="UE3" s="0"/>
+      <c r="UF3" s="0"/>
+      <c r="UG3" s="0"/>
+      <c r="UH3" s="0"/>
+      <c r="UI3" s="0"/>
+      <c r="UJ3" s="0"/>
+      <c r="UK3" s="0"/>
+      <c r="UL3" s="0"/>
+      <c r="UM3" s="0"/>
+      <c r="UN3" s="0"/>
+      <c r="UO3" s="0"/>
+      <c r="UP3" s="0"/>
+      <c r="UQ3" s="0"/>
+      <c r="UR3" s="0"/>
+      <c r="US3" s="0"/>
+      <c r="UT3" s="0"/>
+      <c r="UU3" s="0"/>
+      <c r="UV3" s="0"/>
+      <c r="UW3" s="0"/>
+      <c r="UX3" s="0"/>
+      <c r="UY3" s="0"/>
+      <c r="UZ3" s="0"/>
+      <c r="VA3" s="0"/>
+      <c r="VB3" s="0"/>
+      <c r="VC3" s="0"/>
+      <c r="VD3" s="0"/>
+      <c r="VE3" s="0"/>
+      <c r="VF3" s="0"/>
+      <c r="VG3" s="0"/>
+      <c r="VH3" s="0"/>
+      <c r="VI3" s="0"/>
+      <c r="VJ3" s="0"/>
+      <c r="VK3" s="0"/>
+      <c r="VL3" s="0"/>
+      <c r="VM3" s="0"/>
+      <c r="VN3" s="0"/>
+      <c r="VO3" s="0"/>
+      <c r="VP3" s="0"/>
+      <c r="VQ3" s="0"/>
+      <c r="VR3" s="0"/>
+      <c r="VS3" s="0"/>
+      <c r="VT3" s="0"/>
+      <c r="VU3" s="0"/>
+      <c r="VV3" s="0"/>
+      <c r="VW3" s="0"/>
+      <c r="VX3" s="0"/>
+      <c r="VY3" s="0"/>
+      <c r="VZ3" s="0"/>
+      <c r="WA3" s="0"/>
+      <c r="WB3" s="0"/>
+      <c r="WC3" s="0"/>
+      <c r="WD3" s="0"/>
+      <c r="WE3" s="0"/>
+      <c r="WF3" s="0"/>
+      <c r="WG3" s="0"/>
+      <c r="WH3" s="0"/>
+      <c r="WI3" s="0"/>
+      <c r="WJ3" s="0"/>
+      <c r="WK3" s="0"/>
+      <c r="WL3" s="0"/>
+      <c r="WM3" s="0"/>
+      <c r="WN3" s="0"/>
+      <c r="WO3" s="0"/>
+      <c r="WP3" s="0"/>
+      <c r="WQ3" s="0"/>
+      <c r="WR3" s="0"/>
+      <c r="WS3" s="0"/>
+      <c r="WT3" s="0"/>
+      <c r="WU3" s="0"/>
+      <c r="WV3" s="0"/>
+      <c r="WW3" s="0"/>
+      <c r="WX3" s="0"/>
+      <c r="WY3" s="0"/>
+      <c r="WZ3" s="0"/>
+      <c r="XA3" s="0"/>
+      <c r="XB3" s="0"/>
+      <c r="XC3" s="0"/>
+      <c r="XD3" s="0"/>
+      <c r="XE3" s="0"/>
+      <c r="XF3" s="0"/>
+      <c r="XG3" s="0"/>
+      <c r="XH3" s="0"/>
+      <c r="XI3" s="0"/>
+      <c r="XJ3" s="0"/>
+      <c r="XK3" s="0"/>
+      <c r="XL3" s="0"/>
+      <c r="XM3" s="0"/>
+      <c r="XN3" s="0"/>
+      <c r="XO3" s="0"/>
+      <c r="XP3" s="0"/>
+      <c r="XQ3" s="0"/>
+      <c r="XR3" s="0"/>
+      <c r="XS3" s="0"/>
+      <c r="XT3" s="0"/>
+      <c r="XU3" s="0"/>
+      <c r="XV3" s="0"/>
+      <c r="XW3" s="0"/>
+      <c r="XX3" s="0"/>
+      <c r="XY3" s="0"/>
+      <c r="XZ3" s="0"/>
+      <c r="YA3" s="0"/>
+      <c r="YB3" s="0"/>
+      <c r="YC3" s="0"/>
+      <c r="YD3" s="0"/>
+      <c r="YE3" s="0"/>
+      <c r="YF3" s="0"/>
+      <c r="YG3" s="0"/>
+      <c r="YH3" s="0"/>
+      <c r="YI3" s="0"/>
+      <c r="YJ3" s="0"/>
+      <c r="YK3" s="0"/>
+      <c r="YL3" s="0"/>
+      <c r="YM3" s="0"/>
+      <c r="YN3" s="0"/>
+      <c r="YO3" s="0"/>
+      <c r="YP3" s="0"/>
+      <c r="YQ3" s="0"/>
+      <c r="YR3" s="0"/>
+      <c r="YS3" s="0"/>
+      <c r="YT3" s="0"/>
+      <c r="YU3" s="0"/>
+      <c r="YV3" s="0"/>
+      <c r="YW3" s="0"/>
+      <c r="YX3" s="0"/>
+      <c r="YY3" s="0"/>
+      <c r="YZ3" s="0"/>
+      <c r="ZA3" s="0"/>
+      <c r="ZB3" s="0"/>
+      <c r="ZC3" s="0"/>
+      <c r="ZD3" s="0"/>
+      <c r="ZE3" s="0"/>
+      <c r="ZF3" s="0"/>
+      <c r="ZG3" s="0"/>
+      <c r="ZH3" s="0"/>
+      <c r="ZI3" s="0"/>
+      <c r="ZJ3" s="0"/>
+      <c r="ZK3" s="0"/>
+      <c r="ZL3" s="0"/>
+      <c r="ZM3" s="0"/>
+      <c r="ZN3" s="0"/>
+      <c r="ZO3" s="0"/>
+      <c r="ZP3" s="0"/>
+      <c r="ZQ3" s="0"/>
+      <c r="ZR3" s="0"/>
+      <c r="ZS3" s="0"/>
+      <c r="ZT3" s="0"/>
+      <c r="ZU3" s="0"/>
+      <c r="ZV3" s="0"/>
+      <c r="ZW3" s="0"/>
+      <c r="ZX3" s="0"/>
+      <c r="ZY3" s="0"/>
+      <c r="ZZ3" s="0"/>
+      <c r="AAA3" s="0"/>
+      <c r="AAB3" s="0"/>
+      <c r="AAC3" s="0"/>
+      <c r="AAD3" s="0"/>
+      <c r="AAE3" s="0"/>
+      <c r="AAF3" s="0"/>
+      <c r="AAG3" s="0"/>
+      <c r="AAH3" s="0"/>
+      <c r="AAI3" s="0"/>
+      <c r="AAJ3" s="0"/>
+      <c r="AAK3" s="0"/>
+      <c r="AAL3" s="0"/>
+      <c r="AAM3" s="0"/>
+      <c r="AAN3" s="0"/>
+      <c r="AAO3" s="0"/>
+      <c r="AAP3" s="0"/>
+      <c r="AAQ3" s="0"/>
+      <c r="AAR3" s="0"/>
+      <c r="AAS3" s="0"/>
+      <c r="AAT3" s="0"/>
+      <c r="AAU3" s="0"/>
+      <c r="AAV3" s="0"/>
+      <c r="AAW3" s="0"/>
+      <c r="AAX3" s="0"/>
+      <c r="AAY3" s="0"/>
+      <c r="AAZ3" s="0"/>
+      <c r="ABA3" s="0"/>
+      <c r="ABB3" s="0"/>
+      <c r="ABC3" s="0"/>
+      <c r="ABD3" s="0"/>
+      <c r="ABE3" s="0"/>
+      <c r="ABF3" s="0"/>
+      <c r="ABG3" s="0"/>
+      <c r="ABH3" s="0"/>
+      <c r="ABI3" s="0"/>
+      <c r="ABJ3" s="0"/>
+      <c r="ABK3" s="0"/>
+      <c r="ABL3" s="0"/>
+      <c r="ABM3" s="0"/>
+      <c r="ABN3" s="0"/>
+      <c r="ABO3" s="0"/>
+      <c r="ABP3" s="0"/>
+      <c r="ABQ3" s="0"/>
+      <c r="ABR3" s="0"/>
+      <c r="ABS3" s="0"/>
+      <c r="ABT3" s="0"/>
+      <c r="ABU3" s="0"/>
+      <c r="ABV3" s="0"/>
+      <c r="ABW3" s="0"/>
+      <c r="ABX3" s="0"/>
+      <c r="ABY3" s="0"/>
+      <c r="ABZ3" s="0"/>
+      <c r="ACA3" s="0"/>
+      <c r="ACB3" s="0"/>
+      <c r="ACC3" s="0"/>
+      <c r="ACD3" s="0"/>
+      <c r="ACE3" s="0"/>
+      <c r="ACF3" s="0"/>
+      <c r="ACG3" s="0"/>
+      <c r="ACH3" s="0"/>
+      <c r="ACI3" s="0"/>
+      <c r="ACJ3" s="0"/>
+      <c r="ACK3" s="0"/>
+      <c r="ACL3" s="0"/>
+      <c r="ACM3" s="0"/>
+      <c r="ACN3" s="0"/>
+      <c r="ACO3" s="0"/>
+      <c r="ACP3" s="0"/>
+      <c r="ACQ3" s="0"/>
+      <c r="ACR3" s="0"/>
+      <c r="ACS3" s="0"/>
+      <c r="ACT3" s="0"/>
+      <c r="ACU3" s="0"/>
+      <c r="ACV3" s="0"/>
+      <c r="ACW3" s="0"/>
+      <c r="ACX3" s="0"/>
+      <c r="ACY3" s="0"/>
+      <c r="ACZ3" s="0"/>
+      <c r="ADA3" s="0"/>
+      <c r="ADB3" s="0"/>
+      <c r="ADC3" s="0"/>
+      <c r="ADD3" s="0"/>
+      <c r="ADE3" s="0"/>
+      <c r="ADF3" s="0"/>
+      <c r="ADG3" s="0"/>
+      <c r="ADH3" s="0"/>
+      <c r="ADI3" s="0"/>
+      <c r="ADJ3" s="0"/>
+      <c r="ADK3" s="0"/>
+      <c r="ADL3" s="0"/>
+      <c r="ADM3" s="0"/>
+      <c r="ADN3" s="0"/>
+      <c r="ADO3" s="0"/>
+      <c r="ADP3" s="0"/>
+      <c r="ADQ3" s="0"/>
+      <c r="ADR3" s="0"/>
+      <c r="ADS3" s="0"/>
+      <c r="ADT3" s="0"/>
+      <c r="ADU3" s="0"/>
+      <c r="ADV3" s="0"/>
+      <c r="ADW3" s="0"/>
+      <c r="ADX3" s="0"/>
+      <c r="ADY3" s="0"/>
+      <c r="ADZ3" s="0"/>
+      <c r="AEA3" s="0"/>
+      <c r="AEB3" s="0"/>
+      <c r="AEC3" s="0"/>
+      <c r="AED3" s="0"/>
+      <c r="AEE3" s="0"/>
+      <c r="AEF3" s="0"/>
+      <c r="AEG3" s="0"/>
+      <c r="AEH3" s="0"/>
+      <c r="AEI3" s="0"/>
+      <c r="AEJ3" s="0"/>
+      <c r="AEK3" s="0"/>
+      <c r="AEL3" s="0"/>
+      <c r="AEM3" s="0"/>
+      <c r="AEN3" s="0"/>
+      <c r="AEO3" s="0"/>
+      <c r="AEP3" s="0"/>
+      <c r="AEQ3" s="0"/>
+      <c r="AER3" s="0"/>
+      <c r="AES3" s="0"/>
+      <c r="AET3" s="0"/>
+      <c r="AEU3" s="0"/>
+      <c r="AEV3" s="0"/>
+      <c r="AEW3" s="0"/>
+      <c r="AEX3" s="0"/>
+      <c r="AEY3" s="0"/>
+      <c r="AEZ3" s="0"/>
+      <c r="AFA3" s="0"/>
+      <c r="AFB3" s="0"/>
+      <c r="AFC3" s="0"/>
+      <c r="AFD3" s="0"/>
+      <c r="AFE3" s="0"/>
+      <c r="AFF3" s="0"/>
+      <c r="AFG3" s="0"/>
+      <c r="AFH3" s="0"/>
+      <c r="AFI3" s="0"/>
+      <c r="AFJ3" s="0"/>
+      <c r="AFK3" s="0"/>
+      <c r="AFL3" s="0"/>
+      <c r="AFM3" s="0"/>
+      <c r="AFN3" s="0"/>
+      <c r="AFO3" s="0"/>
+      <c r="AFP3" s="0"/>
+      <c r="AFQ3" s="0"/>
+      <c r="AFR3" s="0"/>
+      <c r="AFS3" s="0"/>
+      <c r="AFT3" s="0"/>
+      <c r="AFU3" s="0"/>
+      <c r="AFV3" s="0"/>
+      <c r="AFW3" s="0"/>
+      <c r="AFX3" s="0"/>
+      <c r="AFY3" s="0"/>
+      <c r="AFZ3" s="0"/>
+      <c r="AGA3" s="0"/>
+      <c r="AGB3" s="0"/>
+      <c r="AGC3" s="0"/>
+      <c r="AGD3" s="0"/>
+      <c r="AGE3" s="0"/>
+      <c r="AGF3" s="0"/>
+      <c r="AGG3" s="0"/>
+      <c r="AGH3" s="0"/>
+      <c r="AGI3" s="0"/>
+      <c r="AGJ3" s="0"/>
+      <c r="AGK3" s="0"/>
+      <c r="AGL3" s="0"/>
+      <c r="AGM3" s="0"/>
+      <c r="AGN3" s="0"/>
+      <c r="AGO3" s="0"/>
+      <c r="AGP3" s="0"/>
+      <c r="AGQ3" s="0"/>
+      <c r="AGR3" s="0"/>
+      <c r="AGS3" s="0"/>
+      <c r="AGT3" s="0"/>
+      <c r="AGU3" s="0"/>
+      <c r="AGV3" s="0"/>
+      <c r="AGW3" s="0"/>
+      <c r="AGX3" s="0"/>
+      <c r="AGY3" s="0"/>
+      <c r="AGZ3" s="0"/>
+      <c r="AHA3" s="0"/>
+      <c r="AHB3" s="0"/>
+      <c r="AHC3" s="0"/>
+      <c r="AHD3" s="0"/>
+      <c r="AHE3" s="0"/>
+      <c r="AHF3" s="0"/>
+      <c r="AHG3" s="0"/>
+      <c r="AHH3" s="0"/>
+      <c r="AHI3" s="0"/>
+      <c r="AHJ3" s="0"/>
+      <c r="AHK3" s="0"/>
+      <c r="AHL3" s="0"/>
+      <c r="AHM3" s="0"/>
+      <c r="AHN3" s="0"/>
+      <c r="AHO3" s="0"/>
+      <c r="AHP3" s="0"/>
+      <c r="AHQ3" s="0"/>
+      <c r="AHR3" s="0"/>
+      <c r="AHS3" s="0"/>
+      <c r="AHT3" s="0"/>
+      <c r="AHU3" s="0"/>
+      <c r="AHV3" s="0"/>
+      <c r="AHW3" s="0"/>
+      <c r="AHX3" s="0"/>
+      <c r="AHY3" s="0"/>
+      <c r="AHZ3" s="0"/>
+      <c r="AIA3" s="0"/>
+      <c r="AIB3" s="0"/>
+      <c r="AIC3" s="0"/>
+      <c r="AID3" s="0"/>
+      <c r="AIE3" s="0"/>
+      <c r="AIF3" s="0"/>
+      <c r="AIG3" s="0"/>
+      <c r="AIH3" s="0"/>
+      <c r="AII3" s="0"/>
+      <c r="AIJ3" s="0"/>
+      <c r="AIK3" s="0"/>
+      <c r="AIL3" s="0"/>
+      <c r="AIM3" s="0"/>
+      <c r="AIN3" s="0"/>
+      <c r="AIO3" s="0"/>
+      <c r="AIP3" s="0"/>
+      <c r="AIQ3" s="0"/>
+      <c r="AIR3" s="0"/>
+      <c r="AIS3" s="0"/>
+      <c r="AIT3" s="0"/>
+      <c r="AIU3" s="0"/>
+      <c r="AIV3" s="0"/>
+      <c r="AIW3" s="0"/>
+      <c r="AIX3" s="0"/>
+      <c r="AIY3" s="0"/>
+      <c r="AIZ3" s="0"/>
+      <c r="AJA3" s="0"/>
+      <c r="AJB3" s="0"/>
+      <c r="AJC3" s="0"/>
+      <c r="AJD3" s="0"/>
+      <c r="AJE3" s="0"/>
+      <c r="AJF3" s="0"/>
+      <c r="AJG3" s="0"/>
+      <c r="AJH3" s="0"/>
+      <c r="AJI3" s="0"/>
+      <c r="AJJ3" s="0"/>
+      <c r="AJK3" s="0"/>
+      <c r="AJL3" s="0"/>
+      <c r="AJM3" s="0"/>
+      <c r="AJN3" s="0"/>
+      <c r="AJO3" s="0"/>
+      <c r="AJP3" s="0"/>
+      <c r="AJQ3" s="0"/>
+      <c r="AJR3" s="0"/>
+      <c r="AJS3" s="0"/>
+      <c r="AJT3" s="0"/>
+      <c r="AJU3" s="0"/>
+      <c r="AJV3" s="0"/>
+      <c r="AJW3" s="0"/>
+      <c r="AJX3" s="0"/>
+      <c r="AJY3" s="0"/>
+      <c r="AJZ3" s="0"/>
+      <c r="AKA3" s="0"/>
+      <c r="AKB3" s="0"/>
+      <c r="AKC3" s="0"/>
+      <c r="AKD3" s="0"/>
+      <c r="AKE3" s="0"/>
+      <c r="AKF3" s="0"/>
+      <c r="AKG3" s="0"/>
+      <c r="AKH3" s="0"/>
+      <c r="AKI3" s="0"/>
+      <c r="AKJ3" s="0"/>
+      <c r="AKK3" s="0"/>
+      <c r="AKL3" s="0"/>
+      <c r="AKM3" s="0"/>
+      <c r="AKN3" s="0"/>
+      <c r="AKO3" s="0"/>
+      <c r="AKP3" s="0"/>
+      <c r="AKQ3" s="0"/>
+      <c r="AKR3" s="0"/>
+      <c r="AKS3" s="0"/>
+      <c r="AKT3" s="0"/>
+      <c r="AKU3" s="0"/>
+      <c r="AKV3" s="0"/>
+      <c r="AKW3" s="0"/>
+      <c r="AKX3" s="0"/>
+      <c r="AKY3" s="0"/>
+      <c r="AKZ3" s="0"/>
+      <c r="ALA3" s="0"/>
+      <c r="ALB3" s="0"/>
+      <c r="ALC3" s="0"/>
+      <c r="ALD3" s="0"/>
+      <c r="ALE3" s="0"/>
+      <c r="ALF3" s="0"/>
+      <c r="ALG3" s="0"/>
+      <c r="ALH3" s="0"/>
+      <c r="ALI3" s="0"/>
+      <c r="ALJ3" s="0"/>
+      <c r="ALK3" s="0"/>
+      <c r="ALL3" s="0"/>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="23" customFormat="true" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="69" t="s">
         <v>14</v>
       </c>
@@ -6371,6 +8404,1024 @@
       <c r="F4" s="74" t="n">
         <v>1</v>
       </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
+      <c r="BR4" s="0"/>
+      <c r="BS4" s="0"/>
+      <c r="BT4" s="0"/>
+      <c r="BU4" s="0"/>
+      <c r="BV4" s="0"/>
+      <c r="BW4" s="0"/>
+      <c r="BX4" s="0"/>
+      <c r="BY4" s="0"/>
+      <c r="BZ4" s="0"/>
+      <c r="CA4" s="0"/>
+      <c r="CB4" s="0"/>
+      <c r="CC4" s="0"/>
+      <c r="CD4" s="0"/>
+      <c r="CE4" s="0"/>
+      <c r="CF4" s="0"/>
+      <c r="CG4" s="0"/>
+      <c r="CH4" s="0"/>
+      <c r="CI4" s="0"/>
+      <c r="CJ4" s="0"/>
+      <c r="CK4" s="0"/>
+      <c r="CL4" s="0"/>
+      <c r="CM4" s="0"/>
+      <c r="CN4" s="0"/>
+      <c r="CO4" s="0"/>
+      <c r="CP4" s="0"/>
+      <c r="CQ4" s="0"/>
+      <c r="CR4" s="0"/>
+      <c r="CS4" s="0"/>
+      <c r="CT4" s="0"/>
+      <c r="CU4" s="0"/>
+      <c r="CV4" s="0"/>
+      <c r="CW4" s="0"/>
+      <c r="CX4" s="0"/>
+      <c r="CY4" s="0"/>
+      <c r="CZ4" s="0"/>
+      <c r="DA4" s="0"/>
+      <c r="DB4" s="0"/>
+      <c r="DC4" s="0"/>
+      <c r="DD4" s="0"/>
+      <c r="DE4" s="0"/>
+      <c r="DF4" s="0"/>
+      <c r="DG4" s="0"/>
+      <c r="DH4" s="0"/>
+      <c r="DI4" s="0"/>
+      <c r="DJ4" s="0"/>
+      <c r="DK4" s="0"/>
+      <c r="DL4" s="0"/>
+      <c r="DM4" s="0"/>
+      <c r="DN4" s="0"/>
+      <c r="DO4" s="0"/>
+      <c r="DP4" s="0"/>
+      <c r="DQ4" s="0"/>
+      <c r="DR4" s="0"/>
+      <c r="DS4" s="0"/>
+      <c r="DT4" s="0"/>
+      <c r="DU4" s="0"/>
+      <c r="DV4" s="0"/>
+      <c r="DW4" s="0"/>
+      <c r="DX4" s="0"/>
+      <c r="DY4" s="0"/>
+      <c r="DZ4" s="0"/>
+      <c r="EA4" s="0"/>
+      <c r="EB4" s="0"/>
+      <c r="EC4" s="0"/>
+      <c r="ED4" s="0"/>
+      <c r="EE4" s="0"/>
+      <c r="EF4" s="0"/>
+      <c r="EG4" s="0"/>
+      <c r="EH4" s="0"/>
+      <c r="EI4" s="0"/>
+      <c r="EJ4" s="0"/>
+      <c r="EK4" s="0"/>
+      <c r="EL4" s="0"/>
+      <c r="EM4" s="0"/>
+      <c r="EN4" s="0"/>
+      <c r="EO4" s="0"/>
+      <c r="EP4" s="0"/>
+      <c r="EQ4" s="0"/>
+      <c r="ER4" s="0"/>
+      <c r="ES4" s="0"/>
+      <c r="ET4" s="0"/>
+      <c r="EU4" s="0"/>
+      <c r="EV4" s="0"/>
+      <c r="EW4" s="0"/>
+      <c r="EX4" s="0"/>
+      <c r="EY4" s="0"/>
+      <c r="EZ4" s="0"/>
+      <c r="FA4" s="0"/>
+      <c r="FB4" s="0"/>
+      <c r="FC4" s="0"/>
+      <c r="FD4" s="0"/>
+      <c r="FE4" s="0"/>
+      <c r="FF4" s="0"/>
+      <c r="FG4" s="0"/>
+      <c r="FH4" s="0"/>
+      <c r="FI4" s="0"/>
+      <c r="FJ4" s="0"/>
+      <c r="FK4" s="0"/>
+      <c r="FL4" s="0"/>
+      <c r="FM4" s="0"/>
+      <c r="FN4" s="0"/>
+      <c r="FO4" s="0"/>
+      <c r="FP4" s="0"/>
+      <c r="FQ4" s="0"/>
+      <c r="FR4" s="0"/>
+      <c r="FS4" s="0"/>
+      <c r="FT4" s="0"/>
+      <c r="FU4" s="0"/>
+      <c r="FV4" s="0"/>
+      <c r="FW4" s="0"/>
+      <c r="FX4" s="0"/>
+      <c r="FY4" s="0"/>
+      <c r="FZ4" s="0"/>
+      <c r="GA4" s="0"/>
+      <c r="GB4" s="0"/>
+      <c r="GC4" s="0"/>
+      <c r="GD4" s="0"/>
+      <c r="GE4" s="0"/>
+      <c r="GF4" s="0"/>
+      <c r="GG4" s="0"/>
+      <c r="GH4" s="0"/>
+      <c r="GI4" s="0"/>
+      <c r="GJ4" s="0"/>
+      <c r="GK4" s="0"/>
+      <c r="GL4" s="0"/>
+      <c r="GM4" s="0"/>
+      <c r="GN4" s="0"/>
+      <c r="GO4" s="0"/>
+      <c r="GP4" s="0"/>
+      <c r="GQ4" s="0"/>
+      <c r="GR4" s="0"/>
+      <c r="GS4" s="0"/>
+      <c r="GT4" s="0"/>
+      <c r="GU4" s="0"/>
+      <c r="GV4" s="0"/>
+      <c r="GW4" s="0"/>
+      <c r="GX4" s="0"/>
+      <c r="GY4" s="0"/>
+      <c r="GZ4" s="0"/>
+      <c r="HA4" s="0"/>
+      <c r="HB4" s="0"/>
+      <c r="HC4" s="0"/>
+      <c r="HD4" s="0"/>
+      <c r="HE4" s="0"/>
+      <c r="HF4" s="0"/>
+      <c r="HG4" s="0"/>
+      <c r="HH4" s="0"/>
+      <c r="HI4" s="0"/>
+      <c r="HJ4" s="0"/>
+      <c r="HK4" s="0"/>
+      <c r="HL4" s="0"/>
+      <c r="HM4" s="0"/>
+      <c r="HN4" s="0"/>
+      <c r="HO4" s="0"/>
+      <c r="HP4" s="0"/>
+      <c r="HQ4" s="0"/>
+      <c r="HR4" s="0"/>
+      <c r="HS4" s="0"/>
+      <c r="HT4" s="0"/>
+      <c r="HU4" s="0"/>
+      <c r="HV4" s="0"/>
+      <c r="HW4" s="0"/>
+      <c r="HX4" s="0"/>
+      <c r="HY4" s="0"/>
+      <c r="HZ4" s="0"/>
+      <c r="IA4" s="0"/>
+      <c r="IB4" s="0"/>
+      <c r="IC4" s="0"/>
+      <c r="ID4" s="0"/>
+      <c r="IE4" s="0"/>
+      <c r="IF4" s="0"/>
+      <c r="IG4" s="0"/>
+      <c r="IH4" s="0"/>
+      <c r="II4" s="0"/>
+      <c r="IJ4" s="0"/>
+      <c r="IK4" s="0"/>
+      <c r="IL4" s="0"/>
+      <c r="IM4" s="0"/>
+      <c r="IN4" s="0"/>
+      <c r="IO4" s="0"/>
+      <c r="IP4" s="0"/>
+      <c r="IQ4" s="0"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
+      <c r="IT4" s="0"/>
+      <c r="IU4" s="0"/>
+      <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
+      <c r="IX4" s="0"/>
+      <c r="IY4" s="0"/>
+      <c r="IZ4" s="0"/>
+      <c r="JA4" s="0"/>
+      <c r="JB4" s="0"/>
+      <c r="JC4" s="0"/>
+      <c r="JD4" s="0"/>
+      <c r="JE4" s="0"/>
+      <c r="JF4" s="0"/>
+      <c r="JG4" s="0"/>
+      <c r="JH4" s="0"/>
+      <c r="JI4" s="0"/>
+      <c r="JJ4" s="0"/>
+      <c r="JK4" s="0"/>
+      <c r="JL4" s="0"/>
+      <c r="JM4" s="0"/>
+      <c r="JN4" s="0"/>
+      <c r="JO4" s="0"/>
+      <c r="JP4" s="0"/>
+      <c r="JQ4" s="0"/>
+      <c r="JR4" s="0"/>
+      <c r="JS4" s="0"/>
+      <c r="JT4" s="0"/>
+      <c r="JU4" s="0"/>
+      <c r="JV4" s="0"/>
+      <c r="JW4" s="0"/>
+      <c r="JX4" s="0"/>
+      <c r="JY4" s="0"/>
+      <c r="JZ4" s="0"/>
+      <c r="KA4" s="0"/>
+      <c r="KB4" s="0"/>
+      <c r="KC4" s="0"/>
+      <c r="KD4" s="0"/>
+      <c r="KE4" s="0"/>
+      <c r="KF4" s="0"/>
+      <c r="KG4" s="0"/>
+      <c r="KH4" s="0"/>
+      <c r="KI4" s="0"/>
+      <c r="KJ4" s="0"/>
+      <c r="KK4" s="0"/>
+      <c r="KL4" s="0"/>
+      <c r="KM4" s="0"/>
+      <c r="KN4" s="0"/>
+      <c r="KO4" s="0"/>
+      <c r="KP4" s="0"/>
+      <c r="KQ4" s="0"/>
+      <c r="KR4" s="0"/>
+      <c r="KS4" s="0"/>
+      <c r="KT4" s="0"/>
+      <c r="KU4" s="0"/>
+      <c r="KV4" s="0"/>
+      <c r="KW4" s="0"/>
+      <c r="KX4" s="0"/>
+      <c r="KY4" s="0"/>
+      <c r="KZ4" s="0"/>
+      <c r="LA4" s="0"/>
+      <c r="LB4" s="0"/>
+      <c r="LC4" s="0"/>
+      <c r="LD4" s="0"/>
+      <c r="LE4" s="0"/>
+      <c r="LF4" s="0"/>
+      <c r="LG4" s="0"/>
+      <c r="LH4" s="0"/>
+      <c r="LI4" s="0"/>
+      <c r="LJ4" s="0"/>
+      <c r="LK4" s="0"/>
+      <c r="LL4" s="0"/>
+      <c r="LM4" s="0"/>
+      <c r="LN4" s="0"/>
+      <c r="LO4" s="0"/>
+      <c r="LP4" s="0"/>
+      <c r="LQ4" s="0"/>
+      <c r="LR4" s="0"/>
+      <c r="LS4" s="0"/>
+      <c r="LT4" s="0"/>
+      <c r="LU4" s="0"/>
+      <c r="LV4" s="0"/>
+      <c r="LW4" s="0"/>
+      <c r="LX4" s="0"/>
+      <c r="LY4" s="0"/>
+      <c r="LZ4" s="0"/>
+      <c r="MA4" s="0"/>
+      <c r="MB4" s="0"/>
+      <c r="MC4" s="0"/>
+      <c r="MD4" s="0"/>
+      <c r="ME4" s="0"/>
+      <c r="MF4" s="0"/>
+      <c r="MG4" s="0"/>
+      <c r="MH4" s="0"/>
+      <c r="MI4" s="0"/>
+      <c r="MJ4" s="0"/>
+      <c r="MK4" s="0"/>
+      <c r="ML4" s="0"/>
+      <c r="MM4" s="0"/>
+      <c r="MN4" s="0"/>
+      <c r="MO4" s="0"/>
+      <c r="MP4" s="0"/>
+      <c r="MQ4" s="0"/>
+      <c r="MR4" s="0"/>
+      <c r="MS4" s="0"/>
+      <c r="MT4" s="0"/>
+      <c r="MU4" s="0"/>
+      <c r="MV4" s="0"/>
+      <c r="MW4" s="0"/>
+      <c r="MX4" s="0"/>
+      <c r="MY4" s="0"/>
+      <c r="MZ4" s="0"/>
+      <c r="NA4" s="0"/>
+      <c r="NB4" s="0"/>
+      <c r="NC4" s="0"/>
+      <c r="ND4" s="0"/>
+      <c r="NE4" s="0"/>
+      <c r="NF4" s="0"/>
+      <c r="NG4" s="0"/>
+      <c r="NH4" s="0"/>
+      <c r="NI4" s="0"/>
+      <c r="NJ4" s="0"/>
+      <c r="NK4" s="0"/>
+      <c r="NL4" s="0"/>
+      <c r="NM4" s="0"/>
+      <c r="NN4" s="0"/>
+      <c r="NO4" s="0"/>
+      <c r="NP4" s="0"/>
+      <c r="NQ4" s="0"/>
+      <c r="NR4" s="0"/>
+      <c r="NS4" s="0"/>
+      <c r="NT4" s="0"/>
+      <c r="NU4" s="0"/>
+      <c r="NV4" s="0"/>
+      <c r="NW4" s="0"/>
+      <c r="NX4" s="0"/>
+      <c r="NY4" s="0"/>
+      <c r="NZ4" s="0"/>
+      <c r="OA4" s="0"/>
+      <c r="OB4" s="0"/>
+      <c r="OC4" s="0"/>
+      <c r="OD4" s="0"/>
+      <c r="OE4" s="0"/>
+      <c r="OF4" s="0"/>
+      <c r="OG4" s="0"/>
+      <c r="OH4" s="0"/>
+      <c r="OI4" s="0"/>
+      <c r="OJ4" s="0"/>
+      <c r="OK4" s="0"/>
+      <c r="OL4" s="0"/>
+      <c r="OM4" s="0"/>
+      <c r="ON4" s="0"/>
+      <c r="OO4" s="0"/>
+      <c r="OP4" s="0"/>
+      <c r="OQ4" s="0"/>
+      <c r="OR4" s="0"/>
+      <c r="OS4" s="0"/>
+      <c r="OT4" s="0"/>
+      <c r="OU4" s="0"/>
+      <c r="OV4" s="0"/>
+      <c r="OW4" s="0"/>
+      <c r="OX4" s="0"/>
+      <c r="OY4" s="0"/>
+      <c r="OZ4" s="0"/>
+      <c r="PA4" s="0"/>
+      <c r="PB4" s="0"/>
+      <c r="PC4" s="0"/>
+      <c r="PD4" s="0"/>
+      <c r="PE4" s="0"/>
+      <c r="PF4" s="0"/>
+      <c r="PG4" s="0"/>
+      <c r="PH4" s="0"/>
+      <c r="PI4" s="0"/>
+      <c r="PJ4" s="0"/>
+      <c r="PK4" s="0"/>
+      <c r="PL4" s="0"/>
+      <c r="PM4" s="0"/>
+      <c r="PN4" s="0"/>
+      <c r="PO4" s="0"/>
+      <c r="PP4" s="0"/>
+      <c r="PQ4" s="0"/>
+      <c r="PR4" s="0"/>
+      <c r="PS4" s="0"/>
+      <c r="PT4" s="0"/>
+      <c r="PU4" s="0"/>
+      <c r="PV4" s="0"/>
+      <c r="PW4" s="0"/>
+      <c r="PX4" s="0"/>
+      <c r="PY4" s="0"/>
+      <c r="PZ4" s="0"/>
+      <c r="QA4" s="0"/>
+      <c r="QB4" s="0"/>
+      <c r="QC4" s="0"/>
+      <c r="QD4" s="0"/>
+      <c r="QE4" s="0"/>
+      <c r="QF4" s="0"/>
+      <c r="QG4" s="0"/>
+      <c r="QH4" s="0"/>
+      <c r="QI4" s="0"/>
+      <c r="QJ4" s="0"/>
+      <c r="QK4" s="0"/>
+      <c r="QL4" s="0"/>
+      <c r="QM4" s="0"/>
+      <c r="QN4" s="0"/>
+      <c r="QO4" s="0"/>
+      <c r="QP4" s="0"/>
+      <c r="QQ4" s="0"/>
+      <c r="QR4" s="0"/>
+      <c r="QS4" s="0"/>
+      <c r="QT4" s="0"/>
+      <c r="QU4" s="0"/>
+      <c r="QV4" s="0"/>
+      <c r="QW4" s="0"/>
+      <c r="QX4" s="0"/>
+      <c r="QY4" s="0"/>
+      <c r="QZ4" s="0"/>
+      <c r="RA4" s="0"/>
+      <c r="RB4" s="0"/>
+      <c r="RC4" s="0"/>
+      <c r="RD4" s="0"/>
+      <c r="RE4" s="0"/>
+      <c r="RF4" s="0"/>
+      <c r="RG4" s="0"/>
+      <c r="RH4" s="0"/>
+      <c r="RI4" s="0"/>
+      <c r="RJ4" s="0"/>
+      <c r="RK4" s="0"/>
+      <c r="RL4" s="0"/>
+      <c r="RM4" s="0"/>
+      <c r="RN4" s="0"/>
+      <c r="RO4" s="0"/>
+      <c r="RP4" s="0"/>
+      <c r="RQ4" s="0"/>
+      <c r="RR4" s="0"/>
+      <c r="RS4" s="0"/>
+      <c r="RT4" s="0"/>
+      <c r="RU4" s="0"/>
+      <c r="RV4" s="0"/>
+      <c r="RW4" s="0"/>
+      <c r="RX4" s="0"/>
+      <c r="RY4" s="0"/>
+      <c r="RZ4" s="0"/>
+      <c r="SA4" s="0"/>
+      <c r="SB4" s="0"/>
+      <c r="SC4" s="0"/>
+      <c r="SD4" s="0"/>
+      <c r="SE4" s="0"/>
+      <c r="SF4" s="0"/>
+      <c r="SG4" s="0"/>
+      <c r="SH4" s="0"/>
+      <c r="SI4" s="0"/>
+      <c r="SJ4" s="0"/>
+      <c r="SK4" s="0"/>
+      <c r="SL4" s="0"/>
+      <c r="SM4" s="0"/>
+      <c r="SN4" s="0"/>
+      <c r="SO4" s="0"/>
+      <c r="SP4" s="0"/>
+      <c r="SQ4" s="0"/>
+      <c r="SR4" s="0"/>
+      <c r="SS4" s="0"/>
+      <c r="ST4" s="0"/>
+      <c r="SU4" s="0"/>
+      <c r="SV4" s="0"/>
+      <c r="SW4" s="0"/>
+      <c r="SX4" s="0"/>
+      <c r="SY4" s="0"/>
+      <c r="SZ4" s="0"/>
+      <c r="TA4" s="0"/>
+      <c r="TB4" s="0"/>
+      <c r="TC4" s="0"/>
+      <c r="TD4" s="0"/>
+      <c r="TE4" s="0"/>
+      <c r="TF4" s="0"/>
+      <c r="TG4" s="0"/>
+      <c r="TH4" s="0"/>
+      <c r="TI4" s="0"/>
+      <c r="TJ4" s="0"/>
+      <c r="TK4" s="0"/>
+      <c r="TL4" s="0"/>
+      <c r="TM4" s="0"/>
+      <c r="TN4" s="0"/>
+      <c r="TO4" s="0"/>
+      <c r="TP4" s="0"/>
+      <c r="TQ4" s="0"/>
+      <c r="TR4" s="0"/>
+      <c r="TS4" s="0"/>
+      <c r="TT4" s="0"/>
+      <c r="TU4" s="0"/>
+      <c r="TV4" s="0"/>
+      <c r="TW4" s="0"/>
+      <c r="TX4" s="0"/>
+      <c r="TY4" s="0"/>
+      <c r="TZ4" s="0"/>
+      <c r="UA4" s="0"/>
+      <c r="UB4" s="0"/>
+      <c r="UC4" s="0"/>
+      <c r="UD4" s="0"/>
+      <c r="UE4" s="0"/>
+      <c r="UF4" s="0"/>
+      <c r="UG4" s="0"/>
+      <c r="UH4" s="0"/>
+      <c r="UI4" s="0"/>
+      <c r="UJ4" s="0"/>
+      <c r="UK4" s="0"/>
+      <c r="UL4" s="0"/>
+      <c r="UM4" s="0"/>
+      <c r="UN4" s="0"/>
+      <c r="UO4" s="0"/>
+      <c r="UP4" s="0"/>
+      <c r="UQ4" s="0"/>
+      <c r="UR4" s="0"/>
+      <c r="US4" s="0"/>
+      <c r="UT4" s="0"/>
+      <c r="UU4" s="0"/>
+      <c r="UV4" s="0"/>
+      <c r="UW4" s="0"/>
+      <c r="UX4" s="0"/>
+      <c r="UY4" s="0"/>
+      <c r="UZ4" s="0"/>
+      <c r="VA4" s="0"/>
+      <c r="VB4" s="0"/>
+      <c r="VC4" s="0"/>
+      <c r="VD4" s="0"/>
+      <c r="VE4" s="0"/>
+      <c r="VF4" s="0"/>
+      <c r="VG4" s="0"/>
+      <c r="VH4" s="0"/>
+      <c r="VI4" s="0"/>
+      <c r="VJ4" s="0"/>
+      <c r="VK4" s="0"/>
+      <c r="VL4" s="0"/>
+      <c r="VM4" s="0"/>
+      <c r="VN4" s="0"/>
+      <c r="VO4" s="0"/>
+      <c r="VP4" s="0"/>
+      <c r="VQ4" s="0"/>
+      <c r="VR4" s="0"/>
+      <c r="VS4" s="0"/>
+      <c r="VT4" s="0"/>
+      <c r="VU4" s="0"/>
+      <c r="VV4" s="0"/>
+      <c r="VW4" s="0"/>
+      <c r="VX4" s="0"/>
+      <c r="VY4" s="0"/>
+      <c r="VZ4" s="0"/>
+      <c r="WA4" s="0"/>
+      <c r="WB4" s="0"/>
+      <c r="WC4" s="0"/>
+      <c r="WD4" s="0"/>
+      <c r="WE4" s="0"/>
+      <c r="WF4" s="0"/>
+      <c r="WG4" s="0"/>
+      <c r="WH4" s="0"/>
+      <c r="WI4" s="0"/>
+      <c r="WJ4" s="0"/>
+      <c r="WK4" s="0"/>
+      <c r="WL4" s="0"/>
+      <c r="WM4" s="0"/>
+      <c r="WN4" s="0"/>
+      <c r="WO4" s="0"/>
+      <c r="WP4" s="0"/>
+      <c r="WQ4" s="0"/>
+      <c r="WR4" s="0"/>
+      <c r="WS4" s="0"/>
+      <c r="WT4" s="0"/>
+      <c r="WU4" s="0"/>
+      <c r="WV4" s="0"/>
+      <c r="WW4" s="0"/>
+      <c r="WX4" s="0"/>
+      <c r="WY4" s="0"/>
+      <c r="WZ4" s="0"/>
+      <c r="XA4" s="0"/>
+      <c r="XB4" s="0"/>
+      <c r="XC4" s="0"/>
+      <c r="XD4" s="0"/>
+      <c r="XE4" s="0"/>
+      <c r="XF4" s="0"/>
+      <c r="XG4" s="0"/>
+      <c r="XH4" s="0"/>
+      <c r="XI4" s="0"/>
+      <c r="XJ4" s="0"/>
+      <c r="XK4" s="0"/>
+      <c r="XL4" s="0"/>
+      <c r="XM4" s="0"/>
+      <c r="XN4" s="0"/>
+      <c r="XO4" s="0"/>
+      <c r="XP4" s="0"/>
+      <c r="XQ4" s="0"/>
+      <c r="XR4" s="0"/>
+      <c r="XS4" s="0"/>
+      <c r="XT4" s="0"/>
+      <c r="XU4" s="0"/>
+      <c r="XV4" s="0"/>
+      <c r="XW4" s="0"/>
+      <c r="XX4" s="0"/>
+      <c r="XY4" s="0"/>
+      <c r="XZ4" s="0"/>
+      <c r="YA4" s="0"/>
+      <c r="YB4" s="0"/>
+      <c r="YC4" s="0"/>
+      <c r="YD4" s="0"/>
+      <c r="YE4" s="0"/>
+      <c r="YF4" s="0"/>
+      <c r="YG4" s="0"/>
+      <c r="YH4" s="0"/>
+      <c r="YI4" s="0"/>
+      <c r="YJ4" s="0"/>
+      <c r="YK4" s="0"/>
+      <c r="YL4" s="0"/>
+      <c r="YM4" s="0"/>
+      <c r="YN4" s="0"/>
+      <c r="YO4" s="0"/>
+      <c r="YP4" s="0"/>
+      <c r="YQ4" s="0"/>
+      <c r="YR4" s="0"/>
+      <c r="YS4" s="0"/>
+      <c r="YT4" s="0"/>
+      <c r="YU4" s="0"/>
+      <c r="YV4" s="0"/>
+      <c r="YW4" s="0"/>
+      <c r="YX4" s="0"/>
+      <c r="YY4" s="0"/>
+      <c r="YZ4" s="0"/>
+      <c r="ZA4" s="0"/>
+      <c r="ZB4" s="0"/>
+      <c r="ZC4" s="0"/>
+      <c r="ZD4" s="0"/>
+      <c r="ZE4" s="0"/>
+      <c r="ZF4" s="0"/>
+      <c r="ZG4" s="0"/>
+      <c r="ZH4" s="0"/>
+      <c r="ZI4" s="0"/>
+      <c r="ZJ4" s="0"/>
+      <c r="ZK4" s="0"/>
+      <c r="ZL4" s="0"/>
+      <c r="ZM4" s="0"/>
+      <c r="ZN4" s="0"/>
+      <c r="ZO4" s="0"/>
+      <c r="ZP4" s="0"/>
+      <c r="ZQ4" s="0"/>
+      <c r="ZR4" s="0"/>
+      <c r="ZS4" s="0"/>
+      <c r="ZT4" s="0"/>
+      <c r="ZU4" s="0"/>
+      <c r="ZV4" s="0"/>
+      <c r="ZW4" s="0"/>
+      <c r="ZX4" s="0"/>
+      <c r="ZY4" s="0"/>
+      <c r="ZZ4" s="0"/>
+      <c r="AAA4" s="0"/>
+      <c r="AAB4" s="0"/>
+      <c r="AAC4" s="0"/>
+      <c r="AAD4" s="0"/>
+      <c r="AAE4" s="0"/>
+      <c r="AAF4" s="0"/>
+      <c r="AAG4" s="0"/>
+      <c r="AAH4" s="0"/>
+      <c r="AAI4" s="0"/>
+      <c r="AAJ4" s="0"/>
+      <c r="AAK4" s="0"/>
+      <c r="AAL4" s="0"/>
+      <c r="AAM4" s="0"/>
+      <c r="AAN4" s="0"/>
+      <c r="AAO4" s="0"/>
+      <c r="AAP4" s="0"/>
+      <c r="AAQ4" s="0"/>
+      <c r="AAR4" s="0"/>
+      <c r="AAS4" s="0"/>
+      <c r="AAT4" s="0"/>
+      <c r="AAU4" s="0"/>
+      <c r="AAV4" s="0"/>
+      <c r="AAW4" s="0"/>
+      <c r="AAX4" s="0"/>
+      <c r="AAY4" s="0"/>
+      <c r="AAZ4" s="0"/>
+      <c r="ABA4" s="0"/>
+      <c r="ABB4" s="0"/>
+      <c r="ABC4" s="0"/>
+      <c r="ABD4" s="0"/>
+      <c r="ABE4" s="0"/>
+      <c r="ABF4" s="0"/>
+      <c r="ABG4" s="0"/>
+      <c r="ABH4" s="0"/>
+      <c r="ABI4" s="0"/>
+      <c r="ABJ4" s="0"/>
+      <c r="ABK4" s="0"/>
+      <c r="ABL4" s="0"/>
+      <c r="ABM4" s="0"/>
+      <c r="ABN4" s="0"/>
+      <c r="ABO4" s="0"/>
+      <c r="ABP4" s="0"/>
+      <c r="ABQ4" s="0"/>
+      <c r="ABR4" s="0"/>
+      <c r="ABS4" s="0"/>
+      <c r="ABT4" s="0"/>
+      <c r="ABU4" s="0"/>
+      <c r="ABV4" s="0"/>
+      <c r="ABW4" s="0"/>
+      <c r="ABX4" s="0"/>
+      <c r="ABY4" s="0"/>
+      <c r="ABZ4" s="0"/>
+      <c r="ACA4" s="0"/>
+      <c r="ACB4" s="0"/>
+      <c r="ACC4" s="0"/>
+      <c r="ACD4" s="0"/>
+      <c r="ACE4" s="0"/>
+      <c r="ACF4" s="0"/>
+      <c r="ACG4" s="0"/>
+      <c r="ACH4" s="0"/>
+      <c r="ACI4" s="0"/>
+      <c r="ACJ4" s="0"/>
+      <c r="ACK4" s="0"/>
+      <c r="ACL4" s="0"/>
+      <c r="ACM4" s="0"/>
+      <c r="ACN4" s="0"/>
+      <c r="ACO4" s="0"/>
+      <c r="ACP4" s="0"/>
+      <c r="ACQ4" s="0"/>
+      <c r="ACR4" s="0"/>
+      <c r="ACS4" s="0"/>
+      <c r="ACT4" s="0"/>
+      <c r="ACU4" s="0"/>
+      <c r="ACV4" s="0"/>
+      <c r="ACW4" s="0"/>
+      <c r="ACX4" s="0"/>
+      <c r="ACY4" s="0"/>
+      <c r="ACZ4" s="0"/>
+      <c r="ADA4" s="0"/>
+      <c r="ADB4" s="0"/>
+      <c r="ADC4" s="0"/>
+      <c r="ADD4" s="0"/>
+      <c r="ADE4" s="0"/>
+      <c r="ADF4" s="0"/>
+      <c r="ADG4" s="0"/>
+      <c r="ADH4" s="0"/>
+      <c r="ADI4" s="0"/>
+      <c r="ADJ4" s="0"/>
+      <c r="ADK4" s="0"/>
+      <c r="ADL4" s="0"/>
+      <c r="ADM4" s="0"/>
+      <c r="ADN4" s="0"/>
+      <c r="ADO4" s="0"/>
+      <c r="ADP4" s="0"/>
+      <c r="ADQ4" s="0"/>
+      <c r="ADR4" s="0"/>
+      <c r="ADS4" s="0"/>
+      <c r="ADT4" s="0"/>
+      <c r="ADU4" s="0"/>
+      <c r="ADV4" s="0"/>
+      <c r="ADW4" s="0"/>
+      <c r="ADX4" s="0"/>
+      <c r="ADY4" s="0"/>
+      <c r="ADZ4" s="0"/>
+      <c r="AEA4" s="0"/>
+      <c r="AEB4" s="0"/>
+      <c r="AEC4" s="0"/>
+      <c r="AED4" s="0"/>
+      <c r="AEE4" s="0"/>
+      <c r="AEF4" s="0"/>
+      <c r="AEG4" s="0"/>
+      <c r="AEH4" s="0"/>
+      <c r="AEI4" s="0"/>
+      <c r="AEJ4" s="0"/>
+      <c r="AEK4" s="0"/>
+      <c r="AEL4" s="0"/>
+      <c r="AEM4" s="0"/>
+      <c r="AEN4" s="0"/>
+      <c r="AEO4" s="0"/>
+      <c r="AEP4" s="0"/>
+      <c r="AEQ4" s="0"/>
+      <c r="AER4" s="0"/>
+      <c r="AES4" s="0"/>
+      <c r="AET4" s="0"/>
+      <c r="AEU4" s="0"/>
+      <c r="AEV4" s="0"/>
+      <c r="AEW4" s="0"/>
+      <c r="AEX4" s="0"/>
+      <c r="AEY4" s="0"/>
+      <c r="AEZ4" s="0"/>
+      <c r="AFA4" s="0"/>
+      <c r="AFB4" s="0"/>
+      <c r="AFC4" s="0"/>
+      <c r="AFD4" s="0"/>
+      <c r="AFE4" s="0"/>
+      <c r="AFF4" s="0"/>
+      <c r="AFG4" s="0"/>
+      <c r="AFH4" s="0"/>
+      <c r="AFI4" s="0"/>
+      <c r="AFJ4" s="0"/>
+      <c r="AFK4" s="0"/>
+      <c r="AFL4" s="0"/>
+      <c r="AFM4" s="0"/>
+      <c r="AFN4" s="0"/>
+      <c r="AFO4" s="0"/>
+      <c r="AFP4" s="0"/>
+      <c r="AFQ4" s="0"/>
+      <c r="AFR4" s="0"/>
+      <c r="AFS4" s="0"/>
+      <c r="AFT4" s="0"/>
+      <c r="AFU4" s="0"/>
+      <c r="AFV4" s="0"/>
+      <c r="AFW4" s="0"/>
+      <c r="AFX4" s="0"/>
+      <c r="AFY4" s="0"/>
+      <c r="AFZ4" s="0"/>
+      <c r="AGA4" s="0"/>
+      <c r="AGB4" s="0"/>
+      <c r="AGC4" s="0"/>
+      <c r="AGD4" s="0"/>
+      <c r="AGE4" s="0"/>
+      <c r="AGF4" s="0"/>
+      <c r="AGG4" s="0"/>
+      <c r="AGH4" s="0"/>
+      <c r="AGI4" s="0"/>
+      <c r="AGJ4" s="0"/>
+      <c r="AGK4" s="0"/>
+      <c r="AGL4" s="0"/>
+      <c r="AGM4" s="0"/>
+      <c r="AGN4" s="0"/>
+      <c r="AGO4" s="0"/>
+      <c r="AGP4" s="0"/>
+      <c r="AGQ4" s="0"/>
+      <c r="AGR4" s="0"/>
+      <c r="AGS4" s="0"/>
+      <c r="AGT4" s="0"/>
+      <c r="AGU4" s="0"/>
+      <c r="AGV4" s="0"/>
+      <c r="AGW4" s="0"/>
+      <c r="AGX4" s="0"/>
+      <c r="AGY4" s="0"/>
+      <c r="AGZ4" s="0"/>
+      <c r="AHA4" s="0"/>
+      <c r="AHB4" s="0"/>
+      <c r="AHC4" s="0"/>
+      <c r="AHD4" s="0"/>
+      <c r="AHE4" s="0"/>
+      <c r="AHF4" s="0"/>
+      <c r="AHG4" s="0"/>
+      <c r="AHH4" s="0"/>
+      <c r="AHI4" s="0"/>
+      <c r="AHJ4" s="0"/>
+      <c r="AHK4" s="0"/>
+      <c r="AHL4" s="0"/>
+      <c r="AHM4" s="0"/>
+      <c r="AHN4" s="0"/>
+      <c r="AHO4" s="0"/>
+      <c r="AHP4" s="0"/>
+      <c r="AHQ4" s="0"/>
+      <c r="AHR4" s="0"/>
+      <c r="AHS4" s="0"/>
+      <c r="AHT4" s="0"/>
+      <c r="AHU4" s="0"/>
+      <c r="AHV4" s="0"/>
+      <c r="AHW4" s="0"/>
+      <c r="AHX4" s="0"/>
+      <c r="AHY4" s="0"/>
+      <c r="AHZ4" s="0"/>
+      <c r="AIA4" s="0"/>
+      <c r="AIB4" s="0"/>
+      <c r="AIC4" s="0"/>
+      <c r="AID4" s="0"/>
+      <c r="AIE4" s="0"/>
+      <c r="AIF4" s="0"/>
+      <c r="AIG4" s="0"/>
+      <c r="AIH4" s="0"/>
+      <c r="AII4" s="0"/>
+      <c r="AIJ4" s="0"/>
+      <c r="AIK4" s="0"/>
+      <c r="AIL4" s="0"/>
+      <c r="AIM4" s="0"/>
+      <c r="AIN4" s="0"/>
+      <c r="AIO4" s="0"/>
+      <c r="AIP4" s="0"/>
+      <c r="AIQ4" s="0"/>
+      <c r="AIR4" s="0"/>
+      <c r="AIS4" s="0"/>
+      <c r="AIT4" s="0"/>
+      <c r="AIU4" s="0"/>
+      <c r="AIV4" s="0"/>
+      <c r="AIW4" s="0"/>
+      <c r="AIX4" s="0"/>
+      <c r="AIY4" s="0"/>
+      <c r="AIZ4" s="0"/>
+      <c r="AJA4" s="0"/>
+      <c r="AJB4" s="0"/>
+      <c r="AJC4" s="0"/>
+      <c r="AJD4" s="0"/>
+      <c r="AJE4" s="0"/>
+      <c r="AJF4" s="0"/>
+      <c r="AJG4" s="0"/>
+      <c r="AJH4" s="0"/>
+      <c r="AJI4" s="0"/>
+      <c r="AJJ4" s="0"/>
+      <c r="AJK4" s="0"/>
+      <c r="AJL4" s="0"/>
+      <c r="AJM4" s="0"/>
+      <c r="AJN4" s="0"/>
+      <c r="AJO4" s="0"/>
+      <c r="AJP4" s="0"/>
+      <c r="AJQ4" s="0"/>
+      <c r="AJR4" s="0"/>
+      <c r="AJS4" s="0"/>
+      <c r="AJT4" s="0"/>
+      <c r="AJU4" s="0"/>
+      <c r="AJV4" s="0"/>
+      <c r="AJW4" s="0"/>
+      <c r="AJX4" s="0"/>
+      <c r="AJY4" s="0"/>
+      <c r="AJZ4" s="0"/>
+      <c r="AKA4" s="0"/>
+      <c r="AKB4" s="0"/>
+      <c r="AKC4" s="0"/>
+      <c r="AKD4" s="0"/>
+      <c r="AKE4" s="0"/>
+      <c r="AKF4" s="0"/>
+      <c r="AKG4" s="0"/>
+      <c r="AKH4" s="0"/>
+      <c r="AKI4" s="0"/>
+      <c r="AKJ4" s="0"/>
+      <c r="AKK4" s="0"/>
+      <c r="AKL4" s="0"/>
+      <c r="AKM4" s="0"/>
+      <c r="AKN4" s="0"/>
+      <c r="AKO4" s="0"/>
+      <c r="AKP4" s="0"/>
+      <c r="AKQ4" s="0"/>
+      <c r="AKR4" s="0"/>
+      <c r="AKS4" s="0"/>
+      <c r="AKT4" s="0"/>
+      <c r="AKU4" s="0"/>
+      <c r="AKV4" s="0"/>
+      <c r="AKW4" s="0"/>
+      <c r="AKX4" s="0"/>
+      <c r="AKY4" s="0"/>
+      <c r="AKZ4" s="0"/>
+      <c r="ALA4" s="0"/>
+      <c r="ALB4" s="0"/>
+      <c r="ALC4" s="0"/>
+      <c r="ALD4" s="0"/>
+      <c r="ALE4" s="0"/>
+      <c r="ALF4" s="0"/>
+      <c r="ALG4" s="0"/>
+      <c r="ALH4" s="0"/>
+      <c r="ALI4" s="0"/>
+      <c r="ALJ4" s="0"/>
+      <c r="ALK4" s="0"/>
+      <c r="ALL4" s="0"/>
+      <c r="ALM4" s="0"/>
+      <c r="ALN4" s="0"/>
+      <c r="ALO4" s="0"/>
+      <c r="ALP4" s="0"/>
+      <c r="ALQ4" s="0"/>
+      <c r="ALR4" s="0"/>
+      <c r="ALS4" s="0"/>
+      <c r="ALT4" s="0"/>
+      <c r="ALU4" s="0"/>
+      <c r="ALV4" s="0"/>
+      <c r="ALW4" s="0"/>
+      <c r="ALX4" s="0"/>
+      <c r="ALY4" s="0"/>
+      <c r="ALZ4" s="0"/>
+      <c r="AMA4" s="0"/>
+      <c r="AMB4" s="0"/>
+      <c r="AMC4" s="0"/>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="49" customFormat="true" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="75" t="s">
@@ -6436,17 +9487,17 @@
   <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="E13:E14 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="79" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="79" width="30.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="79" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="79" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="79" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="79" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="79" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="79" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="79" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="79" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="79" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="79" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -11690,18 +14741,18 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="E13:E14 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="23" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="46.2753036437247"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>

<commit_message>
PROS6112 - Changed Product name 'RHINATHIOL' to capitals as in the DB
</commit_message>
<xml_diff>
--- a/Projects/BIMY/Data/Template.xlsx
+++ b/Projects/BIMY/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,23 +16,24 @@
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
@@ -1452,18 +1453,18 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.1336032388664"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.497975708502"/>
   </cols>
   <sheetData>
@@ -1730,9 +1731,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="16.3886639676113"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="23" width="0"/>
@@ -6201,7 +6202,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H9"/>
+  <autoFilter ref="A2:G9"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6227,9 +6228,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -6287,16 +6288,16 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.0242914979757"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.1012145748988"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8385,7 +8386,7 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="69" t="s">
         <v>14</v>
       </c>
@@ -9492,12 +9493,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="79" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="79" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="79" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="79" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="79" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="79" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="79" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="79" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="79" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="79" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="79" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="79" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -14746,13 +14747,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="23" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="46.5951417004049"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>

<commit_message>
PROS-7403 Sanofi Brand Block removed from all templates
</commit_message>
<xml_diff>
--- a/Projects/BIMY/Data/Template.xlsx
+++ b/Projects/BIMY/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,24 +16,25 @@
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="88">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -297,33 +298,6 @@
   </si>
   <si>
     <t xml:space="preserve">PHARMATON 2X100'S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RHINATHIOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RHINATHIOL ADULT SYRUP 125ml,
-RHINATHIOL CHILDREN SYRUP 125ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3582910009405,
-3582910010296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHARMATON 100S+30S 
-PHARMATON KIDDI SYRUP 100ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9556991220077,
-7610939003137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELFAST TABLETS 180mg 50's
-TELFAST SUSPENSION LIQUID 60ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8993237276046,
-7891058013271</t>
   </si>
   <si>
     <t xml:space="preserve">Primary_Shelftalker_Muco&amp;Rhina</t>
@@ -595,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -793,34 +767,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top/>
@@ -845,6 +791,20 @@
       <left/>
       <right style="thin"/>
       <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -892,7 +852,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="110">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1169,46 +1129,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1237,11 +1157,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="32" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="28" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1257,15 +1177,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1281,11 +1201,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="36" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="34" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1293,7 +1213,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1301,7 +1221,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1309,11 +1229,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1329,7 +1249,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1349,7 +1269,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="9" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="9" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1361,7 +1281,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1453,18 +1377,18 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.497975708502"/>
   </cols>
   <sheetData>
@@ -1731,9 +1655,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="16.3886639676113"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="23" width="0"/>
@@ -6202,7 +6126,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G9"/>
+  <autoFilter ref="A2:H9"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6228,9 +6152,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -6286,18 +6210,18 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:6"/>
+  <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.2105263157895"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7348,2126 +7272,8 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="73" t="n">
-        <v>4048846005328</v>
-      </c>
-      <c r="F3" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
-      <c r="Q3" s="0"/>
-      <c r="R3" s="0"/>
-      <c r="S3" s="0"/>
-      <c r="T3" s="0"/>
-      <c r="U3" s="0"/>
-      <c r="V3" s="0"/>
-      <c r="W3" s="0"/>
-      <c r="X3" s="0"/>
-      <c r="Y3" s="0"/>
-      <c r="Z3" s="0"/>
-      <c r="AA3" s="0"/>
-      <c r="AB3" s="0"/>
-      <c r="AC3" s="0"/>
-      <c r="AD3" s="0"/>
-      <c r="AE3" s="0"/>
-      <c r="AF3" s="0"/>
-      <c r="AG3" s="0"/>
-      <c r="AH3" s="0"/>
-      <c r="AI3" s="0"/>
-      <c r="AJ3" s="0"/>
-      <c r="AK3" s="0"/>
-      <c r="AL3" s="0"/>
-      <c r="AM3" s="0"/>
-      <c r="AN3" s="0"/>
-      <c r="AO3" s="0"/>
-      <c r="AP3" s="0"/>
-      <c r="AQ3" s="0"/>
-      <c r="AR3" s="0"/>
-      <c r="AS3" s="0"/>
-      <c r="AT3" s="0"/>
-      <c r="AU3" s="0"/>
-      <c r="AV3" s="0"/>
-      <c r="AW3" s="0"/>
-      <c r="AX3" s="0"/>
-      <c r="AY3" s="0"/>
-      <c r="AZ3" s="0"/>
-      <c r="BA3" s="0"/>
-      <c r="BB3" s="0"/>
-      <c r="BC3" s="0"/>
-      <c r="BD3" s="0"/>
-      <c r="BE3" s="0"/>
-      <c r="BF3" s="0"/>
-      <c r="BG3" s="0"/>
-      <c r="BH3" s="0"/>
-      <c r="BI3" s="0"/>
-      <c r="BJ3" s="0"/>
-      <c r="BK3" s="0"/>
-      <c r="BL3" s="0"/>
-      <c r="BM3" s="0"/>
-      <c r="BN3" s="0"/>
-      <c r="BO3" s="0"/>
-      <c r="BP3" s="0"/>
-      <c r="BQ3" s="0"/>
-      <c r="BR3" s="0"/>
-      <c r="BS3" s="0"/>
-      <c r="BT3" s="0"/>
-      <c r="BU3" s="0"/>
-      <c r="BV3" s="0"/>
-      <c r="BW3" s="0"/>
-      <c r="BX3" s="0"/>
-      <c r="BY3" s="0"/>
-      <c r="BZ3" s="0"/>
-      <c r="CA3" s="0"/>
-      <c r="CB3" s="0"/>
-      <c r="CC3" s="0"/>
-      <c r="CD3" s="0"/>
-      <c r="CE3" s="0"/>
-      <c r="CF3" s="0"/>
-      <c r="CG3" s="0"/>
-      <c r="CH3" s="0"/>
-      <c r="CI3" s="0"/>
-      <c r="CJ3" s="0"/>
-      <c r="CK3" s="0"/>
-      <c r="CL3" s="0"/>
-      <c r="CM3" s="0"/>
-      <c r="CN3" s="0"/>
-      <c r="CO3" s="0"/>
-      <c r="CP3" s="0"/>
-      <c r="CQ3" s="0"/>
-      <c r="CR3" s="0"/>
-      <c r="CS3" s="0"/>
-      <c r="CT3" s="0"/>
-      <c r="CU3" s="0"/>
-      <c r="CV3" s="0"/>
-      <c r="CW3" s="0"/>
-      <c r="CX3" s="0"/>
-      <c r="CY3" s="0"/>
-      <c r="CZ3" s="0"/>
-      <c r="DA3" s="0"/>
-      <c r="DB3" s="0"/>
-      <c r="DC3" s="0"/>
-      <c r="DD3" s="0"/>
-      <c r="DE3" s="0"/>
-      <c r="DF3" s="0"/>
-      <c r="DG3" s="0"/>
-      <c r="DH3" s="0"/>
-      <c r="DI3" s="0"/>
-      <c r="DJ3" s="0"/>
-      <c r="DK3" s="0"/>
-      <c r="DL3" s="0"/>
-      <c r="DM3" s="0"/>
-      <c r="DN3" s="0"/>
-      <c r="DO3" s="0"/>
-      <c r="DP3" s="0"/>
-      <c r="DQ3" s="0"/>
-      <c r="DR3" s="0"/>
-      <c r="DS3" s="0"/>
-      <c r="DT3" s="0"/>
-      <c r="DU3" s="0"/>
-      <c r="DV3" s="0"/>
-      <c r="DW3" s="0"/>
-      <c r="DX3" s="0"/>
-      <c r="DY3" s="0"/>
-      <c r="DZ3" s="0"/>
-      <c r="EA3" s="0"/>
-      <c r="EB3" s="0"/>
-      <c r="EC3" s="0"/>
-      <c r="ED3" s="0"/>
-      <c r="EE3" s="0"/>
-      <c r="EF3" s="0"/>
-      <c r="EG3" s="0"/>
-      <c r="EH3" s="0"/>
-      <c r="EI3" s="0"/>
-      <c r="EJ3" s="0"/>
-      <c r="EK3" s="0"/>
-      <c r="EL3" s="0"/>
-      <c r="EM3" s="0"/>
-      <c r="EN3" s="0"/>
-      <c r="EO3" s="0"/>
-      <c r="EP3" s="0"/>
-      <c r="EQ3" s="0"/>
-      <c r="ER3" s="0"/>
-      <c r="ES3" s="0"/>
-      <c r="ET3" s="0"/>
-      <c r="EU3" s="0"/>
-      <c r="EV3" s="0"/>
-      <c r="EW3" s="0"/>
-      <c r="EX3" s="0"/>
-      <c r="EY3" s="0"/>
-      <c r="EZ3" s="0"/>
-      <c r="FA3" s="0"/>
-      <c r="FB3" s="0"/>
-      <c r="FC3" s="0"/>
-      <c r="FD3" s="0"/>
-      <c r="FE3" s="0"/>
-      <c r="FF3" s="0"/>
-      <c r="FG3" s="0"/>
-      <c r="FH3" s="0"/>
-      <c r="FI3" s="0"/>
-      <c r="FJ3" s="0"/>
-      <c r="FK3" s="0"/>
-      <c r="FL3" s="0"/>
-      <c r="FM3" s="0"/>
-      <c r="FN3" s="0"/>
-      <c r="FO3" s="0"/>
-      <c r="FP3" s="0"/>
-      <c r="FQ3" s="0"/>
-      <c r="FR3" s="0"/>
-      <c r="FS3" s="0"/>
-      <c r="FT3" s="0"/>
-      <c r="FU3" s="0"/>
-      <c r="FV3" s="0"/>
-      <c r="FW3" s="0"/>
-      <c r="FX3" s="0"/>
-      <c r="FY3" s="0"/>
-      <c r="FZ3" s="0"/>
-      <c r="GA3" s="0"/>
-      <c r="GB3" s="0"/>
-      <c r="GC3" s="0"/>
-      <c r="GD3" s="0"/>
-      <c r="GE3" s="0"/>
-      <c r="GF3" s="0"/>
-      <c r="GG3" s="0"/>
-      <c r="GH3" s="0"/>
-      <c r="GI3" s="0"/>
-      <c r="GJ3" s="0"/>
-      <c r="GK3" s="0"/>
-      <c r="GL3" s="0"/>
-      <c r="GM3" s="0"/>
-      <c r="GN3" s="0"/>
-      <c r="GO3" s="0"/>
-      <c r="GP3" s="0"/>
-      <c r="GQ3" s="0"/>
-      <c r="GR3" s="0"/>
-      <c r="GS3" s="0"/>
-      <c r="GT3" s="0"/>
-      <c r="GU3" s="0"/>
-      <c r="GV3" s="0"/>
-      <c r="GW3" s="0"/>
-      <c r="GX3" s="0"/>
-      <c r="GY3" s="0"/>
-      <c r="GZ3" s="0"/>
-      <c r="HA3" s="0"/>
-      <c r="HB3" s="0"/>
-      <c r="HC3" s="0"/>
-      <c r="HD3" s="0"/>
-      <c r="HE3" s="0"/>
-      <c r="HF3" s="0"/>
-      <c r="HG3" s="0"/>
-      <c r="HH3" s="0"/>
-      <c r="HI3" s="0"/>
-      <c r="HJ3" s="0"/>
-      <c r="HK3" s="0"/>
-      <c r="HL3" s="0"/>
-      <c r="HM3" s="0"/>
-      <c r="HN3" s="0"/>
-      <c r="HO3" s="0"/>
-      <c r="HP3" s="0"/>
-      <c r="HQ3" s="0"/>
-      <c r="HR3" s="0"/>
-      <c r="HS3" s="0"/>
-      <c r="HT3" s="0"/>
-      <c r="HU3" s="0"/>
-      <c r="HV3" s="0"/>
-      <c r="HW3" s="0"/>
-      <c r="HX3" s="0"/>
-      <c r="HY3" s="0"/>
-      <c r="HZ3" s="0"/>
-      <c r="IA3" s="0"/>
-      <c r="IB3" s="0"/>
-      <c r="IC3" s="0"/>
-      <c r="ID3" s="0"/>
-      <c r="IE3" s="0"/>
-      <c r="IF3" s="0"/>
-      <c r="IG3" s="0"/>
-      <c r="IH3" s="0"/>
-      <c r="II3" s="0"/>
-      <c r="IJ3" s="0"/>
-      <c r="IK3" s="0"/>
-      <c r="IL3" s="0"/>
-      <c r="IM3" s="0"/>
-      <c r="IN3" s="0"/>
-      <c r="IO3" s="0"/>
-      <c r="IP3" s="0"/>
-      <c r="IQ3" s="0"/>
-      <c r="IR3" s="0"/>
-      <c r="IS3" s="0"/>
-      <c r="IT3" s="0"/>
-      <c r="IU3" s="0"/>
-      <c r="IV3" s="0"/>
-      <c r="IW3" s="0"/>
-      <c r="IX3" s="0"/>
-      <c r="IY3" s="0"/>
-      <c r="IZ3" s="0"/>
-      <c r="JA3" s="0"/>
-      <c r="JB3" s="0"/>
-      <c r="JC3" s="0"/>
-      <c r="JD3" s="0"/>
-      <c r="JE3" s="0"/>
-      <c r="JF3" s="0"/>
-      <c r="JG3" s="0"/>
-      <c r="JH3" s="0"/>
-      <c r="JI3" s="0"/>
-      <c r="JJ3" s="0"/>
-      <c r="JK3" s="0"/>
-      <c r="JL3" s="0"/>
-      <c r="JM3" s="0"/>
-      <c r="JN3" s="0"/>
-      <c r="JO3" s="0"/>
-      <c r="JP3" s="0"/>
-      <c r="JQ3" s="0"/>
-      <c r="JR3" s="0"/>
-      <c r="JS3" s="0"/>
-      <c r="JT3" s="0"/>
-      <c r="JU3" s="0"/>
-      <c r="JV3" s="0"/>
-      <c r="JW3" s="0"/>
-      <c r="JX3" s="0"/>
-      <c r="JY3" s="0"/>
-      <c r="JZ3" s="0"/>
-      <c r="KA3" s="0"/>
-      <c r="KB3" s="0"/>
-      <c r="KC3" s="0"/>
-      <c r="KD3" s="0"/>
-      <c r="KE3" s="0"/>
-      <c r="KF3" s="0"/>
-      <c r="KG3" s="0"/>
-      <c r="KH3" s="0"/>
-      <c r="KI3" s="0"/>
-      <c r="KJ3" s="0"/>
-      <c r="KK3" s="0"/>
-      <c r="KL3" s="0"/>
-      <c r="KM3" s="0"/>
-      <c r="KN3" s="0"/>
-      <c r="KO3" s="0"/>
-      <c r="KP3" s="0"/>
-      <c r="KQ3" s="0"/>
-      <c r="KR3" s="0"/>
-      <c r="KS3" s="0"/>
-      <c r="KT3" s="0"/>
-      <c r="KU3" s="0"/>
-      <c r="KV3" s="0"/>
-      <c r="KW3" s="0"/>
-      <c r="KX3" s="0"/>
-      <c r="KY3" s="0"/>
-      <c r="KZ3" s="0"/>
-      <c r="LA3" s="0"/>
-      <c r="LB3" s="0"/>
-      <c r="LC3" s="0"/>
-      <c r="LD3" s="0"/>
-      <c r="LE3" s="0"/>
-      <c r="LF3" s="0"/>
-      <c r="LG3" s="0"/>
-      <c r="LH3" s="0"/>
-      <c r="LI3" s="0"/>
-      <c r="LJ3" s="0"/>
-      <c r="LK3" s="0"/>
-      <c r="LL3" s="0"/>
-      <c r="LM3" s="0"/>
-      <c r="LN3" s="0"/>
-      <c r="LO3" s="0"/>
-      <c r="LP3" s="0"/>
-      <c r="LQ3" s="0"/>
-      <c r="LR3" s="0"/>
-      <c r="LS3" s="0"/>
-      <c r="LT3" s="0"/>
-      <c r="LU3" s="0"/>
-      <c r="LV3" s="0"/>
-      <c r="LW3" s="0"/>
-      <c r="LX3" s="0"/>
-      <c r="LY3" s="0"/>
-      <c r="LZ3" s="0"/>
-      <c r="MA3" s="0"/>
-      <c r="MB3" s="0"/>
-      <c r="MC3" s="0"/>
-      <c r="MD3" s="0"/>
-      <c r="ME3" s="0"/>
-      <c r="MF3" s="0"/>
-      <c r="MG3" s="0"/>
-      <c r="MH3" s="0"/>
-      <c r="MI3" s="0"/>
-      <c r="MJ3" s="0"/>
-      <c r="MK3" s="0"/>
-      <c r="ML3" s="0"/>
-      <c r="MM3" s="0"/>
-      <c r="MN3" s="0"/>
-      <c r="MO3" s="0"/>
-      <c r="MP3" s="0"/>
-      <c r="MQ3" s="0"/>
-      <c r="MR3" s="0"/>
-      <c r="MS3" s="0"/>
-      <c r="MT3" s="0"/>
-      <c r="MU3" s="0"/>
-      <c r="MV3" s="0"/>
-      <c r="MW3" s="0"/>
-      <c r="MX3" s="0"/>
-      <c r="MY3" s="0"/>
-      <c r="MZ3" s="0"/>
-      <c r="NA3" s="0"/>
-      <c r="NB3" s="0"/>
-      <c r="NC3" s="0"/>
-      <c r="ND3" s="0"/>
-      <c r="NE3" s="0"/>
-      <c r="NF3" s="0"/>
-      <c r="NG3" s="0"/>
-      <c r="NH3" s="0"/>
-      <c r="NI3" s="0"/>
-      <c r="NJ3" s="0"/>
-      <c r="NK3" s="0"/>
-      <c r="NL3" s="0"/>
-      <c r="NM3" s="0"/>
-      <c r="NN3" s="0"/>
-      <c r="NO3" s="0"/>
-      <c r="NP3" s="0"/>
-      <c r="NQ3" s="0"/>
-      <c r="NR3" s="0"/>
-      <c r="NS3" s="0"/>
-      <c r="NT3" s="0"/>
-      <c r="NU3" s="0"/>
-      <c r="NV3" s="0"/>
-      <c r="NW3" s="0"/>
-      <c r="NX3" s="0"/>
-      <c r="NY3" s="0"/>
-      <c r="NZ3" s="0"/>
-      <c r="OA3" s="0"/>
-      <c r="OB3" s="0"/>
-      <c r="OC3" s="0"/>
-      <c r="OD3" s="0"/>
-      <c r="OE3" s="0"/>
-      <c r="OF3" s="0"/>
-      <c r="OG3" s="0"/>
-      <c r="OH3" s="0"/>
-      <c r="OI3" s="0"/>
-      <c r="OJ3" s="0"/>
-      <c r="OK3" s="0"/>
-      <c r="OL3" s="0"/>
-      <c r="OM3" s="0"/>
-      <c r="ON3" s="0"/>
-      <c r="OO3" s="0"/>
-      <c r="OP3" s="0"/>
-      <c r="OQ3" s="0"/>
-      <c r="OR3" s="0"/>
-      <c r="OS3" s="0"/>
-      <c r="OT3" s="0"/>
-      <c r="OU3" s="0"/>
-      <c r="OV3" s="0"/>
-      <c r="OW3" s="0"/>
-      <c r="OX3" s="0"/>
-      <c r="OY3" s="0"/>
-      <c r="OZ3" s="0"/>
-      <c r="PA3" s="0"/>
-      <c r="PB3" s="0"/>
-      <c r="PC3" s="0"/>
-      <c r="PD3" s="0"/>
-      <c r="PE3" s="0"/>
-      <c r="PF3" s="0"/>
-      <c r="PG3" s="0"/>
-      <c r="PH3" s="0"/>
-      <c r="PI3" s="0"/>
-      <c r="PJ3" s="0"/>
-      <c r="PK3" s="0"/>
-      <c r="PL3" s="0"/>
-      <c r="PM3" s="0"/>
-      <c r="PN3" s="0"/>
-      <c r="PO3" s="0"/>
-      <c r="PP3" s="0"/>
-      <c r="PQ3" s="0"/>
-      <c r="PR3" s="0"/>
-      <c r="PS3" s="0"/>
-      <c r="PT3" s="0"/>
-      <c r="PU3" s="0"/>
-      <c r="PV3" s="0"/>
-      <c r="PW3" s="0"/>
-      <c r="PX3" s="0"/>
-      <c r="PY3" s="0"/>
-      <c r="PZ3" s="0"/>
-      <c r="QA3" s="0"/>
-      <c r="QB3" s="0"/>
-      <c r="QC3" s="0"/>
-      <c r="QD3" s="0"/>
-      <c r="QE3" s="0"/>
-      <c r="QF3" s="0"/>
-      <c r="QG3" s="0"/>
-      <c r="QH3" s="0"/>
-      <c r="QI3" s="0"/>
-      <c r="QJ3" s="0"/>
-      <c r="QK3" s="0"/>
-      <c r="QL3" s="0"/>
-      <c r="QM3" s="0"/>
-      <c r="QN3" s="0"/>
-      <c r="QO3" s="0"/>
-      <c r="QP3" s="0"/>
-      <c r="QQ3" s="0"/>
-      <c r="QR3" s="0"/>
-      <c r="QS3" s="0"/>
-      <c r="QT3" s="0"/>
-      <c r="QU3" s="0"/>
-      <c r="QV3" s="0"/>
-      <c r="QW3" s="0"/>
-      <c r="QX3" s="0"/>
-      <c r="QY3" s="0"/>
-      <c r="QZ3" s="0"/>
-      <c r="RA3" s="0"/>
-      <c r="RB3" s="0"/>
-      <c r="RC3" s="0"/>
-      <c r="RD3" s="0"/>
-      <c r="RE3" s="0"/>
-      <c r="RF3" s="0"/>
-      <c r="RG3" s="0"/>
-      <c r="RH3" s="0"/>
-      <c r="RI3" s="0"/>
-      <c r="RJ3" s="0"/>
-      <c r="RK3" s="0"/>
-      <c r="RL3" s="0"/>
-      <c r="RM3" s="0"/>
-      <c r="RN3" s="0"/>
-      <c r="RO3" s="0"/>
-      <c r="RP3" s="0"/>
-      <c r="RQ3" s="0"/>
-      <c r="RR3" s="0"/>
-      <c r="RS3" s="0"/>
-      <c r="RT3" s="0"/>
-      <c r="RU3" s="0"/>
-      <c r="RV3" s="0"/>
-      <c r="RW3" s="0"/>
-      <c r="RX3" s="0"/>
-      <c r="RY3" s="0"/>
-      <c r="RZ3" s="0"/>
-      <c r="SA3" s="0"/>
-      <c r="SB3" s="0"/>
-      <c r="SC3" s="0"/>
-      <c r="SD3" s="0"/>
-      <c r="SE3" s="0"/>
-      <c r="SF3" s="0"/>
-      <c r="SG3" s="0"/>
-      <c r="SH3" s="0"/>
-      <c r="SI3" s="0"/>
-      <c r="SJ3" s="0"/>
-      <c r="SK3" s="0"/>
-      <c r="SL3" s="0"/>
-      <c r="SM3" s="0"/>
-      <c r="SN3" s="0"/>
-      <c r="SO3" s="0"/>
-      <c r="SP3" s="0"/>
-      <c r="SQ3" s="0"/>
-      <c r="SR3" s="0"/>
-      <c r="SS3" s="0"/>
-      <c r="ST3" s="0"/>
-      <c r="SU3" s="0"/>
-      <c r="SV3" s="0"/>
-      <c r="SW3" s="0"/>
-      <c r="SX3" s="0"/>
-      <c r="SY3" s="0"/>
-      <c r="SZ3" s="0"/>
-      <c r="TA3" s="0"/>
-      <c r="TB3" s="0"/>
-      <c r="TC3" s="0"/>
-      <c r="TD3" s="0"/>
-      <c r="TE3" s="0"/>
-      <c r="TF3" s="0"/>
-      <c r="TG3" s="0"/>
-      <c r="TH3" s="0"/>
-      <c r="TI3" s="0"/>
-      <c r="TJ3" s="0"/>
-      <c r="TK3" s="0"/>
-      <c r="TL3" s="0"/>
-      <c r="TM3" s="0"/>
-      <c r="TN3" s="0"/>
-      <c r="TO3" s="0"/>
-      <c r="TP3" s="0"/>
-      <c r="TQ3" s="0"/>
-      <c r="TR3" s="0"/>
-      <c r="TS3" s="0"/>
-      <c r="TT3" s="0"/>
-      <c r="TU3" s="0"/>
-      <c r="TV3" s="0"/>
-      <c r="TW3" s="0"/>
-      <c r="TX3" s="0"/>
-      <c r="TY3" s="0"/>
-      <c r="TZ3" s="0"/>
-      <c r="UA3" s="0"/>
-      <c r="UB3" s="0"/>
-      <c r="UC3" s="0"/>
-      <c r="UD3" s="0"/>
-      <c r="UE3" s="0"/>
-      <c r="UF3" s="0"/>
-      <c r="UG3" s="0"/>
-      <c r="UH3" s="0"/>
-      <c r="UI3" s="0"/>
-      <c r="UJ3" s="0"/>
-      <c r="UK3" s="0"/>
-      <c r="UL3" s="0"/>
-      <c r="UM3" s="0"/>
-      <c r="UN3" s="0"/>
-      <c r="UO3" s="0"/>
-      <c r="UP3" s="0"/>
-      <c r="UQ3" s="0"/>
-      <c r="UR3" s="0"/>
-      <c r="US3" s="0"/>
-      <c r="UT3" s="0"/>
-      <c r="UU3" s="0"/>
-      <c r="UV3" s="0"/>
-      <c r="UW3" s="0"/>
-      <c r="UX3" s="0"/>
-      <c r="UY3" s="0"/>
-      <c r="UZ3" s="0"/>
-      <c r="VA3" s="0"/>
-      <c r="VB3" s="0"/>
-      <c r="VC3" s="0"/>
-      <c r="VD3" s="0"/>
-      <c r="VE3" s="0"/>
-      <c r="VF3" s="0"/>
-      <c r="VG3" s="0"/>
-      <c r="VH3" s="0"/>
-      <c r="VI3" s="0"/>
-      <c r="VJ3" s="0"/>
-      <c r="VK3" s="0"/>
-      <c r="VL3" s="0"/>
-      <c r="VM3" s="0"/>
-      <c r="VN3" s="0"/>
-      <c r="VO3" s="0"/>
-      <c r="VP3" s="0"/>
-      <c r="VQ3" s="0"/>
-      <c r="VR3" s="0"/>
-      <c r="VS3" s="0"/>
-      <c r="VT3" s="0"/>
-      <c r="VU3" s="0"/>
-      <c r="VV3" s="0"/>
-      <c r="VW3" s="0"/>
-      <c r="VX3" s="0"/>
-      <c r="VY3" s="0"/>
-      <c r="VZ3" s="0"/>
-      <c r="WA3" s="0"/>
-      <c r="WB3" s="0"/>
-      <c r="WC3" s="0"/>
-      <c r="WD3" s="0"/>
-      <c r="WE3" s="0"/>
-      <c r="WF3" s="0"/>
-      <c r="WG3" s="0"/>
-      <c r="WH3" s="0"/>
-      <c r="WI3" s="0"/>
-      <c r="WJ3" s="0"/>
-      <c r="WK3" s="0"/>
-      <c r="WL3" s="0"/>
-      <c r="WM3" s="0"/>
-      <c r="WN3" s="0"/>
-      <c r="WO3" s="0"/>
-      <c r="WP3" s="0"/>
-      <c r="WQ3" s="0"/>
-      <c r="WR3" s="0"/>
-      <c r="WS3" s="0"/>
-      <c r="WT3" s="0"/>
-      <c r="WU3" s="0"/>
-      <c r="WV3" s="0"/>
-      <c r="WW3" s="0"/>
-      <c r="WX3" s="0"/>
-      <c r="WY3" s="0"/>
-      <c r="WZ3" s="0"/>
-      <c r="XA3" s="0"/>
-      <c r="XB3" s="0"/>
-      <c r="XC3" s="0"/>
-      <c r="XD3" s="0"/>
-      <c r="XE3" s="0"/>
-      <c r="XF3" s="0"/>
-      <c r="XG3" s="0"/>
-      <c r="XH3" s="0"/>
-      <c r="XI3" s="0"/>
-      <c r="XJ3" s="0"/>
-      <c r="XK3" s="0"/>
-      <c r="XL3" s="0"/>
-      <c r="XM3" s="0"/>
-      <c r="XN3" s="0"/>
-      <c r="XO3" s="0"/>
-      <c r="XP3" s="0"/>
-      <c r="XQ3" s="0"/>
-      <c r="XR3" s="0"/>
-      <c r="XS3" s="0"/>
-      <c r="XT3" s="0"/>
-      <c r="XU3" s="0"/>
-      <c r="XV3" s="0"/>
-      <c r="XW3" s="0"/>
-      <c r="XX3" s="0"/>
-      <c r="XY3" s="0"/>
-      <c r="XZ3" s="0"/>
-      <c r="YA3" s="0"/>
-      <c r="YB3" s="0"/>
-      <c r="YC3" s="0"/>
-      <c r="YD3" s="0"/>
-      <c r="YE3" s="0"/>
-      <c r="YF3" s="0"/>
-      <c r="YG3" s="0"/>
-      <c r="YH3" s="0"/>
-      <c r="YI3" s="0"/>
-      <c r="YJ3" s="0"/>
-      <c r="YK3" s="0"/>
-      <c r="YL3" s="0"/>
-      <c r="YM3" s="0"/>
-      <c r="YN3" s="0"/>
-      <c r="YO3" s="0"/>
-      <c r="YP3" s="0"/>
-      <c r="YQ3" s="0"/>
-      <c r="YR3" s="0"/>
-      <c r="YS3" s="0"/>
-      <c r="YT3" s="0"/>
-      <c r="YU3" s="0"/>
-      <c r="YV3" s="0"/>
-      <c r="YW3" s="0"/>
-      <c r="YX3" s="0"/>
-      <c r="YY3" s="0"/>
-      <c r="YZ3" s="0"/>
-      <c r="ZA3" s="0"/>
-      <c r="ZB3" s="0"/>
-      <c r="ZC3" s="0"/>
-      <c r="ZD3" s="0"/>
-      <c r="ZE3" s="0"/>
-      <c r="ZF3" s="0"/>
-      <c r="ZG3" s="0"/>
-      <c r="ZH3" s="0"/>
-      <c r="ZI3" s="0"/>
-      <c r="ZJ3" s="0"/>
-      <c r="ZK3" s="0"/>
-      <c r="ZL3" s="0"/>
-      <c r="ZM3" s="0"/>
-      <c r="ZN3" s="0"/>
-      <c r="ZO3" s="0"/>
-      <c r="ZP3" s="0"/>
-      <c r="ZQ3" s="0"/>
-      <c r="ZR3" s="0"/>
-      <c r="ZS3" s="0"/>
-      <c r="ZT3" s="0"/>
-      <c r="ZU3" s="0"/>
-      <c r="ZV3" s="0"/>
-      <c r="ZW3" s="0"/>
-      <c r="ZX3" s="0"/>
-      <c r="ZY3" s="0"/>
-      <c r="ZZ3" s="0"/>
-      <c r="AAA3" s="0"/>
-      <c r="AAB3" s="0"/>
-      <c r="AAC3" s="0"/>
-      <c r="AAD3" s="0"/>
-      <c r="AAE3" s="0"/>
-      <c r="AAF3" s="0"/>
-      <c r="AAG3" s="0"/>
-      <c r="AAH3" s="0"/>
-      <c r="AAI3" s="0"/>
-      <c r="AAJ3" s="0"/>
-      <c r="AAK3" s="0"/>
-      <c r="AAL3" s="0"/>
-      <c r="AAM3" s="0"/>
-      <c r="AAN3" s="0"/>
-      <c r="AAO3" s="0"/>
-      <c r="AAP3" s="0"/>
-      <c r="AAQ3" s="0"/>
-      <c r="AAR3" s="0"/>
-      <c r="AAS3" s="0"/>
-      <c r="AAT3" s="0"/>
-      <c r="AAU3" s="0"/>
-      <c r="AAV3" s="0"/>
-      <c r="AAW3" s="0"/>
-      <c r="AAX3" s="0"/>
-      <c r="AAY3" s="0"/>
-      <c r="AAZ3" s="0"/>
-      <c r="ABA3" s="0"/>
-      <c r="ABB3" s="0"/>
-      <c r="ABC3" s="0"/>
-      <c r="ABD3" s="0"/>
-      <c r="ABE3" s="0"/>
-      <c r="ABF3" s="0"/>
-      <c r="ABG3" s="0"/>
-      <c r="ABH3" s="0"/>
-      <c r="ABI3" s="0"/>
-      <c r="ABJ3" s="0"/>
-      <c r="ABK3" s="0"/>
-      <c r="ABL3" s="0"/>
-      <c r="ABM3" s="0"/>
-      <c r="ABN3" s="0"/>
-      <c r="ABO3" s="0"/>
-      <c r="ABP3" s="0"/>
-      <c r="ABQ3" s="0"/>
-      <c r="ABR3" s="0"/>
-      <c r="ABS3" s="0"/>
-      <c r="ABT3" s="0"/>
-      <c r="ABU3" s="0"/>
-      <c r="ABV3" s="0"/>
-      <c r="ABW3" s="0"/>
-      <c r="ABX3" s="0"/>
-      <c r="ABY3" s="0"/>
-      <c r="ABZ3" s="0"/>
-      <c r="ACA3" s="0"/>
-      <c r="ACB3" s="0"/>
-      <c r="ACC3" s="0"/>
-      <c r="ACD3" s="0"/>
-      <c r="ACE3" s="0"/>
-      <c r="ACF3" s="0"/>
-      <c r="ACG3" s="0"/>
-      <c r="ACH3" s="0"/>
-      <c r="ACI3" s="0"/>
-      <c r="ACJ3" s="0"/>
-      <c r="ACK3" s="0"/>
-      <c r="ACL3" s="0"/>
-      <c r="ACM3" s="0"/>
-      <c r="ACN3" s="0"/>
-      <c r="ACO3" s="0"/>
-      <c r="ACP3" s="0"/>
-      <c r="ACQ3" s="0"/>
-      <c r="ACR3" s="0"/>
-      <c r="ACS3" s="0"/>
-      <c r="ACT3" s="0"/>
-      <c r="ACU3" s="0"/>
-      <c r="ACV3" s="0"/>
-      <c r="ACW3" s="0"/>
-      <c r="ACX3" s="0"/>
-      <c r="ACY3" s="0"/>
-      <c r="ACZ3" s="0"/>
-      <c r="ADA3" s="0"/>
-      <c r="ADB3" s="0"/>
-      <c r="ADC3" s="0"/>
-      <c r="ADD3" s="0"/>
-      <c r="ADE3" s="0"/>
-      <c r="ADF3" s="0"/>
-      <c r="ADG3" s="0"/>
-      <c r="ADH3" s="0"/>
-      <c r="ADI3" s="0"/>
-      <c r="ADJ3" s="0"/>
-      <c r="ADK3" s="0"/>
-      <c r="ADL3" s="0"/>
-      <c r="ADM3" s="0"/>
-      <c r="ADN3" s="0"/>
-      <c r="ADO3" s="0"/>
-      <c r="ADP3" s="0"/>
-      <c r="ADQ3" s="0"/>
-      <c r="ADR3" s="0"/>
-      <c r="ADS3" s="0"/>
-      <c r="ADT3" s="0"/>
-      <c r="ADU3" s="0"/>
-      <c r="ADV3" s="0"/>
-      <c r="ADW3" s="0"/>
-      <c r="ADX3" s="0"/>
-      <c r="ADY3" s="0"/>
-      <c r="ADZ3" s="0"/>
-      <c r="AEA3" s="0"/>
-      <c r="AEB3" s="0"/>
-      <c r="AEC3" s="0"/>
-      <c r="AED3" s="0"/>
-      <c r="AEE3" s="0"/>
-      <c r="AEF3" s="0"/>
-      <c r="AEG3" s="0"/>
-      <c r="AEH3" s="0"/>
-      <c r="AEI3" s="0"/>
-      <c r="AEJ3" s="0"/>
-      <c r="AEK3" s="0"/>
-      <c r="AEL3" s="0"/>
-      <c r="AEM3" s="0"/>
-      <c r="AEN3" s="0"/>
-      <c r="AEO3" s="0"/>
-      <c r="AEP3" s="0"/>
-      <c r="AEQ3" s="0"/>
-      <c r="AER3" s="0"/>
-      <c r="AES3" s="0"/>
-      <c r="AET3" s="0"/>
-      <c r="AEU3" s="0"/>
-      <c r="AEV3" s="0"/>
-      <c r="AEW3" s="0"/>
-      <c r="AEX3" s="0"/>
-      <c r="AEY3" s="0"/>
-      <c r="AEZ3" s="0"/>
-      <c r="AFA3" s="0"/>
-      <c r="AFB3" s="0"/>
-      <c r="AFC3" s="0"/>
-      <c r="AFD3" s="0"/>
-      <c r="AFE3" s="0"/>
-      <c r="AFF3" s="0"/>
-      <c r="AFG3" s="0"/>
-      <c r="AFH3" s="0"/>
-      <c r="AFI3" s="0"/>
-      <c r="AFJ3" s="0"/>
-      <c r="AFK3" s="0"/>
-      <c r="AFL3" s="0"/>
-      <c r="AFM3" s="0"/>
-      <c r="AFN3" s="0"/>
-      <c r="AFO3" s="0"/>
-      <c r="AFP3" s="0"/>
-      <c r="AFQ3" s="0"/>
-      <c r="AFR3" s="0"/>
-      <c r="AFS3" s="0"/>
-      <c r="AFT3" s="0"/>
-      <c r="AFU3" s="0"/>
-      <c r="AFV3" s="0"/>
-      <c r="AFW3" s="0"/>
-      <c r="AFX3" s="0"/>
-      <c r="AFY3" s="0"/>
-      <c r="AFZ3" s="0"/>
-      <c r="AGA3" s="0"/>
-      <c r="AGB3" s="0"/>
-      <c r="AGC3" s="0"/>
-      <c r="AGD3" s="0"/>
-      <c r="AGE3" s="0"/>
-      <c r="AGF3" s="0"/>
-      <c r="AGG3" s="0"/>
-      <c r="AGH3" s="0"/>
-      <c r="AGI3" s="0"/>
-      <c r="AGJ3" s="0"/>
-      <c r="AGK3" s="0"/>
-      <c r="AGL3" s="0"/>
-      <c r="AGM3" s="0"/>
-      <c r="AGN3" s="0"/>
-      <c r="AGO3" s="0"/>
-      <c r="AGP3" s="0"/>
-      <c r="AGQ3" s="0"/>
-      <c r="AGR3" s="0"/>
-      <c r="AGS3" s="0"/>
-      <c r="AGT3" s="0"/>
-      <c r="AGU3" s="0"/>
-      <c r="AGV3" s="0"/>
-      <c r="AGW3" s="0"/>
-      <c r="AGX3" s="0"/>
-      <c r="AGY3" s="0"/>
-      <c r="AGZ3" s="0"/>
-      <c r="AHA3" s="0"/>
-      <c r="AHB3" s="0"/>
-      <c r="AHC3" s="0"/>
-      <c r="AHD3" s="0"/>
-      <c r="AHE3" s="0"/>
-      <c r="AHF3" s="0"/>
-      <c r="AHG3" s="0"/>
-      <c r="AHH3" s="0"/>
-      <c r="AHI3" s="0"/>
-      <c r="AHJ3" s="0"/>
-      <c r="AHK3" s="0"/>
-      <c r="AHL3" s="0"/>
-      <c r="AHM3" s="0"/>
-      <c r="AHN3" s="0"/>
-      <c r="AHO3" s="0"/>
-      <c r="AHP3" s="0"/>
-      <c r="AHQ3" s="0"/>
-      <c r="AHR3" s="0"/>
-      <c r="AHS3" s="0"/>
-      <c r="AHT3" s="0"/>
-      <c r="AHU3" s="0"/>
-      <c r="AHV3" s="0"/>
-      <c r="AHW3" s="0"/>
-      <c r="AHX3" s="0"/>
-      <c r="AHY3" s="0"/>
-      <c r="AHZ3" s="0"/>
-      <c r="AIA3" s="0"/>
-      <c r="AIB3" s="0"/>
-      <c r="AIC3" s="0"/>
-      <c r="AID3" s="0"/>
-      <c r="AIE3" s="0"/>
-      <c r="AIF3" s="0"/>
-      <c r="AIG3" s="0"/>
-      <c r="AIH3" s="0"/>
-      <c r="AII3" s="0"/>
-      <c r="AIJ3" s="0"/>
-      <c r="AIK3" s="0"/>
-      <c r="AIL3" s="0"/>
-      <c r="AIM3" s="0"/>
-      <c r="AIN3" s="0"/>
-      <c r="AIO3" s="0"/>
-      <c r="AIP3" s="0"/>
-      <c r="AIQ3" s="0"/>
-      <c r="AIR3" s="0"/>
-      <c r="AIS3" s="0"/>
-      <c r="AIT3" s="0"/>
-      <c r="AIU3" s="0"/>
-      <c r="AIV3" s="0"/>
-      <c r="AIW3" s="0"/>
-      <c r="AIX3" s="0"/>
-      <c r="AIY3" s="0"/>
-      <c r="AIZ3" s="0"/>
-      <c r="AJA3" s="0"/>
-      <c r="AJB3" s="0"/>
-      <c r="AJC3" s="0"/>
-      <c r="AJD3" s="0"/>
-      <c r="AJE3" s="0"/>
-      <c r="AJF3" s="0"/>
-      <c r="AJG3" s="0"/>
-      <c r="AJH3" s="0"/>
-      <c r="AJI3" s="0"/>
-      <c r="AJJ3" s="0"/>
-      <c r="AJK3" s="0"/>
-      <c r="AJL3" s="0"/>
-      <c r="AJM3" s="0"/>
-      <c r="AJN3" s="0"/>
-      <c r="AJO3" s="0"/>
-      <c r="AJP3" s="0"/>
-      <c r="AJQ3" s="0"/>
-      <c r="AJR3" s="0"/>
-      <c r="AJS3" s="0"/>
-      <c r="AJT3" s="0"/>
-      <c r="AJU3" s="0"/>
-      <c r="AJV3" s="0"/>
-      <c r="AJW3" s="0"/>
-      <c r="AJX3" s="0"/>
-      <c r="AJY3" s="0"/>
-      <c r="AJZ3" s="0"/>
-      <c r="AKA3" s="0"/>
-      <c r="AKB3" s="0"/>
-      <c r="AKC3" s="0"/>
-      <c r="AKD3" s="0"/>
-      <c r="AKE3" s="0"/>
-      <c r="AKF3" s="0"/>
-      <c r="AKG3" s="0"/>
-      <c r="AKH3" s="0"/>
-      <c r="AKI3" s="0"/>
-      <c r="AKJ3" s="0"/>
-      <c r="AKK3" s="0"/>
-      <c r="AKL3" s="0"/>
-      <c r="AKM3" s="0"/>
-      <c r="AKN3" s="0"/>
-      <c r="AKO3" s="0"/>
-      <c r="AKP3" s="0"/>
-      <c r="AKQ3" s="0"/>
-      <c r="AKR3" s="0"/>
-      <c r="AKS3" s="0"/>
-      <c r="AKT3" s="0"/>
-      <c r="AKU3" s="0"/>
-      <c r="AKV3" s="0"/>
-      <c r="AKW3" s="0"/>
-      <c r="AKX3" s="0"/>
-      <c r="AKY3" s="0"/>
-      <c r="AKZ3" s="0"/>
-      <c r="ALA3" s="0"/>
-      <c r="ALB3" s="0"/>
-      <c r="ALC3" s="0"/>
-      <c r="ALD3" s="0"/>
-      <c r="ALE3" s="0"/>
-      <c r="ALF3" s="0"/>
-      <c r="ALG3" s="0"/>
-      <c r="ALH3" s="0"/>
-      <c r="ALI3" s="0"/>
-      <c r="ALJ3" s="0"/>
-      <c r="ALK3" s="0"/>
-      <c r="ALL3" s="0"/>
-      <c r="ALM3" s="0"/>
-      <c r="ALN3" s="0"/>
-      <c r="ALO3" s="0"/>
-      <c r="ALP3" s="0"/>
-      <c r="ALQ3" s="0"/>
-      <c r="ALR3" s="0"/>
-      <c r="ALS3" s="0"/>
-      <c r="ALT3" s="0"/>
-      <c r="ALU3" s="0"/>
-      <c r="ALV3" s="0"/>
-      <c r="ALW3" s="0"/>
-      <c r="ALX3" s="0"/>
-      <c r="ALY3" s="0"/>
-      <c r="ALZ3" s="0"/>
-      <c r="AMA3" s="0"/>
-      <c r="AMB3" s="0"/>
-      <c r="AMC3" s="0"/>
-      <c r="AMD3" s="0"/>
-      <c r="AME3" s="0"/>
-      <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="0"/>
-      <c r="K4" s="0"/>
-      <c r="L4" s="0"/>
-      <c r="M4" s="0"/>
-      <c r="N4" s="0"/>
-      <c r="O4" s="0"/>
-      <c r="P4" s="0"/>
-      <c r="Q4" s="0"/>
-      <c r="R4" s="0"/>
-      <c r="S4" s="0"/>
-      <c r="T4" s="0"/>
-      <c r="U4" s="0"/>
-      <c r="V4" s="0"/>
-      <c r="W4" s="0"/>
-      <c r="X4" s="0"/>
-      <c r="Y4" s="0"/>
-      <c r="Z4" s="0"/>
-      <c r="AA4" s="0"/>
-      <c r="AB4" s="0"/>
-      <c r="AC4" s="0"/>
-      <c r="AD4" s="0"/>
-      <c r="AE4" s="0"/>
-      <c r="AF4" s="0"/>
-      <c r="AG4" s="0"/>
-      <c r="AH4" s="0"/>
-      <c r="AI4" s="0"/>
-      <c r="AJ4" s="0"/>
-      <c r="AK4" s="0"/>
-      <c r="AL4" s="0"/>
-      <c r="AM4" s="0"/>
-      <c r="AN4" s="0"/>
-      <c r="AO4" s="0"/>
-      <c r="AP4" s="0"/>
-      <c r="AQ4" s="0"/>
-      <c r="AR4" s="0"/>
-      <c r="AS4" s="0"/>
-      <c r="AT4" s="0"/>
-      <c r="AU4" s="0"/>
-      <c r="AV4" s="0"/>
-      <c r="AW4" s="0"/>
-      <c r="AX4" s="0"/>
-      <c r="AY4" s="0"/>
-      <c r="AZ4" s="0"/>
-      <c r="BA4" s="0"/>
-      <c r="BB4" s="0"/>
-      <c r="BC4" s="0"/>
-      <c r="BD4" s="0"/>
-      <c r="BE4" s="0"/>
-      <c r="BF4" s="0"/>
-      <c r="BG4" s="0"/>
-      <c r="BH4" s="0"/>
-      <c r="BI4" s="0"/>
-      <c r="BJ4" s="0"/>
-      <c r="BK4" s="0"/>
-      <c r="BL4" s="0"/>
-      <c r="BM4" s="0"/>
-      <c r="BN4" s="0"/>
-      <c r="BO4" s="0"/>
-      <c r="BP4" s="0"/>
-      <c r="BQ4" s="0"/>
-      <c r="BR4" s="0"/>
-      <c r="BS4" s="0"/>
-      <c r="BT4" s="0"/>
-      <c r="BU4" s="0"/>
-      <c r="BV4" s="0"/>
-      <c r="BW4" s="0"/>
-      <c r="BX4" s="0"/>
-      <c r="BY4" s="0"/>
-      <c r="BZ4" s="0"/>
-      <c r="CA4" s="0"/>
-      <c r="CB4" s="0"/>
-      <c r="CC4" s="0"/>
-      <c r="CD4" s="0"/>
-      <c r="CE4" s="0"/>
-      <c r="CF4" s="0"/>
-      <c r="CG4" s="0"/>
-      <c r="CH4" s="0"/>
-      <c r="CI4" s="0"/>
-      <c r="CJ4" s="0"/>
-      <c r="CK4" s="0"/>
-      <c r="CL4" s="0"/>
-      <c r="CM4" s="0"/>
-      <c r="CN4" s="0"/>
-      <c r="CO4" s="0"/>
-      <c r="CP4" s="0"/>
-      <c r="CQ4" s="0"/>
-      <c r="CR4" s="0"/>
-      <c r="CS4" s="0"/>
-      <c r="CT4" s="0"/>
-      <c r="CU4" s="0"/>
-      <c r="CV4" s="0"/>
-      <c r="CW4" s="0"/>
-      <c r="CX4" s="0"/>
-      <c r="CY4" s="0"/>
-      <c r="CZ4" s="0"/>
-      <c r="DA4" s="0"/>
-      <c r="DB4" s="0"/>
-      <c r="DC4" s="0"/>
-      <c r="DD4" s="0"/>
-      <c r="DE4" s="0"/>
-      <c r="DF4" s="0"/>
-      <c r="DG4" s="0"/>
-      <c r="DH4" s="0"/>
-      <c r="DI4" s="0"/>
-      <c r="DJ4" s="0"/>
-      <c r="DK4" s="0"/>
-      <c r="DL4" s="0"/>
-      <c r="DM4" s="0"/>
-      <c r="DN4" s="0"/>
-      <c r="DO4" s="0"/>
-      <c r="DP4" s="0"/>
-      <c r="DQ4" s="0"/>
-      <c r="DR4" s="0"/>
-      <c r="DS4" s="0"/>
-      <c r="DT4" s="0"/>
-      <c r="DU4" s="0"/>
-      <c r="DV4" s="0"/>
-      <c r="DW4" s="0"/>
-      <c r="DX4" s="0"/>
-      <c r="DY4" s="0"/>
-      <c r="DZ4" s="0"/>
-      <c r="EA4" s="0"/>
-      <c r="EB4" s="0"/>
-      <c r="EC4" s="0"/>
-      <c r="ED4" s="0"/>
-      <c r="EE4" s="0"/>
-      <c r="EF4" s="0"/>
-      <c r="EG4" s="0"/>
-      <c r="EH4" s="0"/>
-      <c r="EI4" s="0"/>
-      <c r="EJ4" s="0"/>
-      <c r="EK4" s="0"/>
-      <c r="EL4" s="0"/>
-      <c r="EM4" s="0"/>
-      <c r="EN4" s="0"/>
-      <c r="EO4" s="0"/>
-      <c r="EP4" s="0"/>
-      <c r="EQ4" s="0"/>
-      <c r="ER4" s="0"/>
-      <c r="ES4" s="0"/>
-      <c r="ET4" s="0"/>
-      <c r="EU4" s="0"/>
-      <c r="EV4" s="0"/>
-      <c r="EW4" s="0"/>
-      <c r="EX4" s="0"/>
-      <c r="EY4" s="0"/>
-      <c r="EZ4" s="0"/>
-      <c r="FA4" s="0"/>
-      <c r="FB4" s="0"/>
-      <c r="FC4" s="0"/>
-      <c r="FD4" s="0"/>
-      <c r="FE4" s="0"/>
-      <c r="FF4" s="0"/>
-      <c r="FG4" s="0"/>
-      <c r="FH4" s="0"/>
-      <c r="FI4" s="0"/>
-      <c r="FJ4" s="0"/>
-      <c r="FK4" s="0"/>
-      <c r="FL4" s="0"/>
-      <c r="FM4" s="0"/>
-      <c r="FN4" s="0"/>
-      <c r="FO4" s="0"/>
-      <c r="FP4" s="0"/>
-      <c r="FQ4" s="0"/>
-      <c r="FR4" s="0"/>
-      <c r="FS4" s="0"/>
-      <c r="FT4" s="0"/>
-      <c r="FU4" s="0"/>
-      <c r="FV4" s="0"/>
-      <c r="FW4" s="0"/>
-      <c r="FX4" s="0"/>
-      <c r="FY4" s="0"/>
-      <c r="FZ4" s="0"/>
-      <c r="GA4" s="0"/>
-      <c r="GB4" s="0"/>
-      <c r="GC4" s="0"/>
-      <c r="GD4" s="0"/>
-      <c r="GE4" s="0"/>
-      <c r="GF4" s="0"/>
-      <c r="GG4" s="0"/>
-      <c r="GH4" s="0"/>
-      <c r="GI4" s="0"/>
-      <c r="GJ4" s="0"/>
-      <c r="GK4" s="0"/>
-      <c r="GL4" s="0"/>
-      <c r="GM4" s="0"/>
-      <c r="GN4" s="0"/>
-      <c r="GO4" s="0"/>
-      <c r="GP4" s="0"/>
-      <c r="GQ4" s="0"/>
-      <c r="GR4" s="0"/>
-      <c r="GS4" s="0"/>
-      <c r="GT4" s="0"/>
-      <c r="GU4" s="0"/>
-      <c r="GV4" s="0"/>
-      <c r="GW4" s="0"/>
-      <c r="GX4" s="0"/>
-      <c r="GY4" s="0"/>
-      <c r="GZ4" s="0"/>
-      <c r="HA4" s="0"/>
-      <c r="HB4" s="0"/>
-      <c r="HC4" s="0"/>
-      <c r="HD4" s="0"/>
-      <c r="HE4" s="0"/>
-      <c r="HF4" s="0"/>
-      <c r="HG4" s="0"/>
-      <c r="HH4" s="0"/>
-      <c r="HI4" s="0"/>
-      <c r="HJ4" s="0"/>
-      <c r="HK4" s="0"/>
-      <c r="HL4" s="0"/>
-      <c r="HM4" s="0"/>
-      <c r="HN4" s="0"/>
-      <c r="HO4" s="0"/>
-      <c r="HP4" s="0"/>
-      <c r="HQ4" s="0"/>
-      <c r="HR4" s="0"/>
-      <c r="HS4" s="0"/>
-      <c r="HT4" s="0"/>
-      <c r="HU4" s="0"/>
-      <c r="HV4" s="0"/>
-      <c r="HW4" s="0"/>
-      <c r="HX4" s="0"/>
-      <c r="HY4" s="0"/>
-      <c r="HZ4" s="0"/>
-      <c r="IA4" s="0"/>
-      <c r="IB4" s="0"/>
-      <c r="IC4" s="0"/>
-      <c r="ID4" s="0"/>
-      <c r="IE4" s="0"/>
-      <c r="IF4" s="0"/>
-      <c r="IG4" s="0"/>
-      <c r="IH4" s="0"/>
-      <c r="II4" s="0"/>
-      <c r="IJ4" s="0"/>
-      <c r="IK4" s="0"/>
-      <c r="IL4" s="0"/>
-      <c r="IM4" s="0"/>
-      <c r="IN4" s="0"/>
-      <c r="IO4" s="0"/>
-      <c r="IP4" s="0"/>
-      <c r="IQ4" s="0"/>
-      <c r="IR4" s="0"/>
-      <c r="IS4" s="0"/>
-      <c r="IT4" s="0"/>
-      <c r="IU4" s="0"/>
-      <c r="IV4" s="0"/>
-      <c r="IW4" s="0"/>
-      <c r="IX4" s="0"/>
-      <c r="IY4" s="0"/>
-      <c r="IZ4" s="0"/>
-      <c r="JA4" s="0"/>
-      <c r="JB4" s="0"/>
-      <c r="JC4" s="0"/>
-      <c r="JD4" s="0"/>
-      <c r="JE4" s="0"/>
-      <c r="JF4" s="0"/>
-      <c r="JG4" s="0"/>
-      <c r="JH4" s="0"/>
-      <c r="JI4" s="0"/>
-      <c r="JJ4" s="0"/>
-      <c r="JK4" s="0"/>
-      <c r="JL4" s="0"/>
-      <c r="JM4" s="0"/>
-      <c r="JN4" s="0"/>
-      <c r="JO4" s="0"/>
-      <c r="JP4" s="0"/>
-      <c r="JQ4" s="0"/>
-      <c r="JR4" s="0"/>
-      <c r="JS4" s="0"/>
-      <c r="JT4" s="0"/>
-      <c r="JU4" s="0"/>
-      <c r="JV4" s="0"/>
-      <c r="JW4" s="0"/>
-      <c r="JX4" s="0"/>
-      <c r="JY4" s="0"/>
-      <c r="JZ4" s="0"/>
-      <c r="KA4" s="0"/>
-      <c r="KB4" s="0"/>
-      <c r="KC4" s="0"/>
-      <c r="KD4" s="0"/>
-      <c r="KE4" s="0"/>
-      <c r="KF4" s="0"/>
-      <c r="KG4" s="0"/>
-      <c r="KH4" s="0"/>
-      <c r="KI4" s="0"/>
-      <c r="KJ4" s="0"/>
-      <c r="KK4" s="0"/>
-      <c r="KL4" s="0"/>
-      <c r="KM4" s="0"/>
-      <c r="KN4" s="0"/>
-      <c r="KO4" s="0"/>
-      <c r="KP4" s="0"/>
-      <c r="KQ4" s="0"/>
-      <c r="KR4" s="0"/>
-      <c r="KS4" s="0"/>
-      <c r="KT4" s="0"/>
-      <c r="KU4" s="0"/>
-      <c r="KV4" s="0"/>
-      <c r="KW4" s="0"/>
-      <c r="KX4" s="0"/>
-      <c r="KY4" s="0"/>
-      <c r="KZ4" s="0"/>
-      <c r="LA4" s="0"/>
-      <c r="LB4" s="0"/>
-      <c r="LC4" s="0"/>
-      <c r="LD4" s="0"/>
-      <c r="LE4" s="0"/>
-      <c r="LF4" s="0"/>
-      <c r="LG4" s="0"/>
-      <c r="LH4" s="0"/>
-      <c r="LI4" s="0"/>
-      <c r="LJ4" s="0"/>
-      <c r="LK4" s="0"/>
-      <c r="LL4" s="0"/>
-      <c r="LM4" s="0"/>
-      <c r="LN4" s="0"/>
-      <c r="LO4" s="0"/>
-      <c r="LP4" s="0"/>
-      <c r="LQ4" s="0"/>
-      <c r="LR4" s="0"/>
-      <c r="LS4" s="0"/>
-      <c r="LT4" s="0"/>
-      <c r="LU4" s="0"/>
-      <c r="LV4" s="0"/>
-      <c r="LW4" s="0"/>
-      <c r="LX4" s="0"/>
-      <c r="LY4" s="0"/>
-      <c r="LZ4" s="0"/>
-      <c r="MA4" s="0"/>
-      <c r="MB4" s="0"/>
-      <c r="MC4" s="0"/>
-      <c r="MD4" s="0"/>
-      <c r="ME4" s="0"/>
-      <c r="MF4" s="0"/>
-      <c r="MG4" s="0"/>
-      <c r="MH4" s="0"/>
-      <c r="MI4" s="0"/>
-      <c r="MJ4" s="0"/>
-      <c r="MK4" s="0"/>
-      <c r="ML4" s="0"/>
-      <c r="MM4" s="0"/>
-      <c r="MN4" s="0"/>
-      <c r="MO4" s="0"/>
-      <c r="MP4" s="0"/>
-      <c r="MQ4" s="0"/>
-      <c r="MR4" s="0"/>
-      <c r="MS4" s="0"/>
-      <c r="MT4" s="0"/>
-      <c r="MU4" s="0"/>
-      <c r="MV4" s="0"/>
-      <c r="MW4" s="0"/>
-      <c r="MX4" s="0"/>
-      <c r="MY4" s="0"/>
-      <c r="MZ4" s="0"/>
-      <c r="NA4" s="0"/>
-      <c r="NB4" s="0"/>
-      <c r="NC4" s="0"/>
-      <c r="ND4" s="0"/>
-      <c r="NE4" s="0"/>
-      <c r="NF4" s="0"/>
-      <c r="NG4" s="0"/>
-      <c r="NH4" s="0"/>
-      <c r="NI4" s="0"/>
-      <c r="NJ4" s="0"/>
-      <c r="NK4" s="0"/>
-      <c r="NL4" s="0"/>
-      <c r="NM4" s="0"/>
-      <c r="NN4" s="0"/>
-      <c r="NO4" s="0"/>
-      <c r="NP4" s="0"/>
-      <c r="NQ4" s="0"/>
-      <c r="NR4" s="0"/>
-      <c r="NS4" s="0"/>
-      <c r="NT4" s="0"/>
-      <c r="NU4" s="0"/>
-      <c r="NV4" s="0"/>
-      <c r="NW4" s="0"/>
-      <c r="NX4" s="0"/>
-      <c r="NY4" s="0"/>
-      <c r="NZ4" s="0"/>
-      <c r="OA4" s="0"/>
-      <c r="OB4" s="0"/>
-      <c r="OC4" s="0"/>
-      <c r="OD4" s="0"/>
-      <c r="OE4" s="0"/>
-      <c r="OF4" s="0"/>
-      <c r="OG4" s="0"/>
-      <c r="OH4" s="0"/>
-      <c r="OI4" s="0"/>
-      <c r="OJ4" s="0"/>
-      <c r="OK4" s="0"/>
-      <c r="OL4" s="0"/>
-      <c r="OM4" s="0"/>
-      <c r="ON4" s="0"/>
-      <c r="OO4" s="0"/>
-      <c r="OP4" s="0"/>
-      <c r="OQ4" s="0"/>
-      <c r="OR4" s="0"/>
-      <c r="OS4" s="0"/>
-      <c r="OT4" s="0"/>
-      <c r="OU4" s="0"/>
-      <c r="OV4" s="0"/>
-      <c r="OW4" s="0"/>
-      <c r="OX4" s="0"/>
-      <c r="OY4" s="0"/>
-      <c r="OZ4" s="0"/>
-      <c r="PA4" s="0"/>
-      <c r="PB4" s="0"/>
-      <c r="PC4" s="0"/>
-      <c r="PD4" s="0"/>
-      <c r="PE4" s="0"/>
-      <c r="PF4" s="0"/>
-      <c r="PG4" s="0"/>
-      <c r="PH4" s="0"/>
-      <c r="PI4" s="0"/>
-      <c r="PJ4" s="0"/>
-      <c r="PK4" s="0"/>
-      <c r="PL4" s="0"/>
-      <c r="PM4" s="0"/>
-      <c r="PN4" s="0"/>
-      <c r="PO4" s="0"/>
-      <c r="PP4" s="0"/>
-      <c r="PQ4" s="0"/>
-      <c r="PR4" s="0"/>
-      <c r="PS4" s="0"/>
-      <c r="PT4" s="0"/>
-      <c r="PU4" s="0"/>
-      <c r="PV4" s="0"/>
-      <c r="PW4" s="0"/>
-      <c r="PX4" s="0"/>
-      <c r="PY4" s="0"/>
-      <c r="PZ4" s="0"/>
-      <c r="QA4" s="0"/>
-      <c r="QB4" s="0"/>
-      <c r="QC4" s="0"/>
-      <c r="QD4" s="0"/>
-      <c r="QE4" s="0"/>
-      <c r="QF4" s="0"/>
-      <c r="QG4" s="0"/>
-      <c r="QH4" s="0"/>
-      <c r="QI4" s="0"/>
-      <c r="QJ4" s="0"/>
-      <c r="QK4" s="0"/>
-      <c r="QL4" s="0"/>
-      <c r="QM4" s="0"/>
-      <c r="QN4" s="0"/>
-      <c r="QO4" s="0"/>
-      <c r="QP4" s="0"/>
-      <c r="QQ4" s="0"/>
-      <c r="QR4" s="0"/>
-      <c r="QS4" s="0"/>
-      <c r="QT4" s="0"/>
-      <c r="QU4" s="0"/>
-      <c r="QV4" s="0"/>
-      <c r="QW4" s="0"/>
-      <c r="QX4" s="0"/>
-      <c r="QY4" s="0"/>
-      <c r="QZ4" s="0"/>
-      <c r="RA4" s="0"/>
-      <c r="RB4" s="0"/>
-      <c r="RC4" s="0"/>
-      <c r="RD4" s="0"/>
-      <c r="RE4" s="0"/>
-      <c r="RF4" s="0"/>
-      <c r="RG4" s="0"/>
-      <c r="RH4" s="0"/>
-      <c r="RI4" s="0"/>
-      <c r="RJ4" s="0"/>
-      <c r="RK4" s="0"/>
-      <c r="RL4" s="0"/>
-      <c r="RM4" s="0"/>
-      <c r="RN4" s="0"/>
-      <c r="RO4" s="0"/>
-      <c r="RP4" s="0"/>
-      <c r="RQ4" s="0"/>
-      <c r="RR4" s="0"/>
-      <c r="RS4" s="0"/>
-      <c r="RT4" s="0"/>
-      <c r="RU4" s="0"/>
-      <c r="RV4" s="0"/>
-      <c r="RW4" s="0"/>
-      <c r="RX4" s="0"/>
-      <c r="RY4" s="0"/>
-      <c r="RZ4" s="0"/>
-      <c r="SA4" s="0"/>
-      <c r="SB4" s="0"/>
-      <c r="SC4" s="0"/>
-      <c r="SD4" s="0"/>
-      <c r="SE4" s="0"/>
-      <c r="SF4" s="0"/>
-      <c r="SG4" s="0"/>
-      <c r="SH4" s="0"/>
-      <c r="SI4" s="0"/>
-      <c r="SJ4" s="0"/>
-      <c r="SK4" s="0"/>
-      <c r="SL4" s="0"/>
-      <c r="SM4" s="0"/>
-      <c r="SN4" s="0"/>
-      <c r="SO4" s="0"/>
-      <c r="SP4" s="0"/>
-      <c r="SQ4" s="0"/>
-      <c r="SR4" s="0"/>
-      <c r="SS4" s="0"/>
-      <c r="ST4" s="0"/>
-      <c r="SU4" s="0"/>
-      <c r="SV4" s="0"/>
-      <c r="SW4" s="0"/>
-      <c r="SX4" s="0"/>
-      <c r="SY4" s="0"/>
-      <c r="SZ4" s="0"/>
-      <c r="TA4" s="0"/>
-      <c r="TB4" s="0"/>
-      <c r="TC4" s="0"/>
-      <c r="TD4" s="0"/>
-      <c r="TE4" s="0"/>
-      <c r="TF4" s="0"/>
-      <c r="TG4" s="0"/>
-      <c r="TH4" s="0"/>
-      <c r="TI4" s="0"/>
-      <c r="TJ4" s="0"/>
-      <c r="TK4" s="0"/>
-      <c r="TL4" s="0"/>
-      <c r="TM4" s="0"/>
-      <c r="TN4" s="0"/>
-      <c r="TO4" s="0"/>
-      <c r="TP4" s="0"/>
-      <c r="TQ4" s="0"/>
-      <c r="TR4" s="0"/>
-      <c r="TS4" s="0"/>
-      <c r="TT4" s="0"/>
-      <c r="TU4" s="0"/>
-      <c r="TV4" s="0"/>
-      <c r="TW4" s="0"/>
-      <c r="TX4" s="0"/>
-      <c r="TY4" s="0"/>
-      <c r="TZ4" s="0"/>
-      <c r="UA4" s="0"/>
-      <c r="UB4" s="0"/>
-      <c r="UC4" s="0"/>
-      <c r="UD4" s="0"/>
-      <c r="UE4" s="0"/>
-      <c r="UF4" s="0"/>
-      <c r="UG4" s="0"/>
-      <c r="UH4" s="0"/>
-      <c r="UI4" s="0"/>
-      <c r="UJ4" s="0"/>
-      <c r="UK4" s="0"/>
-      <c r="UL4" s="0"/>
-      <c r="UM4" s="0"/>
-      <c r="UN4" s="0"/>
-      <c r="UO4" s="0"/>
-      <c r="UP4" s="0"/>
-      <c r="UQ4" s="0"/>
-      <c r="UR4" s="0"/>
-      <c r="US4" s="0"/>
-      <c r="UT4" s="0"/>
-      <c r="UU4" s="0"/>
-      <c r="UV4" s="0"/>
-      <c r="UW4" s="0"/>
-      <c r="UX4" s="0"/>
-      <c r="UY4" s="0"/>
-      <c r="UZ4" s="0"/>
-      <c r="VA4" s="0"/>
-      <c r="VB4" s="0"/>
-      <c r="VC4" s="0"/>
-      <c r="VD4" s="0"/>
-      <c r="VE4" s="0"/>
-      <c r="VF4" s="0"/>
-      <c r="VG4" s="0"/>
-      <c r="VH4" s="0"/>
-      <c r="VI4" s="0"/>
-      <c r="VJ4" s="0"/>
-      <c r="VK4" s="0"/>
-      <c r="VL4" s="0"/>
-      <c r="VM4" s="0"/>
-      <c r="VN4" s="0"/>
-      <c r="VO4" s="0"/>
-      <c r="VP4" s="0"/>
-      <c r="VQ4" s="0"/>
-      <c r="VR4" s="0"/>
-      <c r="VS4" s="0"/>
-      <c r="VT4" s="0"/>
-      <c r="VU4" s="0"/>
-      <c r="VV4" s="0"/>
-      <c r="VW4" s="0"/>
-      <c r="VX4" s="0"/>
-      <c r="VY4" s="0"/>
-      <c r="VZ4" s="0"/>
-      <c r="WA4" s="0"/>
-      <c r="WB4" s="0"/>
-      <c r="WC4" s="0"/>
-      <c r="WD4" s="0"/>
-      <c r="WE4" s="0"/>
-      <c r="WF4" s="0"/>
-      <c r="WG4" s="0"/>
-      <c r="WH4" s="0"/>
-      <c r="WI4" s="0"/>
-      <c r="WJ4" s="0"/>
-      <c r="WK4" s="0"/>
-      <c r="WL4" s="0"/>
-      <c r="WM4" s="0"/>
-      <c r="WN4" s="0"/>
-      <c r="WO4" s="0"/>
-      <c r="WP4" s="0"/>
-      <c r="WQ4" s="0"/>
-      <c r="WR4" s="0"/>
-      <c r="WS4" s="0"/>
-      <c r="WT4" s="0"/>
-      <c r="WU4" s="0"/>
-      <c r="WV4" s="0"/>
-      <c r="WW4" s="0"/>
-      <c r="WX4" s="0"/>
-      <c r="WY4" s="0"/>
-      <c r="WZ4" s="0"/>
-      <c r="XA4" s="0"/>
-      <c r="XB4" s="0"/>
-      <c r="XC4" s="0"/>
-      <c r="XD4" s="0"/>
-      <c r="XE4" s="0"/>
-      <c r="XF4" s="0"/>
-      <c r="XG4" s="0"/>
-      <c r="XH4" s="0"/>
-      <c r="XI4" s="0"/>
-      <c r="XJ4" s="0"/>
-      <c r="XK4" s="0"/>
-      <c r="XL4" s="0"/>
-      <c r="XM4" s="0"/>
-      <c r="XN4" s="0"/>
-      <c r="XO4" s="0"/>
-      <c r="XP4" s="0"/>
-      <c r="XQ4" s="0"/>
-      <c r="XR4" s="0"/>
-      <c r="XS4" s="0"/>
-      <c r="XT4" s="0"/>
-      <c r="XU4" s="0"/>
-      <c r="XV4" s="0"/>
-      <c r="XW4" s="0"/>
-      <c r="XX4" s="0"/>
-      <c r="XY4" s="0"/>
-      <c r="XZ4" s="0"/>
-      <c r="YA4" s="0"/>
-      <c r="YB4" s="0"/>
-      <c r="YC4" s="0"/>
-      <c r="YD4" s="0"/>
-      <c r="YE4" s="0"/>
-      <c r="YF4" s="0"/>
-      <c r="YG4" s="0"/>
-      <c r="YH4" s="0"/>
-      <c r="YI4" s="0"/>
-      <c r="YJ4" s="0"/>
-      <c r="YK4" s="0"/>
-      <c r="YL4" s="0"/>
-      <c r="YM4" s="0"/>
-      <c r="YN4" s="0"/>
-      <c r="YO4" s="0"/>
-      <c r="YP4" s="0"/>
-      <c r="YQ4" s="0"/>
-      <c r="YR4" s="0"/>
-      <c r="YS4" s="0"/>
-      <c r="YT4" s="0"/>
-      <c r="YU4" s="0"/>
-      <c r="YV4" s="0"/>
-      <c r="YW4" s="0"/>
-      <c r="YX4" s="0"/>
-      <c r="YY4" s="0"/>
-      <c r="YZ4" s="0"/>
-      <c r="ZA4" s="0"/>
-      <c r="ZB4" s="0"/>
-      <c r="ZC4" s="0"/>
-      <c r="ZD4" s="0"/>
-      <c r="ZE4" s="0"/>
-      <c r="ZF4" s="0"/>
-      <c r="ZG4" s="0"/>
-      <c r="ZH4" s="0"/>
-      <c r="ZI4" s="0"/>
-      <c r="ZJ4" s="0"/>
-      <c r="ZK4" s="0"/>
-      <c r="ZL4" s="0"/>
-      <c r="ZM4" s="0"/>
-      <c r="ZN4" s="0"/>
-      <c r="ZO4" s="0"/>
-      <c r="ZP4" s="0"/>
-      <c r="ZQ4" s="0"/>
-      <c r="ZR4" s="0"/>
-      <c r="ZS4" s="0"/>
-      <c r="ZT4" s="0"/>
-      <c r="ZU4" s="0"/>
-      <c r="ZV4" s="0"/>
-      <c r="ZW4" s="0"/>
-      <c r="ZX4" s="0"/>
-      <c r="ZY4" s="0"/>
-      <c r="ZZ4" s="0"/>
-      <c r="AAA4" s="0"/>
-      <c r="AAB4" s="0"/>
-      <c r="AAC4" s="0"/>
-      <c r="AAD4" s="0"/>
-      <c r="AAE4" s="0"/>
-      <c r="AAF4" s="0"/>
-      <c r="AAG4" s="0"/>
-      <c r="AAH4" s="0"/>
-      <c r="AAI4" s="0"/>
-      <c r="AAJ4" s="0"/>
-      <c r="AAK4" s="0"/>
-      <c r="AAL4" s="0"/>
-      <c r="AAM4" s="0"/>
-      <c r="AAN4" s="0"/>
-      <c r="AAO4" s="0"/>
-      <c r="AAP4" s="0"/>
-      <c r="AAQ4" s="0"/>
-      <c r="AAR4" s="0"/>
-      <c r="AAS4" s="0"/>
-      <c r="AAT4" s="0"/>
-      <c r="AAU4" s="0"/>
-      <c r="AAV4" s="0"/>
-      <c r="AAW4" s="0"/>
-      <c r="AAX4" s="0"/>
-      <c r="AAY4" s="0"/>
-      <c r="AAZ4" s="0"/>
-      <c r="ABA4" s="0"/>
-      <c r="ABB4" s="0"/>
-      <c r="ABC4" s="0"/>
-      <c r="ABD4" s="0"/>
-      <c r="ABE4" s="0"/>
-      <c r="ABF4" s="0"/>
-      <c r="ABG4" s="0"/>
-      <c r="ABH4" s="0"/>
-      <c r="ABI4" s="0"/>
-      <c r="ABJ4" s="0"/>
-      <c r="ABK4" s="0"/>
-      <c r="ABL4" s="0"/>
-      <c r="ABM4" s="0"/>
-      <c r="ABN4" s="0"/>
-      <c r="ABO4" s="0"/>
-      <c r="ABP4" s="0"/>
-      <c r="ABQ4" s="0"/>
-      <c r="ABR4" s="0"/>
-      <c r="ABS4" s="0"/>
-      <c r="ABT4" s="0"/>
-      <c r="ABU4" s="0"/>
-      <c r="ABV4" s="0"/>
-      <c r="ABW4" s="0"/>
-      <c r="ABX4" s="0"/>
-      <c r="ABY4" s="0"/>
-      <c r="ABZ4" s="0"/>
-      <c r="ACA4" s="0"/>
-      <c r="ACB4" s="0"/>
-      <c r="ACC4" s="0"/>
-      <c r="ACD4" s="0"/>
-      <c r="ACE4" s="0"/>
-      <c r="ACF4" s="0"/>
-      <c r="ACG4" s="0"/>
-      <c r="ACH4" s="0"/>
-      <c r="ACI4" s="0"/>
-      <c r="ACJ4" s="0"/>
-      <c r="ACK4" s="0"/>
-      <c r="ACL4" s="0"/>
-      <c r="ACM4" s="0"/>
-      <c r="ACN4" s="0"/>
-      <c r="ACO4" s="0"/>
-      <c r="ACP4" s="0"/>
-      <c r="ACQ4" s="0"/>
-      <c r="ACR4" s="0"/>
-      <c r="ACS4" s="0"/>
-      <c r="ACT4" s="0"/>
-      <c r="ACU4" s="0"/>
-      <c r="ACV4" s="0"/>
-      <c r="ACW4" s="0"/>
-      <c r="ACX4" s="0"/>
-      <c r="ACY4" s="0"/>
-      <c r="ACZ4" s="0"/>
-      <c r="ADA4" s="0"/>
-      <c r="ADB4" s="0"/>
-      <c r="ADC4" s="0"/>
-      <c r="ADD4" s="0"/>
-      <c r="ADE4" s="0"/>
-      <c r="ADF4" s="0"/>
-      <c r="ADG4" s="0"/>
-      <c r="ADH4" s="0"/>
-      <c r="ADI4" s="0"/>
-      <c r="ADJ4" s="0"/>
-      <c r="ADK4" s="0"/>
-      <c r="ADL4" s="0"/>
-      <c r="ADM4" s="0"/>
-      <c r="ADN4" s="0"/>
-      <c r="ADO4" s="0"/>
-      <c r="ADP4" s="0"/>
-      <c r="ADQ4" s="0"/>
-      <c r="ADR4" s="0"/>
-      <c r="ADS4" s="0"/>
-      <c r="ADT4" s="0"/>
-      <c r="ADU4" s="0"/>
-      <c r="ADV4" s="0"/>
-      <c r="ADW4" s="0"/>
-      <c r="ADX4" s="0"/>
-      <c r="ADY4" s="0"/>
-      <c r="ADZ4" s="0"/>
-      <c r="AEA4" s="0"/>
-      <c r="AEB4" s="0"/>
-      <c r="AEC4" s="0"/>
-      <c r="AED4" s="0"/>
-      <c r="AEE4" s="0"/>
-      <c r="AEF4" s="0"/>
-      <c r="AEG4" s="0"/>
-      <c r="AEH4" s="0"/>
-      <c r="AEI4" s="0"/>
-      <c r="AEJ4" s="0"/>
-      <c r="AEK4" s="0"/>
-      <c r="AEL4" s="0"/>
-      <c r="AEM4" s="0"/>
-      <c r="AEN4" s="0"/>
-      <c r="AEO4" s="0"/>
-      <c r="AEP4" s="0"/>
-      <c r="AEQ4" s="0"/>
-      <c r="AER4" s="0"/>
-      <c r="AES4" s="0"/>
-      <c r="AET4" s="0"/>
-      <c r="AEU4" s="0"/>
-      <c r="AEV4" s="0"/>
-      <c r="AEW4" s="0"/>
-      <c r="AEX4" s="0"/>
-      <c r="AEY4" s="0"/>
-      <c r="AEZ4" s="0"/>
-      <c r="AFA4" s="0"/>
-      <c r="AFB4" s="0"/>
-      <c r="AFC4" s="0"/>
-      <c r="AFD4" s="0"/>
-      <c r="AFE4" s="0"/>
-      <c r="AFF4" s="0"/>
-      <c r="AFG4" s="0"/>
-      <c r="AFH4" s="0"/>
-      <c r="AFI4" s="0"/>
-      <c r="AFJ4" s="0"/>
-      <c r="AFK4" s="0"/>
-      <c r="AFL4" s="0"/>
-      <c r="AFM4" s="0"/>
-      <c r="AFN4" s="0"/>
-      <c r="AFO4" s="0"/>
-      <c r="AFP4" s="0"/>
-      <c r="AFQ4" s="0"/>
-      <c r="AFR4" s="0"/>
-      <c r="AFS4" s="0"/>
-      <c r="AFT4" s="0"/>
-      <c r="AFU4" s="0"/>
-      <c r="AFV4" s="0"/>
-      <c r="AFW4" s="0"/>
-      <c r="AFX4" s="0"/>
-      <c r="AFY4" s="0"/>
-      <c r="AFZ4" s="0"/>
-      <c r="AGA4" s="0"/>
-      <c r="AGB4" s="0"/>
-      <c r="AGC4" s="0"/>
-      <c r="AGD4" s="0"/>
-      <c r="AGE4" s="0"/>
-      <c r="AGF4" s="0"/>
-      <c r="AGG4" s="0"/>
-      <c r="AGH4" s="0"/>
-      <c r="AGI4" s="0"/>
-      <c r="AGJ4" s="0"/>
-      <c r="AGK4" s="0"/>
-      <c r="AGL4" s="0"/>
-      <c r="AGM4" s="0"/>
-      <c r="AGN4" s="0"/>
-      <c r="AGO4" s="0"/>
-      <c r="AGP4" s="0"/>
-      <c r="AGQ4" s="0"/>
-      <c r="AGR4" s="0"/>
-      <c r="AGS4" s="0"/>
-      <c r="AGT4" s="0"/>
-      <c r="AGU4" s="0"/>
-      <c r="AGV4" s="0"/>
-      <c r="AGW4" s="0"/>
-      <c r="AGX4" s="0"/>
-      <c r="AGY4" s="0"/>
-      <c r="AGZ4" s="0"/>
-      <c r="AHA4" s="0"/>
-      <c r="AHB4" s="0"/>
-      <c r="AHC4" s="0"/>
-      <c r="AHD4" s="0"/>
-      <c r="AHE4" s="0"/>
-      <c r="AHF4" s="0"/>
-      <c r="AHG4" s="0"/>
-      <c r="AHH4" s="0"/>
-      <c r="AHI4" s="0"/>
-      <c r="AHJ4" s="0"/>
-      <c r="AHK4" s="0"/>
-      <c r="AHL4" s="0"/>
-      <c r="AHM4" s="0"/>
-      <c r="AHN4" s="0"/>
-      <c r="AHO4" s="0"/>
-      <c r="AHP4" s="0"/>
-      <c r="AHQ4" s="0"/>
-      <c r="AHR4" s="0"/>
-      <c r="AHS4" s="0"/>
-      <c r="AHT4" s="0"/>
-      <c r="AHU4" s="0"/>
-      <c r="AHV4" s="0"/>
-      <c r="AHW4" s="0"/>
-      <c r="AHX4" s="0"/>
-      <c r="AHY4" s="0"/>
-      <c r="AHZ4" s="0"/>
-      <c r="AIA4" s="0"/>
-      <c r="AIB4" s="0"/>
-      <c r="AIC4" s="0"/>
-      <c r="AID4" s="0"/>
-      <c r="AIE4" s="0"/>
-      <c r="AIF4" s="0"/>
-      <c r="AIG4" s="0"/>
-      <c r="AIH4" s="0"/>
-      <c r="AII4" s="0"/>
-      <c r="AIJ4" s="0"/>
-      <c r="AIK4" s="0"/>
-      <c r="AIL4" s="0"/>
-      <c r="AIM4" s="0"/>
-      <c r="AIN4" s="0"/>
-      <c r="AIO4" s="0"/>
-      <c r="AIP4" s="0"/>
-      <c r="AIQ4" s="0"/>
-      <c r="AIR4" s="0"/>
-      <c r="AIS4" s="0"/>
-      <c r="AIT4" s="0"/>
-      <c r="AIU4" s="0"/>
-      <c r="AIV4" s="0"/>
-      <c r="AIW4" s="0"/>
-      <c r="AIX4" s="0"/>
-      <c r="AIY4" s="0"/>
-      <c r="AIZ4" s="0"/>
-      <c r="AJA4" s="0"/>
-      <c r="AJB4" s="0"/>
-      <c r="AJC4" s="0"/>
-      <c r="AJD4" s="0"/>
-      <c r="AJE4" s="0"/>
-      <c r="AJF4" s="0"/>
-      <c r="AJG4" s="0"/>
-      <c r="AJH4" s="0"/>
-      <c r="AJI4" s="0"/>
-      <c r="AJJ4" s="0"/>
-      <c r="AJK4" s="0"/>
-      <c r="AJL4" s="0"/>
-      <c r="AJM4" s="0"/>
-      <c r="AJN4" s="0"/>
-      <c r="AJO4" s="0"/>
-      <c r="AJP4" s="0"/>
-      <c r="AJQ4" s="0"/>
-      <c r="AJR4" s="0"/>
-      <c r="AJS4" s="0"/>
-      <c r="AJT4" s="0"/>
-      <c r="AJU4" s="0"/>
-      <c r="AJV4" s="0"/>
-      <c r="AJW4" s="0"/>
-      <c r="AJX4" s="0"/>
-      <c r="AJY4" s="0"/>
-      <c r="AJZ4" s="0"/>
-      <c r="AKA4" s="0"/>
-      <c r="AKB4" s="0"/>
-      <c r="AKC4" s="0"/>
-      <c r="AKD4" s="0"/>
-      <c r="AKE4" s="0"/>
-      <c r="AKF4" s="0"/>
-      <c r="AKG4" s="0"/>
-      <c r="AKH4" s="0"/>
-      <c r="AKI4" s="0"/>
-      <c r="AKJ4" s="0"/>
-      <c r="AKK4" s="0"/>
-      <c r="AKL4" s="0"/>
-      <c r="AKM4" s="0"/>
-      <c r="AKN4" s="0"/>
-      <c r="AKO4" s="0"/>
-      <c r="AKP4" s="0"/>
-      <c r="AKQ4" s="0"/>
-      <c r="AKR4" s="0"/>
-      <c r="AKS4" s="0"/>
-      <c r="AKT4" s="0"/>
-      <c r="AKU4" s="0"/>
-      <c r="AKV4" s="0"/>
-      <c r="AKW4" s="0"/>
-      <c r="AKX4" s="0"/>
-      <c r="AKY4" s="0"/>
-      <c r="AKZ4" s="0"/>
-      <c r="ALA4" s="0"/>
-      <c r="ALB4" s="0"/>
-      <c r="ALC4" s="0"/>
-      <c r="ALD4" s="0"/>
-      <c r="ALE4" s="0"/>
-      <c r="ALF4" s="0"/>
-      <c r="ALG4" s="0"/>
-      <c r="ALH4" s="0"/>
-      <c r="ALI4" s="0"/>
-      <c r="ALJ4" s="0"/>
-      <c r="ALK4" s="0"/>
-      <c r="ALL4" s="0"/>
-      <c r="ALM4" s="0"/>
-      <c r="ALN4" s="0"/>
-      <c r="ALO4" s="0"/>
-      <c r="ALP4" s="0"/>
-      <c r="ALQ4" s="0"/>
-      <c r="ALR4" s="0"/>
-      <c r="ALS4" s="0"/>
-      <c r="ALT4" s="0"/>
-      <c r="ALU4" s="0"/>
-      <c r="ALV4" s="0"/>
-      <c r="ALW4" s="0"/>
-      <c r="ALX4" s="0"/>
-      <c r="ALY4" s="0"/>
-      <c r="ALZ4" s="0"/>
-      <c r="AMA4" s="0"/>
-      <c r="AMB4" s="0"/>
-      <c r="AMC4" s="0"/>
-      <c r="AMD4" s="0"/>
-      <c r="AME4" s="0"/>
-      <c r="AMF4" s="0"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="49" customFormat="true" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="70" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="AMH5" s="61"/>
-      <c r="AMI5" s="61"/>
-      <c r="AMJ5" s="23"/>
-    </row>
-    <row r="6" s="23" customFormat="true" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="78" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9493,22 +7299,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="79" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="79" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="79" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="79" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="79" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="79" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="79" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="69" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="69" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="69" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="69" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="69" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="69" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="69" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51"/>
       <c r="B1" s="52"/>
-      <c r="C1" s="80"/>
+      <c r="C1" s="70"/>
       <c r="D1" s="53"/>
       <c r="E1" s="53"/>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="71" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="0"/>
@@ -10531,22 +8337,22 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="76" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="0"/>
@@ -11569,22 +9375,22 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="89" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="90" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="91" t="s">
+      <c r="B3" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="92" t="n">
+      <c r="F3" s="82" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0"/>
@@ -12607,22 +10413,22 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="96" t="s">
+      <c r="B4" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="98" t="n">
+      <c r="F4" s="88" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="0"/>
@@ -13645,22 +11451,22 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="96" t="s">
+      <c r="B5" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="100" t="n">
+      <c r="F5" s="90" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="0"/>
@@ -14683,42 +12489,42 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="102" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="103" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="103" t="s">
+      <c r="B6" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="104" t="s">
+      <c r="E6" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="105" t="n">
+      <c r="F6" s="95" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="107" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="108" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="108" t="s">
+      <c r="B7" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="110" t="n">
+      <c r="F7" s="100" t="n">
         <v>1</v>
       </c>
     </row>
@@ -14747,13 +12553,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="23" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="46.919028340081"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>
@@ -14769,16 +12575,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="101" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="101" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="34" t="s">
@@ -14789,13 +12595,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="104" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="45" t="s">
@@ -14804,18 +12610,18 @@
       <c r="E3" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="115" t="n">
+      <c r="F3" s="105" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="114" t="n">
+      <c r="C4" s="104" t="n">
         <v>3582910009405</v>
       </c>
       <c r="D4" s="45" t="s">
@@ -14824,18 +12630,18 @@
       <c r="E4" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="115" t="n">
+      <c r="F4" s="105" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="114" t="n">
+      <c r="C5" s="104" t="n">
         <v>3582910010296</v>
       </c>
       <c r="D5" s="45" t="s">
@@ -14844,18 +12650,18 @@
       <c r="E5" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="115" t="n">
+      <c r="F5" s="105" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="114" t="n">
+      <c r="C6" s="104" t="n">
         <v>8993237276046</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -14864,18 +12670,18 @@
       <c r="E6" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="115" t="n">
+      <c r="F6" s="105" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="114" t="n">
+      <c r="C7" s="104" t="n">
         <v>7891058013271</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -14884,18 +12690,18 @@
       <c r="E7" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="115" t="n">
+      <c r="F7" s="105" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="114" t="s">
+      <c r="C8" s="104" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -14904,18 +12710,18 @@
       <c r="E8" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="115" t="n">
+      <c r="F8" s="105" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="113" t="s">
+      <c r="B9" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="114" t="n">
+      <c r="C9" s="104" t="n">
         <v>7610939003137</v>
       </c>
       <c r="D9" s="45" t="s">
@@ -14924,18 +12730,18 @@
       <c r="E9" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="115" t="n">
+      <c r="F9" s="105" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="78" t="n">
+      <c r="C10" s="107" t="n">
         <v>9556499160684</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -14944,18 +12750,18 @@
       <c r="E10" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="117" t="n">
+      <c r="F10" s="108" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="113" t="s">
+      <c r="B11" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="107" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -14964,7 +12770,7 @@
       <c r="E11" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="117" t="n">
+      <c r="F11" s="108" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROS-7522 BIMY Kpi Update
</commit_message>
<xml_diff>
--- a/Projects/BIMY/Data/Template.xlsx
+++ b/Projects/BIMY/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,25 +16,26 @@
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$8</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$F$2</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="78">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -210,12 +211,6 @@
     <t xml:space="preserve">Digestive Health</t>
   </si>
   <si>
-    <t xml:space="preserve">DULCOLAX TABLETS 30's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9556991220282</t>
-  </si>
-  <si>
     <t xml:space="preserve">PHARMATON 100S+30S </t>
   </si>
   <si>
@@ -240,18 +235,6 @@
     <t xml:space="preserve">Essentiale</t>
   </si>
   <si>
-    <t xml:space="preserve">BUSCOPAN TABLETS 10mg 100's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4048846005496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscopan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain</t>
-  </si>
-  <si>
     <t xml:space="preserve">MAALOX PLUS TABLETS 25mg 40's</t>
   </si>
   <si>
@@ -259,30 +242,6 @@
   </si>
   <si>
     <t xml:space="preserve">MAALOX SACHET 4.3ml x 20's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELFAST TABLETS 180mg 50's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8993237276046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telfast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELFAST SUSPENSION LIQUID 60ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7891058013271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NASACORT AQ NASAL SPRAY 120 DOSES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasacort</t>
   </si>
   <si>
     <t xml:space="preserve">RHINATHIOL ADULT SYRUP 125ml</t>
@@ -298,6 +257,15 @@
   </si>
   <si>
     <t xml:space="preserve">PHARMATON 2X100'S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTEROGERMINA 5ML SUSP BT20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterogermina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probiotic</t>
   </si>
   <si>
     <t xml:space="preserve">Primary_Shelftalker_Muco&amp;Rhina</t>
@@ -321,16 +289,19 @@
     <t xml:space="preserve">MY_Primary_03</t>
   </si>
   <si>
+    <t xml:space="preserve">Telfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allergy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Secondary_Shelftalker_Essentiale</t>
   </si>
   <si>
     <t xml:space="preserve">MY_Secondary_01</t>
   </si>
   <si>
-    <t xml:space="preserve">Secondary_Standee_PharmatonMerdeka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MY_Secondary_0818</t>
+    <t xml:space="preserve">DULCOLAX TAB 200S (BLISTER PACK)</t>
   </si>
 </sst>
 </file>
@@ -569,7 +540,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="35">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -815,13 +786,6 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -852,7 +816,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="104">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1221,10 +1185,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1234,26 +1194,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1377,18 +1317,18 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.5627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.497975708502"/>
   </cols>
   <sheetData>
@@ -1647,17 +1587,17 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:19"/>
+  <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="16.3886639676113"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="23" width="0"/>
@@ -5842,10 +5782,10 @@
         <v>48</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F6" s="47"/>
       <c r="G6" s="48" t="n">
@@ -5857,16 +5797,16 @@
         <v>23</v>
       </c>
       <c r="B7" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="44" t="n">
+        <v>7610939003137</v>
+      </c>
+      <c r="D7" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="E7" s="46" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>52</v>
       </c>
       <c r="F7" s="47"/>
       <c r="G7" s="48" t="n">
@@ -5878,16 +5818,16 @@
         <v>23</v>
       </c>
       <c r="B8" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="44" t="n">
-        <v>7610939003137</v>
-      </c>
       <c r="D8" s="45" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="48" t="n">
@@ -5899,16 +5839,16 @@
         <v>23</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="44" t="s">
         <v>55</v>
+      </c>
+      <c r="C9" s="44" t="n">
+        <v>9556499172861</v>
       </c>
       <c r="D9" s="45" t="s">
         <v>56</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F9" s="47"/>
       <c r="G9" s="48" t="n">
@@ -5922,14 +5862,14 @@
       <c r="B10" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>58</v>
+      <c r="C10" s="44" t="n">
+        <v>9556499331442</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="48" t="n">
@@ -5941,16 +5881,16 @@
         <v>23</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" s="44" t="n">
-        <v>9556499172861</v>
+        <v>3582910009405</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F11" s="47"/>
       <c r="G11" s="48" t="n">
@@ -5962,16 +5902,16 @@
         <v>23</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C12" s="44" t="n">
-        <v>9556499331442</v>
+        <v>3582910010296</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F12" s="47"/>
       <c r="G12" s="48" t="n">
@@ -5983,150 +5923,69 @@
         <v>23</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C13" s="44" t="n">
+        <v>9556991220640</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="F13" s="47"/>
       <c r="G13" s="48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="C14" s="44" t="n">
+        <v>9556991220572</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="47"/>
+        <v>50</v>
+      </c>
+      <c r="F14" s="50"/>
       <c r="G14" s="48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C15" s="44" t="n">
-        <v>3582910052104</v>
+        <v>582910034988</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="47"/>
+        <v>64</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="46" t="n">
+        <v>1</v>
+      </c>
       <c r="G15" s="48" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="44" t="n">
-        <v>3582910009405</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="44" t="n">
-        <v>3582910010296</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="44" t="n">
-        <v>9556991220640</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="44" t="n">
-        <v>9556991220572</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="48" t="n">
-        <v>0</v>
-      </c>
+      <c r="H15" s="48"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H9"/>
+  <autoFilter ref="A2:G8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6146,15 +6005,15 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -6212,16 +6071,16 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="61" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="18.3157894736842"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7291,18 +7150,18 @@
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="69" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="69" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="69" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="69" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="69" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="69" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="69" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="69" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="69" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="69" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="69" width="9.10526315789474"/>
@@ -9379,13 +9238,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="78" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D3" s="80" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E3" s="81" t="s">
         <v>40</v>
@@ -10417,16 +10276,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="84" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C4" s="85" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="87" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" s="88" t="n">
         <v>1</v>
@@ -11455,16 +11314,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C5" s="85" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F5" s="90" t="n">
         <v>1</v>
@@ -12492,39 +12351,19 @@
       <c r="A6" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="92" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="94" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="95" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="96" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="99" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="100" t="n">
+      <c r="B6" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="94" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12547,19 +12386,19 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="23" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="23" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="47.2388663967611"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>
@@ -12575,16 +12414,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="95" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="95" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="34" t="s">
@@ -12595,13 +12434,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="98" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="45" t="s">
@@ -12610,168 +12449,168 @@
       <c r="E3" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="105" t="n">
-        <v>2</v>
+      <c r="F3" s="99" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="103" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="104" t="n">
-        <v>3582910009405</v>
+      <c r="B4" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="98" t="n">
+        <v>9556991220275</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="105" t="n">
+      <c r="F4" s="99" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="103" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="104" t="n">
-        <v>3582910010296</v>
+      <c r="B5" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="98" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="105" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F5" s="99" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="103" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="104" t="n">
-        <v>8993237276046</v>
+      <c r="B6" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="98" t="n">
+        <v>7610939003137</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="105" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" s="99" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="103" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="104" t="n">
-        <v>7891058013271</v>
+      <c r="B7" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="98" t="n">
+        <v>9556499160684</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="105" t="n">
+        <v>46</v>
+      </c>
+      <c r="F7" s="99" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="102" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="103" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="104" t="s">
-        <v>50</v>
+      <c r="A8" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="101" t="n">
+        <v>9556499160684</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="105" t="n">
+        <v>46</v>
+      </c>
+      <c r="F8" s="102" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="102" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="104" t="n">
-        <v>7610939003137</v>
+      <c r="A9" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="101" t="s">
+        <v>48</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="105" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F9" s="102" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="103" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="107" t="n">
-        <v>9556499160684</v>
+      <c r="B10" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="101" t="n">
+        <v>9556991220275</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="108" t="n">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="F10" s="102" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="103" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="107" t="s">
-        <v>50</v>
+      <c r="B11" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="101" t="n">
+        <v>9556991220299</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="108" t="n">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="F11" s="102" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>